<commit_message>
updated pinlist, sorted pins in scrap tab
</commit_message>
<xml_diff>
--- a/doc/LPC1769_pinmapping.xlsx
+++ b/doc/LPC1769_pinmapping.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LPC1769FBD100,551" sheetId="1" r:id="rId1"/>
     <sheet name="V1.0" sheetId="2" r:id="rId2"/>
     <sheet name="V1.1" sheetId="4" r:id="rId3"/>
-    <sheet name="KiCAD" sheetId="3" r:id="rId4"/>
+    <sheet name="Scrap" sheetId="5" r:id="rId4"/>
+    <sheet name="KiCAD" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">V1.0!$A$1:$O$101</definedName>
@@ -55,8 +56,31 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="M45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Note the reverse order of X3/X4</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="450">
   <si>
     <t>Pin Name</t>
   </si>
@@ -1583,12 +1607,45 @@
   <si>
     <t>J8</t>
   </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>PEX Pin</t>
+  </si>
+  <si>
+    <t>Pex Order</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1687,6 +1744,20 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1868,10 +1939,158 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1974,19 +2193,188 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="149">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4185,7 +4573,7 @@
     <col min="15" max="15" width="11" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="142" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="141" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -7515,8 +7903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7611,18 +7999,18 @@
       <c r="L2" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="60" t="s">
+      <c r="M2" s="60"/>
+      <c r="N2" s="59" t="s">
         <v>438</v>
       </c>
-      <c r="O2" s="59" t="s">
+      <c r="O2" s="57" t="s">
         <v>414</v>
       </c>
       <c r="P2" t="s">
         <v>427</v>
       </c>
       <c r="Q2" t="str">
-        <f t="shared" ref="Q2:Q13" si="0">I2</f>
+        <f t="shared" ref="Q2:Q7" si="0">I2</f>
         <v>P0[26]</v>
       </c>
       <c r="V2" t="s">
@@ -7661,8 +8049,8 @@
       <c r="L3" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="M3" s="57"/>
-      <c r="N3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="59"/>
       <c r="O3" t="s">
         <v>413</v>
       </c>
@@ -7707,8 +8095,8 @@
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="56" t="s">
+      <c r="M4" s="60"/>
+      <c r="N4" s="58" t="s">
         <v>435</v>
       </c>
       <c r="O4" t="s">
@@ -7761,8 +8149,8 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="56"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="58"/>
       <c r="O5" t="s">
         <v>414</v>
       </c>
@@ -7815,8 +8203,8 @@
         <v>207</v>
       </c>
       <c r="L6" s="16"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="56"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="58"/>
       <c r="O6" t="s">
         <v>415</v>
       </c>
@@ -7857,8 +8245,8 @@
         <v>211</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="56"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="58"/>
       <c r="O7" t="s">
         <v>416</v>
       </c>
@@ -7945,6 +8333,19 @@
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
+      <c r="N10" t="s">
+        <v>443</v>
+      </c>
+      <c r="O10" t="s">
+        <v>414</v>
+      </c>
+      <c r="P10" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" ref="Q10" si="1">I10</f>
+        <v>P3[26]</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -8051,11 +8452,11 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
-      <c r="M14" s="57" t="s">
+      <c r="M14" s="60" t="s">
         <v>410</v>
       </c>
-      <c r="N14" s="56" t="s">
-        <v>434</v>
+      <c r="N14" s="58" t="s">
+        <v>441</v>
       </c>
       <c r="O14" t="s">
         <v>416</v>
@@ -8064,7 +8465,7 @@
         <v>429</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" ref="Q14:Q17" si="1">I14</f>
+        <f t="shared" ref="Q14:Q17" si="2">I14</f>
         <v>P1[18]</v>
       </c>
     </row>
@@ -8091,8 +8492,8 @@
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="56"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="58"/>
       <c r="O15" t="s">
         <v>415</v>
       </c>
@@ -8100,7 +8501,7 @@
         <v>428</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>P1[19]</v>
       </c>
     </row>
@@ -8127,8 +8528,8 @@
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="56"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="58"/>
       <c r="O16" t="s">
         <v>414</v>
       </c>
@@ -8136,7 +8537,7 @@
         <v>427</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>P1[20]</v>
       </c>
     </row>
@@ -8163,8 +8564,8 @@
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="56"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="58"/>
       <c r="O17" t="s">
         <v>413</v>
       </c>
@@ -8172,7 +8573,7 @@
         <v>426</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>P1[21]</v>
       </c>
     </row>
@@ -8199,10 +8600,10 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="57" t="s">
+      <c r="M18" s="60" t="s">
         <v>412</v>
       </c>
-      <c r="N18" s="56" t="s">
+      <c r="N18" s="58" t="s">
         <v>433</v>
       </c>
       <c r="O18" t="s">
@@ -8212,7 +8613,7 @@
         <v>429</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" ref="Q18:Q21" si="2">I18</f>
+        <f t="shared" ref="Q18:Q21" si="3">I18</f>
         <v>P1[22]</v>
       </c>
     </row>
@@ -8241,8 +8642,8 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="56"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="58"/>
       <c r="O19" t="s">
         <v>415</v>
       </c>
@@ -8250,7 +8651,7 @@
         <v>428</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>P1[23]</v>
       </c>
     </row>
@@ -8279,8 +8680,8 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="56"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="58"/>
       <c r="O20" t="s">
         <v>414</v>
       </c>
@@ -8288,7 +8689,7 @@
         <v>427</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>P1[24]</v>
       </c>
     </row>
@@ -8315,8 +8716,8 @@
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="56"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="58"/>
       <c r="O21" t="s">
         <v>413</v>
       </c>
@@ -8324,7 +8725,7 @@
         <v>426</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>P1[25]</v>
       </c>
     </row>
@@ -8351,10 +8752,10 @@
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
-      <c r="M22" s="57" t="s">
+      <c r="M22" s="60" t="s">
         <v>412</v>
       </c>
-      <c r="N22" s="56" t="s">
+      <c r="N22" s="58" t="s">
         <v>432</v>
       </c>
       <c r="O22" t="s">
@@ -8364,7 +8765,7 @@
         <v>429</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ref="Q22:Q25" si="3">I22</f>
+        <f t="shared" ref="Q22:Q25" si="4">I22</f>
         <v>P1[26]</v>
       </c>
     </row>
@@ -8391,8 +8792,8 @@
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="56"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="58"/>
       <c r="O23" t="s">
         <v>415</v>
       </c>
@@ -8400,7 +8801,7 @@
         <v>428</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>P1[27]</v>
       </c>
     </row>
@@ -8427,8 +8828,8 @@
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="56"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="58"/>
       <c r="O24" t="s">
         <v>414</v>
       </c>
@@ -8436,7 +8837,7 @@
         <v>427</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>P1[28]</v>
       </c>
     </row>
@@ -8463,8 +8864,8 @@
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="56"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="58"/>
       <c r="O25" t="s">
         <v>413</v>
       </c>
@@ -8472,7 +8873,7 @@
         <v>426</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>P1[29]</v>
       </c>
     </row>
@@ -8501,10 +8902,10 @@
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
-      <c r="M26" s="57" t="s">
+      <c r="M26" s="60" t="s">
         <v>424</v>
       </c>
-      <c r="N26" s="56" t="s">
+      <c r="N26" s="58" t="s">
         <v>431</v>
       </c>
       <c r="O26" t="s">
@@ -8543,8 +8944,8 @@
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="56"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="58"/>
       <c r="O27" t="s">
         <v>414</v>
       </c>
@@ -8552,7 +8953,7 @@
         <v>427</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" ref="Q27:Q37" si="4">I27</f>
+        <f t="shared" ref="Q27:Q41" si="5">I27</f>
         <v>P0[1]</v>
       </c>
     </row>
@@ -8585,16 +8986,16 @@
         <v>300</v>
       </c>
       <c r="L28" s="27"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="58" t="s">
+      <c r="M28" s="60"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="56" t="s">
         <v>416</v>
       </c>
-      <c r="P28" s="58" t="s">
+      <c r="P28" s="56" t="s">
         <v>429</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P0[10]</v>
       </c>
     </row>
@@ -8627,16 +9028,16 @@
         <v>297</v>
       </c>
       <c r="L29" s="27"/>
-      <c r="M29" s="57"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="58" t="s">
+      <c r="M29" s="60"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="56" t="s">
         <v>415</v>
       </c>
-      <c r="P29" s="58" t="s">
+      <c r="P29" s="56" t="s">
         <v>428</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P0[11]</v>
       </c>
     </row>
@@ -8663,7 +9064,7 @@
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29"/>
-      <c r="N30" s="56" t="s">
+      <c r="N30" s="58" t="s">
         <v>425</v>
       </c>
       <c r="O30" t="s">
@@ -8673,7 +9074,7 @@
         <v>426</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P2[13]</v>
       </c>
     </row>
@@ -8700,7 +9101,7 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="N31" s="56"/>
+      <c r="N31" s="58"/>
       <c r="O31" t="s">
         <v>414</v>
       </c>
@@ -8708,7 +9109,7 @@
         <v>427</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P2[12]</v>
       </c>
     </row>
@@ -8735,7 +9136,7 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="29"/>
-      <c r="N32" s="56"/>
+      <c r="N32" s="58"/>
       <c r="O32" t="s">
         <v>415</v>
       </c>
@@ -8743,7 +9144,7 @@
         <v>428</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P2[11]</v>
       </c>
     </row>
@@ -8772,7 +9173,7 @@
       </c>
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
-      <c r="N33" s="56"/>
+      <c r="N33" s="58"/>
       <c r="O33" t="s">
         <v>416</v>
       </c>
@@ -8780,7 +9181,7 @@
         <v>429</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P2[10]</v>
       </c>
     </row>
@@ -8807,7 +9208,7 @@
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
-      <c r="N34" s="56" t="s">
+      <c r="N34" s="58" t="s">
         <v>430</v>
       </c>
       <c r="O34" t="s">
@@ -8817,7 +9218,7 @@
         <v>426</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P0[22]</v>
       </c>
     </row>
@@ -8844,7 +9245,7 @@
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
-      <c r="N35" s="56"/>
+      <c r="N35" s="58"/>
       <c r="O35" t="s">
         <v>414</v>
       </c>
@@ -8852,7 +9253,7 @@
         <v>427</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P0[21]</v>
       </c>
     </row>
@@ -8883,7 +9284,7 @@
         <v>287</v>
       </c>
       <c r="L36" s="24"/>
-      <c r="N36" s="56"/>
+      <c r="N36" s="58"/>
       <c r="O36" t="s">
         <v>415</v>
       </c>
@@ -8891,7 +9292,7 @@
         <v>428</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P0[20]</v>
       </c>
     </row>
@@ -8922,7 +9323,7 @@
         <v>290</v>
       </c>
       <c r="L37" s="24"/>
-      <c r="N37" s="56"/>
+      <c r="N37" s="58"/>
       <c r="O37" t="s">
         <v>416</v>
       </c>
@@ -8930,7 +9331,7 @@
         <v>429</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>P0[19]</v>
       </c>
     </row>
@@ -8961,6 +9362,19 @@
         <v>257</v>
       </c>
       <c r="L38" s="25"/>
+      <c r="N38" s="58" t="s">
+        <v>439</v>
+      </c>
+      <c r="O38" t="s">
+        <v>413</v>
+      </c>
+      <c r="P38" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="5"/>
+        <v>P0[18]</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
@@ -8989,6 +9403,17 @@
         <v>261</v>
       </c>
       <c r="L39" s="25"/>
+      <c r="N39" s="58"/>
+      <c r="O39" t="s">
+        <v>414</v>
+      </c>
+      <c r="P39" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="5"/>
+        <v>P0[17]</v>
+      </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
@@ -9017,6 +9442,17 @@
         <v>264</v>
       </c>
       <c r="L40" s="25"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="P40" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="5"/>
+        <v>P0[15]</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
@@ -9046,6 +9482,17 @@
       </c>
       <c r="L41" s="25" t="s">
         <v>268</v>
+      </c>
+      <c r="N41" s="58"/>
+      <c r="O41" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="P41" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" si="5"/>
+        <v>P0[16]</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -9096,10 +9543,21 @@
         <v>229</v>
       </c>
       <c r="J43" s="23"/>
-      <c r="K43" s="23" t="s">
-        <v>230</v>
-      </c>
+      <c r="K43" s="23"/>
       <c r="L43" s="23"/>
+      <c r="N43" t="s">
+        <v>443</v>
+      </c>
+      <c r="O43" t="s">
+        <v>413</v>
+      </c>
+      <c r="P43" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" ref="Q43:Q47" si="6">I43</f>
+        <v>P2[8]</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
@@ -9124,6 +9582,19 @@
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
+      <c r="N44" s="58" t="s">
+        <v>440</v>
+      </c>
+      <c r="O44" t="s">
+        <v>413</v>
+      </c>
+      <c r="P44" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" si="6"/>
+        <v>P2[7]</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
@@ -9148,6 +9619,17 @@
       <c r="J45" s="23"/>
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
+      <c r="N45" s="58"/>
+      <c r="O45" t="s">
+        <v>414</v>
+      </c>
+      <c r="P45" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" si="6"/>
+        <v>P2[6]</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
@@ -9174,6 +9656,17 @@
       </c>
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
+      <c r="N46" s="58"/>
+      <c r="O46" t="s">
+        <v>415</v>
+      </c>
+      <c r="P46" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" si="6"/>
+        <v>P2[5]</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
@@ -9200,6 +9693,17 @@
       </c>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
+      <c r="N47" s="58"/>
+      <c r="O47" t="s">
+        <v>416</v>
+      </c>
+      <c r="P47" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" si="6"/>
+        <v>P2[4]</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
@@ -9226,8 +9730,21 @@
       </c>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N48" s="58" t="s">
+        <v>434</v>
+      </c>
+      <c r="O48" t="s">
+        <v>413</v>
+      </c>
+      <c r="P48" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q48" t="str">
+        <f>I48</f>
+        <v>P2[3]</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>126</v>
       </c>
@@ -9252,8 +9769,19 @@
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N49" s="58"/>
+      <c r="O49" t="s">
+        <v>414</v>
+      </c>
+      <c r="P49" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" ref="Q49:Q51" si="7">I49</f>
+        <v>P2[2]</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>128</v>
       </c>
@@ -9280,8 +9808,19 @@
         <v>241</v>
       </c>
       <c r="L50" s="23"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N50" s="58"/>
+      <c r="O50" t="s">
+        <v>415</v>
+      </c>
+      <c r="P50" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" si="7"/>
+        <v>P2[1]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
         <v>130</v>
       </c>
@@ -9308,8 +9847,19 @@
         <v>245</v>
       </c>
       <c r="L51" s="23"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N51" s="58"/>
+      <c r="O51" t="s">
+        <v>416</v>
+      </c>
+      <c r="P51" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" si="7"/>
+        <v>P2[0]</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="38" t="s">
         <v>132</v>
       </c>
@@ -9335,7 +9885,7 @@
       <c r="K52" s="49"/>
       <c r="L52" s="50"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="38" t="s">
         <v>134</v>
       </c>
@@ -9361,7 +9911,7 @@
       <c r="K53" s="49"/>
       <c r="L53" s="50"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="38" t="s">
         <v>135</v>
       </c>
@@ -9387,7 +9937,7 @@
       <c r="K54" s="49"/>
       <c r="L54" s="50"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
         <v>136</v>
       </c>
@@ -9413,7 +9963,7 @@
       <c r="K55" s="49"/>
       <c r="L55" s="50"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>137</v>
       </c>
@@ -9436,8 +9986,21 @@
       <c r="J56" s="24"/>
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N56" s="58" t="s">
+        <v>442</v>
+      </c>
+      <c r="O56" t="s">
+        <v>413</v>
+      </c>
+      <c r="P56" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q56" t="str">
+        <f>I56</f>
+        <v>P0[5]</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>139</v>
       </c>
@@ -9460,8 +10023,19 @@
       <c r="J57" s="24"/>
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N57" s="58"/>
+      <c r="O57" t="s">
+        <v>414</v>
+      </c>
+      <c r="P57" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" ref="Q57:Q63" si="8">I57</f>
+        <v>P0[4]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
         <v>141</v>
       </c>
@@ -9486,8 +10060,19 @@
       <c r="L58" s="24" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N58" s="58"/>
+      <c r="O58" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="P58" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q58" t="str">
+        <f t="shared" si="8"/>
+        <v>P4[28]</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
         <v>144</v>
       </c>
@@ -9512,8 +10097,19 @@
       <c r="L59" s="24" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N59" s="58"/>
+      <c r="O59" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="P59" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q59" t="str">
+        <f t="shared" si="8"/>
+        <v>P4[29]</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>146</v>
       </c>
@@ -9538,8 +10134,21 @@
       </c>
       <c r="K60" s="29"/>
       <c r="L60" s="29"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N60" s="58" t="s">
+        <v>444</v>
+      </c>
+      <c r="O60" t="s">
+        <v>413</v>
+      </c>
+      <c r="P60" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q60" t="str">
+        <f t="shared" si="8"/>
+        <v>P1[17]</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>148</v>
       </c>
@@ -9564,8 +10173,19 @@
       </c>
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N61" s="58"/>
+      <c r="O61" t="s">
+        <v>414</v>
+      </c>
+      <c r="P61" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q61" t="str">
+        <f t="shared" si="8"/>
+        <v>P1[16]</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
         <v>149</v>
       </c>
@@ -9590,8 +10210,19 @@
       </c>
       <c r="K62" s="29"/>
       <c r="L62" s="29"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N62" s="58"/>
+      <c r="O62" t="s">
+        <v>415</v>
+      </c>
+      <c r="P62" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q62" t="str">
+        <f t="shared" si="8"/>
+        <v>P1[15]</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>150</v>
       </c>
@@ -9616,8 +10247,19 @@
       </c>
       <c r="K63" s="29"/>
       <c r="L63" s="29"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N63" s="58"/>
+      <c r="O63" t="s">
+        <v>416</v>
+      </c>
+      <c r="P63" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q63" t="str">
+        <f t="shared" si="8"/>
+        <v>P1[14]</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
         <v>151</v>
       </c>
@@ -9642,6 +10284,19 @@
       </c>
       <c r="K64" s="30"/>
       <c r="L64" s="30"/>
+      <c r="N64" s="58" t="s">
+        <v>445</v>
+      </c>
+      <c r="O64" t="s">
+        <v>413</v>
+      </c>
+      <c r="P64" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q64" t="str">
+        <f t="shared" ref="Q64:Q67" si="9">I64</f>
+        <v>P1[10]</v>
+      </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
@@ -9668,6 +10323,17 @@
       </c>
       <c r="K65" s="30"/>
       <c r="L65" s="30"/>
+      <c r="N65" s="58"/>
+      <c r="O65" t="s">
+        <v>414</v>
+      </c>
+      <c r="P65" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q65" t="str">
+        <f t="shared" si="9"/>
+        <v>P1[9]</v>
+      </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
@@ -9694,6 +10360,17 @@
       </c>
       <c r="K66" s="30"/>
       <c r="L66" s="30"/>
+      <c r="N66" s="58"/>
+      <c r="O66" t="s">
+        <v>415</v>
+      </c>
+      <c r="P66" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q66" t="str">
+        <f t="shared" si="9"/>
+        <v>P1[8]</v>
+      </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
@@ -9720,6 +10397,17 @@
       </c>
       <c r="K67" s="30"/>
       <c r="L67" s="30"/>
+      <c r="N67" s="58"/>
+      <c r="O67" t="s">
+        <v>416</v>
+      </c>
+      <c r="P67" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q67" t="str">
+        <f t="shared" si="9"/>
+        <v>P1[4]</v>
+      </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
@@ -9746,6 +10434,19 @@
       </c>
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
+      <c r="N68" t="s">
+        <v>443</v>
+      </c>
+      <c r="O68" t="s">
+        <v>416</v>
+      </c>
+      <c r="P68" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q68" t="str">
+        <f t="shared" ref="Q68:Q71" si="10">I68</f>
+        <v>P1[1]</v>
+      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
@@ -9772,6 +10473,19 @@
       </c>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
+      <c r="N69" t="s">
+        <v>443</v>
+      </c>
+      <c r="O69" t="s">
+        <v>415</v>
+      </c>
+      <c r="P69" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q69" t="str">
+        <f t="shared" si="10"/>
+        <v>P1[0]</v>
+      </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
@@ -9802,10 +10516,10 @@
         <v>219</v>
       </c>
       <c r="L70" s="13"/>
-      <c r="M70" s="57" t="s">
+      <c r="M70" s="60" t="s">
         <v>411</v>
       </c>
-      <c r="N70" s="56" t="s">
+      <c r="N70" s="58" t="s">
         <v>438</v>
       </c>
       <c r="O70" t="s">
@@ -9815,7 +10529,7 @@
         <v>429</v>
       </c>
       <c r="Q70" t="str">
-        <f t="shared" ref="Q70:Q71" si="5">I70</f>
+        <f t="shared" si="10"/>
         <v>P0[2]</v>
       </c>
     </row>
@@ -9848,8 +10562,8 @@
         <v>215</v>
       </c>
       <c r="L71" s="13"/>
-      <c r="M71" s="57"/>
-      <c r="N71" s="56"/>
+      <c r="M71" s="60"/>
+      <c r="N71" s="58"/>
       <c r="O71" t="s">
         <v>415</v>
       </c>
@@ -9857,12 +10571,12 @@
         <v>428</v>
       </c>
       <c r="Q71" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>P0[3]</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="N4:N7"/>
     <mergeCell ref="N2:N3"/>
@@ -9879,13 +10593,2763 @@
     <mergeCell ref="M14:M17"/>
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N60:N63"/>
+    <mergeCell ref="N64:N67"/>
+    <mergeCell ref="N38:N41"/>
+    <mergeCell ref="N48:N51"/>
+    <mergeCell ref="N56:N59"/>
+    <mergeCell ref="N44:N47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26:O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="36"/>
+    <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="142" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" s="61" t="s">
+        <v>448</v>
+      </c>
+      <c r="N1" t="s">
+        <v>447</v>
+      </c>
+      <c r="O1" t="s">
+        <v>446</v>
+      </c>
+      <c r="P1" s="61" t="s">
+        <v>449</v>
+      </c>
+      <c r="U1" t="s">
+        <v>222</v>
+      </c>
+      <c r="V1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="17">
+        <v>8</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22">
+        <v>1</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" t="s">
+        <v>413</v>
+      </c>
+      <c r="N2" t="s">
+        <v>426</v>
+      </c>
+      <c r="O2" t="str">
+        <f>I2</f>
+        <v>P0[24]</v>
+      </c>
+      <c r="P2" t="s">
+        <v>435</v>
+      </c>
+      <c r="T2" t="s">
+        <v>413</v>
+      </c>
+      <c r="W2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="17">
+        <v>9</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" t="s">
+        <v>414</v>
+      </c>
+      <c r="N3" t="s">
+        <v>427</v>
+      </c>
+      <c r="O3" t="str">
+        <f>I3</f>
+        <v>P0[23]</v>
+      </c>
+      <c r="P3" t="s">
+        <v>435</v>
+      </c>
+      <c r="T3" t="s">
+        <v>414</v>
+      </c>
+      <c r="W3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="17">
+        <v>20</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" t="s">
+        <v>415</v>
+      </c>
+      <c r="N4" t="s">
+        <v>428</v>
+      </c>
+      <c r="O4" t="str">
+        <f>I4</f>
+        <v>P1[31]</v>
+      </c>
+      <c r="P4" t="s">
+        <v>435</v>
+      </c>
+      <c r="T4" t="s">
+        <v>415</v>
+      </c>
+      <c r="U4" t="s">
+        <v>417</v>
+      </c>
+      <c r="V4" t="s">
+        <v>419</v>
+      </c>
+      <c r="W4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="B5" s="17">
+        <v>21</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" t="s">
+        <v>416</v>
+      </c>
+      <c r="N5" t="s">
+        <v>429</v>
+      </c>
+      <c r="O5" t="str">
+        <f>I5</f>
+        <v>P1[30]</v>
+      </c>
+      <c r="P5" t="s">
+        <v>435</v>
+      </c>
+      <c r="T5" t="s">
+        <v>416</v>
+      </c>
+      <c r="U5" t="s">
+        <v>418</v>
+      </c>
+      <c r="V5" t="s">
+        <v>420</v>
+      </c>
+      <c r="W5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="17">
+        <v>66</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" t="s">
+        <v>413</v>
+      </c>
+      <c r="N6" t="s">
+        <v>426</v>
+      </c>
+      <c r="O6" t="str">
+        <f>I6</f>
+        <v>P2[7]</v>
+      </c>
+      <c r="P6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="17">
+        <v>67</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" t="s">
+        <v>414</v>
+      </c>
+      <c r="N7" t="s">
+        <v>427</v>
+      </c>
+      <c r="O7" t="str">
+        <f>I7</f>
+        <v>P2[6]</v>
+      </c>
+      <c r="P7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="17">
+        <v>68</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="J8" s="65" t="s">
+        <v>276</v>
+      </c>
+      <c r="K8" s="71"/>
+      <c r="L8" s="76"/>
+      <c r="M8" t="s">
+        <v>415</v>
+      </c>
+      <c r="N8" t="s">
+        <v>428</v>
+      </c>
+      <c r="O8" t="str">
+        <f>I8</f>
+        <v>P2[5]</v>
+      </c>
+      <c r="P8" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="17">
+        <v>69</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="J9" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="K9" s="71"/>
+      <c r="L9" s="76"/>
+      <c r="M9" t="s">
+        <v>416</v>
+      </c>
+      <c r="N9" t="s">
+        <v>429</v>
+      </c>
+      <c r="O9" t="str">
+        <f>I9</f>
+        <v>P2[4]</v>
+      </c>
+      <c r="P9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="17">
+        <v>35</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" t="s">
+        <v>413</v>
+      </c>
+      <c r="N10" t="s">
+        <v>426</v>
+      </c>
+      <c r="O10" t="str">
+        <f>I10</f>
+        <v>P1[21]</v>
+      </c>
+      <c r="P10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="17">
+        <v>34</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" t="s">
+        <v>414</v>
+      </c>
+      <c r="N11" t="s">
+        <v>427</v>
+      </c>
+      <c r="O11" t="str">
+        <f>I11</f>
+        <v>P1[20]</v>
+      </c>
+      <c r="P11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B12" s="17">
+        <v>33</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="J12" s="68"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="78"/>
+      <c r="M12" t="s">
+        <v>415</v>
+      </c>
+      <c r="N12" t="s">
+        <v>428</v>
+      </c>
+      <c r="O12" t="str">
+        <f>I12</f>
+        <v>P1[19]</v>
+      </c>
+      <c r="P12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="17">
+        <v>32</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="J13" s="65"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="76"/>
+      <c r="M13" t="s">
+        <v>416</v>
+      </c>
+      <c r="N13" t="s">
+        <v>429</v>
+      </c>
+      <c r="O13" t="str">
+        <f>I13</f>
+        <v>P1[18]</v>
+      </c>
+      <c r="P13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="17">
+        <v>80</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" t="s">
+        <v>413</v>
+      </c>
+      <c r="N14" t="s">
+        <v>426</v>
+      </c>
+      <c r="O14" t="str">
+        <f>I14</f>
+        <v>P0[5]</v>
+      </c>
+      <c r="P14" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="17">
+        <v>81</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" t="s">
+        <v>414</v>
+      </c>
+      <c r="N15" t="s">
+        <v>427</v>
+      </c>
+      <c r="O15" t="str">
+        <f>I15</f>
+        <v>P0[4]</v>
+      </c>
+      <c r="P15" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="17">
+        <v>85</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="M16" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="N16" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="O16" t="str">
+        <f>I16</f>
+        <v>P4[29]</v>
+      </c>
+      <c r="P16" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="17">
+        <v>82</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="M17" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="N17" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="O17" t="str">
+        <f>I17</f>
+        <v>P4[28]</v>
+      </c>
+      <c r="P17" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="17">
+        <v>65</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" t="s">
+        <v>413</v>
+      </c>
+      <c r="N18" t="s">
+        <v>426</v>
+      </c>
+      <c r="O18" t="str">
+        <f>I18</f>
+        <v>P2[8]</v>
+      </c>
+      <c r="P18" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="17">
+        <v>26</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" t="s">
+        <v>414</v>
+      </c>
+      <c r="N19" t="s">
+        <v>427</v>
+      </c>
+      <c r="O19" t="str">
+        <f>I19</f>
+        <v>P3[26]</v>
+      </c>
+      <c r="P19" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="17">
+        <v>95</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" t="s">
+        <v>415</v>
+      </c>
+      <c r="N20" t="s">
+        <v>428</v>
+      </c>
+      <c r="O20" t="str">
+        <f>I20</f>
+        <v>P1[0]</v>
+      </c>
+      <c r="P20" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="17">
+        <v>94</v>
+      </c>
+      <c r="C21" s="22">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" t="s">
+        <v>416</v>
+      </c>
+      <c r="N21" t="s">
+        <v>429</v>
+      </c>
+      <c r="O21" t="str">
+        <f>I21</f>
+        <v>P1[1]</v>
+      </c>
+      <c r="P21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="17">
+        <v>86</v>
+      </c>
+      <c r="C22" s="22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" t="s">
+        <v>413</v>
+      </c>
+      <c r="N22" t="s">
+        <v>426</v>
+      </c>
+      <c r="O22" t="str">
+        <f>I22</f>
+        <v>P1[17]</v>
+      </c>
+      <c r="P22" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" s="17">
+        <v>87</v>
+      </c>
+      <c r="C23" s="22">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" t="s">
+        <v>414</v>
+      </c>
+      <c r="N23" t="s">
+        <v>427</v>
+      </c>
+      <c r="O23" t="str">
+        <f>I23</f>
+        <v>P1[16]</v>
+      </c>
+      <c r="P23" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="17">
+        <v>88</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" t="s">
+        <v>415</v>
+      </c>
+      <c r="N24" t="s">
+        <v>428</v>
+      </c>
+      <c r="O24" t="str">
+        <f>I24</f>
+        <v>P1[15]</v>
+      </c>
+      <c r="P24" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="17">
+        <v>89</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1</v>
+      </c>
+      <c r="D25" s="22"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" t="s">
+        <v>416</v>
+      </c>
+      <c r="N25" t="s">
+        <v>429</v>
+      </c>
+      <c r="O25" t="str">
+        <f>I25</f>
+        <v>P1[14]</v>
+      </c>
+      <c r="P25" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="17">
+        <v>90</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" t="s">
+        <v>413</v>
+      </c>
+      <c r="N26" t="s">
+        <v>426</v>
+      </c>
+      <c r="O26" t="str">
+        <f>I26</f>
+        <v>P1[10]</v>
+      </c>
+      <c r="P26" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" s="17">
+        <v>91</v>
+      </c>
+      <c r="C27" s="22">
+        <v>1</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" t="s">
+        <v>414</v>
+      </c>
+      <c r="N27" t="s">
+        <v>427</v>
+      </c>
+      <c r="O27" t="str">
+        <f>I27</f>
+        <v>P1[9]</v>
+      </c>
+      <c r="P27" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="17">
+        <v>92</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="J28" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" t="s">
+        <v>415</v>
+      </c>
+      <c r="N28" t="s">
+        <v>428</v>
+      </c>
+      <c r="O28" t="str">
+        <f>I28</f>
+        <v>P1[8]</v>
+      </c>
+      <c r="P28" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="17">
+        <v>93</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" t="s">
+        <v>416</v>
+      </c>
+      <c r="N29" t="s">
+        <v>429</v>
+      </c>
+      <c r="O29" t="str">
+        <f>I29</f>
+        <v>P1[4]</v>
+      </c>
+      <c r="P29" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="17">
+        <v>70</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" t="s">
+        <v>413</v>
+      </c>
+      <c r="N30" t="s">
+        <v>426</v>
+      </c>
+      <c r="O30" t="str">
+        <f>I30</f>
+        <v>P2[3]</v>
+      </c>
+      <c r="P30" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="17">
+        <v>73</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" t="s">
+        <v>414</v>
+      </c>
+      <c r="N31" t="s">
+        <v>427</v>
+      </c>
+      <c r="O31" t="str">
+        <f>I31</f>
+        <v>P2[2]</v>
+      </c>
+      <c r="P31" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="17">
+        <v>74</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22">
+        <v>1</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J32" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="K32" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="L32" s="23"/>
+      <c r="M32" t="s">
+        <v>415</v>
+      </c>
+      <c r="N32" t="s">
+        <v>428</v>
+      </c>
+      <c r="O32" t="str">
+        <f>I32</f>
+        <v>P2[1]</v>
+      </c>
+      <c r="P32" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="17">
+        <v>75</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="J33" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="K33" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="L33" s="23"/>
+      <c r="M33" t="s">
+        <v>416</v>
+      </c>
+      <c r="N33" t="s">
+        <v>429</v>
+      </c>
+      <c r="O33" t="str">
+        <f>I33</f>
+        <v>P2[0]</v>
+      </c>
+      <c r="P33" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="17">
+        <v>39</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" t="s">
+        <v>413</v>
+      </c>
+      <c r="N34" t="s">
+        <v>426</v>
+      </c>
+      <c r="O34" t="str">
+        <f>I34</f>
+        <v>P1[25]</v>
+      </c>
+      <c r="P34" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="17">
+        <v>38</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22">
+        <v>1</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" t="s">
+        <v>414</v>
+      </c>
+      <c r="N35" t="s">
+        <v>427</v>
+      </c>
+      <c r="O35" t="str">
+        <f>I35</f>
+        <v>P1[24]</v>
+      </c>
+      <c r="P35" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="17">
+        <v>37</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22">
+        <v>1</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" t="s">
+        <v>415</v>
+      </c>
+      <c r="N36" t="s">
+        <v>428</v>
+      </c>
+      <c r="O36" t="str">
+        <f>I36</f>
+        <v>P1[23]</v>
+      </c>
+      <c r="P36" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="17">
+        <v>36</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" t="s">
+        <v>416</v>
+      </c>
+      <c r="N37" t="s">
+        <v>429</v>
+      </c>
+      <c r="O37" t="str">
+        <f>I37</f>
+        <v>P1[22]</v>
+      </c>
+      <c r="P37" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="17">
+        <v>45</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" t="s">
+        <v>413</v>
+      </c>
+      <c r="N38" t="s">
+        <v>426</v>
+      </c>
+      <c r="O38" t="str">
+        <f>I38</f>
+        <v>P1[29]</v>
+      </c>
+      <c r="P38" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="17">
+        <v>44</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" t="s">
+        <v>414</v>
+      </c>
+      <c r="N39" t="s">
+        <v>427</v>
+      </c>
+      <c r="O39" t="str">
+        <f>I39</f>
+        <v>P1[28]</v>
+      </c>
+      <c r="P39" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="B40" s="17">
+        <v>43</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22">
+        <v>1</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I40" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" t="s">
+        <v>415</v>
+      </c>
+      <c r="N40" t="s">
+        <v>428</v>
+      </c>
+      <c r="O40" t="str">
+        <f>I40</f>
+        <v>P1[27]</v>
+      </c>
+      <c r="P40" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="17">
+        <v>40</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" t="s">
+        <v>416</v>
+      </c>
+      <c r="N41" t="s">
+        <v>429</v>
+      </c>
+      <c r="O41" t="str">
+        <f>I41</f>
+        <v>P1[26]</v>
+      </c>
+      <c r="P41" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="17">
+        <v>46</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22">
+        <v>1</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="22">
+        <v>1</v>
+      </c>
+      <c r="G42" s="22"/>
+      <c r="H42" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="J42" s="63"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="75"/>
+      <c r="M42" t="s">
+        <v>413</v>
+      </c>
+      <c r="N42" t="s">
+        <v>426</v>
+      </c>
+      <c r="O42" t="str">
+        <f>I42</f>
+        <v>P0[0]</v>
+      </c>
+      <c r="P42" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="17">
+        <v>47</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22">
+        <v>1</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="22">
+        <v>1</v>
+      </c>
+      <c r="G43" s="22"/>
+      <c r="H43" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" t="s">
+        <v>414</v>
+      </c>
+      <c r="N43" t="s">
+        <v>427</v>
+      </c>
+      <c r="O43" t="str">
+        <f>I43</f>
+        <v>P0[1]</v>
+      </c>
+      <c r="P43" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="17">
+        <v>49</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="22">
+        <v>1</v>
+      </c>
+      <c r="G44" s="22"/>
+      <c r="H44" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="J44" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="K44" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="L44" s="27"/>
+      <c r="M44" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="N44" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="O44" t="str">
+        <f>I44</f>
+        <v>P0[11]</v>
+      </c>
+      <c r="P44" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="17">
+        <v>48</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22">
+        <v>1</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="22">
+        <v>1</v>
+      </c>
+      <c r="G45" s="22"/>
+      <c r="H45" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="J45" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="K45" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="L45" s="27"/>
+      <c r="M45" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="N45" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="O45" t="str">
+        <f>I45</f>
+        <v>P0[10]</v>
+      </c>
+      <c r="P45" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="17">
+        <v>50</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22">
+        <v>1</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" t="s">
+        <v>413</v>
+      </c>
+      <c r="N46" t="s">
+        <v>426</v>
+      </c>
+      <c r="O46" t="str">
+        <f>I46</f>
+        <v>P2[13]</v>
+      </c>
+      <c r="P46" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="17">
+        <v>51</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22">
+        <v>1</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" t="s">
+        <v>414</v>
+      </c>
+      <c r="N47" t="s">
+        <v>427</v>
+      </c>
+      <c r="O47" t="str">
+        <f>I47</f>
+        <v>P2[12]</v>
+      </c>
+      <c r="P47" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="17">
+        <v>52</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22">
+        <v>1</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" t="s">
+        <v>415</v>
+      </c>
+      <c r="N48" t="s">
+        <v>428</v>
+      </c>
+      <c r="O48" t="str">
+        <f>I48</f>
+        <v>P2[11]</v>
+      </c>
+      <c r="P48" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="52">
+        <v>53</v>
+      </c>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53">
+        <v>1</v>
+      </c>
+      <c r="E49" s="51"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="I49" s="51" t="s">
+        <v>309</v>
+      </c>
+      <c r="J49" s="55" t="s">
+        <v>409</v>
+      </c>
+      <c r="K49" s="55"/>
+      <c r="L49" s="55"/>
+      <c r="M49" t="s">
+        <v>416</v>
+      </c>
+      <c r="N49" t="s">
+        <v>429</v>
+      </c>
+      <c r="O49" t="str">
+        <f>I49</f>
+        <v>P2[10]</v>
+      </c>
+      <c r="P49" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="17">
+        <v>56</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22">
+        <v>1</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24"/>
+      <c r="M50" t="s">
+        <v>413</v>
+      </c>
+      <c r="N50" t="s">
+        <v>426</v>
+      </c>
+      <c r="O50" t="str">
+        <f>I50</f>
+        <v>P0[22]</v>
+      </c>
+      <c r="P50" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="17">
+        <v>57</v>
+      </c>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22">
+        <v>1</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" t="s">
+        <v>414</v>
+      </c>
+      <c r="N51" t="s">
+        <v>427</v>
+      </c>
+      <c r="O51" t="str">
+        <f>I51</f>
+        <v>P0[21]</v>
+      </c>
+      <c r="P51" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="17">
+        <v>58</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22">
+        <v>1</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="22">
+        <v>1</v>
+      </c>
+      <c r="G52" s="22"/>
+      <c r="H52" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="J52" s="67"/>
+      <c r="K52" s="72" t="s">
+        <v>287</v>
+      </c>
+      <c r="L52" s="77"/>
+      <c r="M52" t="s">
+        <v>415</v>
+      </c>
+      <c r="N52" t="s">
+        <v>428</v>
+      </c>
+      <c r="O52" t="str">
+        <f>I52</f>
+        <v>P0[20]</v>
+      </c>
+      <c r="P52" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="17">
+        <v>59</v>
+      </c>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22">
+        <v>1</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="22">
+        <v>1</v>
+      </c>
+      <c r="G53" s="22"/>
+      <c r="H53" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="J53" s="67"/>
+      <c r="K53" s="72" t="s">
+        <v>290</v>
+      </c>
+      <c r="L53" s="77"/>
+      <c r="M53" t="s">
+        <v>416</v>
+      </c>
+      <c r="N53" t="s">
+        <v>429</v>
+      </c>
+      <c r="O53" t="str">
+        <f>I53</f>
+        <v>P0[19]</v>
+      </c>
+      <c r="P53" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="17">
+        <v>7</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22">
+        <v>1</v>
+      </c>
+      <c r="E54" s="22">
+        <v>1</v>
+      </c>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="J54" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="K54" s="74"/>
+      <c r="L54" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="M54" t="s">
+        <v>413</v>
+      </c>
+      <c r="N54" t="s">
+        <v>426</v>
+      </c>
+      <c r="O54" t="str">
+        <f>I54</f>
+        <v>P0[25]</v>
+      </c>
+      <c r="P54" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55" s="17">
+        <v>6</v>
+      </c>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22">
+        <v>1</v>
+      </c>
+      <c r="E55" s="22">
+        <v>1</v>
+      </c>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="J55" s="69" t="s">
+        <v>198</v>
+      </c>
+      <c r="K55" s="74" t="s">
+        <v>199</v>
+      </c>
+      <c r="L55" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="M55" s="57" t="s">
+        <v>414</v>
+      </c>
+      <c r="N55" t="s">
+        <v>427</v>
+      </c>
+      <c r="O55" t="str">
+        <f>I55</f>
+        <v>P0[26]</v>
+      </c>
+      <c r="P55" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="17">
+        <v>99</v>
+      </c>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22">
+        <v>1</v>
+      </c>
+      <c r="E56" s="22">
+        <v>1</v>
+      </c>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J56" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="K56" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="L56" s="13"/>
+      <c r="M56" t="s">
+        <v>415</v>
+      </c>
+      <c r="N56" t="s">
+        <v>428</v>
+      </c>
+      <c r="O56" t="str">
+        <f>I56</f>
+        <v>P0[3]</v>
+      </c>
+      <c r="P56" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" s="17">
+        <v>98</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22">
+        <v>1</v>
+      </c>
+      <c r="E57" s="22">
+        <v>1</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="J57" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="K57" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="L57" s="13"/>
+      <c r="M57" t="s">
+        <v>416</v>
+      </c>
+      <c r="N57" t="s">
+        <v>429</v>
+      </c>
+      <c r="O57" t="str">
+        <f>I57</f>
+        <v>P0[2]</v>
+      </c>
+      <c r="P57" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="17">
+        <v>60</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22">
+        <v>1</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22">
+        <v>1</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="J58" s="25"/>
+      <c r="K58" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="L58" s="25"/>
+      <c r="M58" t="s">
+        <v>413</v>
+      </c>
+      <c r="N58" t="s">
+        <v>426</v>
+      </c>
+      <c r="O58" t="str">
+        <f>I58</f>
+        <v>P0[18]</v>
+      </c>
+      <c r="P58" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="17">
+        <v>61</v>
+      </c>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22">
+        <v>1</v>
+      </c>
+      <c r="E59" s="13"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22">
+        <v>1</v>
+      </c>
+      <c r="H59" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="J59" s="25"/>
+      <c r="K59" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="L59" s="25"/>
+      <c r="M59" t="s">
+        <v>414</v>
+      </c>
+      <c r="N59" t="s">
+        <v>427</v>
+      </c>
+      <c r="O59" t="str">
+        <f>I59</f>
+        <v>P0[17]</v>
+      </c>
+      <c r="P59" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="17">
+        <v>63</v>
+      </c>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22">
+        <v>1</v>
+      </c>
+      <c r="E60" s="13"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22">
+        <v>1</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="L60" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="M60" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="N60" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="O60" t="str">
+        <f>I60</f>
+        <v>P0[16]</v>
+      </c>
+      <c r="P60" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" s="17">
+        <v>62</v>
+      </c>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22">
+        <v>1</v>
+      </c>
+      <c r="E61" s="13"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22">
+        <v>1</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="J61" s="25"/>
+      <c r="K61" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="L61" s="25"/>
+      <c r="M61" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="N61" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="O61" t="str">
+        <f>I61</f>
+        <v>P0[15]</v>
+      </c>
+      <c r="P61" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="17">
+        <v>27</v>
+      </c>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22">
+        <v>1</v>
+      </c>
+      <c r="E62" s="13"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="J62" s="30"/>
+      <c r="K62" s="30"/>
+      <c r="L62" s="30"/>
+      <c r="P62" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="33">
+        <v>24</v>
+      </c>
+      <c r="C63" s="34">
+        <v>1</v>
+      </c>
+      <c r="D63" s="34"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I63" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="J63" s="64" t="s">
+        <v>403</v>
+      </c>
+      <c r="K63" s="64"/>
+      <c r="L63" s="64"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A64" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="33">
+        <v>25</v>
+      </c>
+      <c r="C64" s="34">
+        <v>1</v>
+      </c>
+      <c r="D64" s="34"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="J64" s="64" t="s">
+        <v>404</v>
+      </c>
+      <c r="K64" s="64"/>
+      <c r="L64" s="64"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="33">
+        <v>29</v>
+      </c>
+      <c r="C65" s="34">
+        <v>1</v>
+      </c>
+      <c r="D65" s="34"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I65" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="J65" s="64" t="s">
+        <v>401</v>
+      </c>
+      <c r="K65" s="64"/>
+      <c r="L65" s="64"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B66" s="33">
+        <v>30</v>
+      </c>
+      <c r="C66" s="34">
+        <v>1</v>
+      </c>
+      <c r="D66" s="34"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I66" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="J66" s="64" t="s">
+        <v>402</v>
+      </c>
+      <c r="K66" s="64"/>
+      <c r="L66" s="64"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="39">
+        <v>64</v>
+      </c>
+      <c r="C67" s="40">
+        <v>1</v>
+      </c>
+      <c r="D67" s="40"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I67" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="J67" s="62" t="s">
+        <v>400</v>
+      </c>
+      <c r="K67" s="62"/>
+      <c r="L67" s="62"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="39">
+        <v>76</v>
+      </c>
+      <c r="C68" s="40">
+        <v>1</v>
+      </c>
+      <c r="D68" s="40"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="40"/>
+      <c r="H68" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I68" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J68" s="66" t="s">
+        <v>405</v>
+      </c>
+      <c r="K68" s="66"/>
+      <c r="L68" s="66"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="39">
+        <v>77</v>
+      </c>
+      <c r="C69" s="40">
+        <v>1</v>
+      </c>
+      <c r="D69" s="40"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="40"/>
+      <c r="G69" s="40"/>
+      <c r="H69" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I69" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="J69" s="66" t="s">
+        <v>406</v>
+      </c>
+      <c r="K69" s="66"/>
+      <c r="L69" s="66"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" s="39">
+        <v>78</v>
+      </c>
+      <c r="C70" s="40">
+        <v>1</v>
+      </c>
+      <c r="D70" s="40"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="40"/>
+      <c r="H70" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I70" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="J70" s="66" t="s">
+        <v>407</v>
+      </c>
+      <c r="K70" s="66"/>
+      <c r="L70" s="66"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="39">
+        <v>79</v>
+      </c>
+      <c r="C71" s="40">
+        <v>1</v>
+      </c>
+      <c r="D71" s="40"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="40"/>
+      <c r="H71" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I71" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="J71" s="66" t="s">
+        <v>408</v>
+      </c>
+      <c r="K71" s="66"/>
+      <c r="L71" s="66"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:P71">
+    <sortCondition ref="P2:P71"/>
+    <sortCondition ref="M2:M71"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated pin map with swapping ISP0 and MRESET
</commit_message>
<xml_diff>
--- a/doc/LPC1769_pinmapping.xlsx
+++ b/doc/LPC1769_pinmapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="3"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LPC1769FBD100,551" sheetId="1" r:id="rId1"/>
@@ -2195,15 +2195,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -2225,6 +2216,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -7903,8 +7903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="S59" sqref="S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7999,8 +7999,8 @@
       <c r="L2" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="59" t="s">
+      <c r="M2" s="79"/>
+      <c r="N2" s="78" t="s">
         <v>438</v>
       </c>
       <c r="O2" s="57" t="s">
@@ -8049,8 +8049,8 @@
       <c r="L3" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="M3" s="60"/>
-      <c r="N3" s="59"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="78"/>
       <c r="O3" t="s">
         <v>413</v>
       </c>
@@ -8095,8 +8095,8 @@
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="58" t="s">
+      <c r="M4" s="79"/>
+      <c r="N4" s="77" t="s">
         <v>435</v>
       </c>
       <c r="O4" t="s">
@@ -8149,8 +8149,8 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="58"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="77"/>
       <c r="O5" t="s">
         <v>414</v>
       </c>
@@ -8203,8 +8203,8 @@
         <v>207</v>
       </c>
       <c r="L6" s="16"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="58"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="77"/>
       <c r="O6" t="s">
         <v>415</v>
       </c>
@@ -8245,8 +8245,8 @@
         <v>211</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="58"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="77"/>
       <c r="O7" t="s">
         <v>416</v>
       </c>
@@ -8452,10 +8452,10 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
-      <c r="M14" s="60" t="s">
+      <c r="M14" s="79" t="s">
         <v>410</v>
       </c>
-      <c r="N14" s="58" t="s">
+      <c r="N14" s="77" t="s">
         <v>441</v>
       </c>
       <c r="O14" t="s">
@@ -8492,8 +8492,8 @@
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="58"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="77"/>
       <c r="O15" t="s">
         <v>415</v>
       </c>
@@ -8528,8 +8528,8 @@
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="58"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="77"/>
       <c r="O16" t="s">
         <v>414</v>
       </c>
@@ -8564,8 +8564,8 @@
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="58"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="77"/>
       <c r="O17" t="s">
         <v>413</v>
       </c>
@@ -8600,10 +8600,10 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="60" t="s">
+      <c r="M18" s="79" t="s">
         <v>412</v>
       </c>
-      <c r="N18" s="58" t="s">
+      <c r="N18" s="77" t="s">
         <v>433</v>
       </c>
       <c r="O18" t="s">
@@ -8642,8 +8642,8 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="58"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="77"/>
       <c r="O19" t="s">
         <v>415</v>
       </c>
@@ -8680,8 +8680,8 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="58"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="77"/>
       <c r="O20" t="s">
         <v>414</v>
       </c>
@@ -8716,8 +8716,8 @@
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="58"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="77"/>
       <c r="O21" t="s">
         <v>413</v>
       </c>
@@ -8752,10 +8752,10 @@
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
-      <c r="M22" s="60" t="s">
+      <c r="M22" s="79" t="s">
         <v>412</v>
       </c>
-      <c r="N22" s="58" t="s">
+      <c r="N22" s="77" t="s">
         <v>432</v>
       </c>
       <c r="O22" t="s">
@@ -8792,8 +8792,8 @@
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="58"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="77"/>
       <c r="O23" t="s">
         <v>415</v>
       </c>
@@ -8828,8 +8828,8 @@
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="58"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="77"/>
       <c r="O24" t="s">
         <v>414</v>
       </c>
@@ -8864,8 +8864,8 @@
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="58"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="77"/>
       <c r="O25" t="s">
         <v>413</v>
       </c>
@@ -8902,10 +8902,10 @@
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
-      <c r="M26" s="60" t="s">
+      <c r="M26" s="79" t="s">
         <v>424</v>
       </c>
-      <c r="N26" s="58" t="s">
+      <c r="N26" s="77" t="s">
         <v>431</v>
       </c>
       <c r="O26" t="s">
@@ -8944,8 +8944,8 @@
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="58"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="77"/>
       <c r="O27" t="s">
         <v>414</v>
       </c>
@@ -8986,8 +8986,8 @@
         <v>300</v>
       </c>
       <c r="L28" s="27"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="58"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="77"/>
       <c r="O28" s="56" t="s">
         <v>416</v>
       </c>
@@ -9028,8 +9028,8 @@
         <v>297</v>
       </c>
       <c r="L29" s="27"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="58"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="77"/>
       <c r="O29" s="56" t="s">
         <v>415</v>
       </c>
@@ -9064,7 +9064,7 @@
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29"/>
-      <c r="N30" s="58" t="s">
+      <c r="N30" s="77" t="s">
         <v>425</v>
       </c>
       <c r="O30" t="s">
@@ -9101,7 +9101,7 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="N31" s="58"/>
+      <c r="N31" s="77"/>
       <c r="O31" t="s">
         <v>414</v>
       </c>
@@ -9136,7 +9136,7 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="29"/>
-      <c r="N32" s="58"/>
+      <c r="N32" s="77"/>
       <c r="O32" t="s">
         <v>415</v>
       </c>
@@ -9173,7 +9173,7 @@
       </c>
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
-      <c r="N33" s="58"/>
+      <c r="N33" s="77"/>
       <c r="O33" t="s">
         <v>416</v>
       </c>
@@ -9208,7 +9208,7 @@
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
-      <c r="N34" s="58" t="s">
+      <c r="N34" s="77" t="s">
         <v>430</v>
       </c>
       <c r="O34" t="s">
@@ -9245,7 +9245,7 @@
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
-      <c r="N35" s="58"/>
+      <c r="N35" s="77"/>
       <c r="O35" t="s">
         <v>414</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>287</v>
       </c>
       <c r="L36" s="24"/>
-      <c r="N36" s="58"/>
+      <c r="N36" s="77"/>
       <c r="O36" t="s">
         <v>415</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>290</v>
       </c>
       <c r="L37" s="24"/>
-      <c r="N37" s="58"/>
+      <c r="N37" s="77"/>
       <c r="O37" t="s">
         <v>416</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>257</v>
       </c>
       <c r="L38" s="25"/>
-      <c r="N38" s="58" t="s">
+      <c r="N38" s="77" t="s">
         <v>439</v>
       </c>
       <c r="O38" t="s">
@@ -9403,7 +9403,7 @@
         <v>261</v>
       </c>
       <c r="L39" s="25"/>
-      <c r="N39" s="58"/>
+      <c r="N39" s="77"/>
       <c r="O39" t="s">
         <v>414</v>
       </c>
@@ -9442,7 +9442,7 @@
         <v>264</v>
       </c>
       <c r="L40" s="25"/>
-      <c r="N40" s="58"/>
+      <c r="N40" s="77"/>
       <c r="O40" s="56" t="s">
         <v>416</v>
       </c>
@@ -9483,7 +9483,7 @@
       <c r="L41" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="N41" s="58"/>
+      <c r="N41" s="77"/>
       <c r="O41" s="56" t="s">
         <v>415</v>
       </c>
@@ -9582,7 +9582,7 @@
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
-      <c r="N44" s="58" t="s">
+      <c r="N44" s="77" t="s">
         <v>440</v>
       </c>
       <c r="O44" t="s">
@@ -9619,7 +9619,7 @@
       <c r="J45" s="23"/>
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
-      <c r="N45" s="58"/>
+      <c r="N45" s="77"/>
       <c r="O45" t="s">
         <v>414</v>
       </c>
@@ -9656,7 +9656,7 @@
       </c>
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
-      <c r="N46" s="58"/>
+      <c r="N46" s="77"/>
       <c r="O46" t="s">
         <v>415</v>
       </c>
@@ -9693,7 +9693,7 @@
       </c>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
-      <c r="N47" s="58"/>
+      <c r="N47" s="77"/>
       <c r="O47" t="s">
         <v>416</v>
       </c>
@@ -9730,7 +9730,7 @@
       </c>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
-      <c r="N48" s="58" t="s">
+      <c r="N48" s="77" t="s">
         <v>434</v>
       </c>
       <c r="O48" t="s">
@@ -9769,7 +9769,7 @@
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
-      <c r="N49" s="58"/>
+      <c r="N49" s="77"/>
       <c r="O49" t="s">
         <v>414</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>241</v>
       </c>
       <c r="L50" s="23"/>
-      <c r="N50" s="58"/>
+      <c r="N50" s="77"/>
       <c r="O50" t="s">
         <v>415</v>
       </c>
@@ -9847,7 +9847,7 @@
         <v>245</v>
       </c>
       <c r="L51" s="23"/>
-      <c r="N51" s="58"/>
+      <c r="N51" s="77"/>
       <c r="O51" t="s">
         <v>416</v>
       </c>
@@ -9986,7 +9986,7 @@
       <c r="J56" s="24"/>
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
-      <c r="N56" s="58" t="s">
+      <c r="N56" s="77" t="s">
         <v>442</v>
       </c>
       <c r="O56" t="s">
@@ -10023,7 +10023,7 @@
       <c r="J57" s="24"/>
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
-      <c r="N57" s="58"/>
+      <c r="N57" s="77"/>
       <c r="O57" t="s">
         <v>414</v>
       </c>
@@ -10060,7 +10060,7 @@
       <c r="L58" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="N58" s="58"/>
+      <c r="N58" s="77"/>
       <c r="O58" s="56" t="s">
         <v>416</v>
       </c>
@@ -10097,7 +10097,7 @@
       <c r="L59" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="N59" s="58"/>
+      <c r="N59" s="77"/>
       <c r="O59" s="56" t="s">
         <v>415</v>
       </c>
@@ -10134,7 +10134,7 @@
       </c>
       <c r="K60" s="29"/>
       <c r="L60" s="29"/>
-      <c r="N60" s="58" t="s">
+      <c r="N60" s="77" t="s">
         <v>444</v>
       </c>
       <c r="O60" t="s">
@@ -10173,7 +10173,7 @@
       </c>
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
-      <c r="N61" s="58"/>
+      <c r="N61" s="77"/>
       <c r="O61" t="s">
         <v>414</v>
       </c>
@@ -10210,7 +10210,7 @@
       </c>
       <c r="K62" s="29"/>
       <c r="L62" s="29"/>
-      <c r="N62" s="58"/>
+      <c r="N62" s="77"/>
       <c r="O62" t="s">
         <v>415</v>
       </c>
@@ -10247,7 +10247,7 @@
       </c>
       <c r="K63" s="29"/>
       <c r="L63" s="29"/>
-      <c r="N63" s="58"/>
+      <c r="N63" s="77"/>
       <c r="O63" t="s">
         <v>416</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
       <c r="K64" s="30"/>
       <c r="L64" s="30"/>
-      <c r="N64" s="58" t="s">
+      <c r="N64" s="77" t="s">
         <v>445</v>
       </c>
       <c r="O64" t="s">
@@ -10323,7 +10323,7 @@
       </c>
       <c r="K65" s="30"/>
       <c r="L65" s="30"/>
-      <c r="N65" s="58"/>
+      <c r="N65" s="77"/>
       <c r="O65" t="s">
         <v>414</v>
       </c>
@@ -10360,7 +10360,7 @@
       </c>
       <c r="K66" s="30"/>
       <c r="L66" s="30"/>
-      <c r="N66" s="58"/>
+      <c r="N66" s="77"/>
       <c r="O66" t="s">
         <v>415</v>
       </c>
@@ -10397,7 +10397,7 @@
       </c>
       <c r="K67" s="30"/>
       <c r="L67" s="30"/>
-      <c r="N67" s="58"/>
+      <c r="N67" s="77"/>
       <c r="O67" t="s">
         <v>416</v>
       </c>
@@ -10516,10 +10516,10 @@
         <v>219</v>
       </c>
       <c r="L70" s="13"/>
-      <c r="M70" s="60" t="s">
+      <c r="M70" s="79" t="s">
         <v>411</v>
       </c>
-      <c r="N70" s="58" t="s">
+      <c r="N70" s="77" t="s">
         <v>438</v>
       </c>
       <c r="O70" t="s">
@@ -10562,8 +10562,8 @@
         <v>215</v>
       </c>
       <c r="L71" s="13"/>
-      <c r="M71" s="60"/>
-      <c r="N71" s="58"/>
+      <c r="M71" s="79"/>
+      <c r="N71" s="77"/>
       <c r="O71" t="s">
         <v>415</v>
       </c>
@@ -10577,6 +10577,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="N60:N63"/>
+    <mergeCell ref="N64:N67"/>
+    <mergeCell ref="N38:N41"/>
+    <mergeCell ref="N48:N51"/>
+    <mergeCell ref="N56:N59"/>
+    <mergeCell ref="N44:N47"/>
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="N4:N7"/>
     <mergeCell ref="N2:N3"/>
@@ -10593,12 +10599,6 @@
     <mergeCell ref="M14:M17"/>
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N60:N63"/>
-    <mergeCell ref="N64:N67"/>
-    <mergeCell ref="N38:N41"/>
-    <mergeCell ref="N48:N51"/>
-    <mergeCell ref="N56:N59"/>
-    <mergeCell ref="N44:N47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -10610,7 +10610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="O26" sqref="O26:O29"/>
     </sheetView>
   </sheetViews>
@@ -10628,7 +10628,7 @@
     <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="142" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="141" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -10665,7 +10665,7 @@
       <c r="L1" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="58" t="s">
         <v>448</v>
       </c>
       <c r="N1" t="s">
@@ -10674,7 +10674,7 @@
       <c r="O1" t="s">
         <v>446</v>
       </c>
-      <c r="P1" s="61" t="s">
+      <c r="P1" s="58" t="s">
         <v>449</v>
       </c>
       <c r="U1" t="s">
@@ -10721,7 +10721,7 @@
         <v>426</v>
       </c>
       <c r="O2" t="str">
-        <f>I2</f>
+        <f t="shared" ref="O2:O33" si="0">I2</f>
         <v>P0[24]</v>
       </c>
       <c r="P2" t="s">
@@ -10768,7 +10768,7 @@
         <v>427</v>
       </c>
       <c r="O3" t="str">
-        <f>I3</f>
+        <f t="shared" si="0"/>
         <v>P0[23]</v>
       </c>
       <c r="P3" t="s">
@@ -10817,7 +10817,7 @@
         <v>428</v>
       </c>
       <c r="O4" t="str">
-        <f>I4</f>
+        <f t="shared" si="0"/>
         <v>P1[31]</v>
       </c>
       <c r="P4" t="s">
@@ -10872,7 +10872,7 @@
         <v>429</v>
       </c>
       <c r="O5" t="str">
-        <f>I5</f>
+        <f t="shared" si="0"/>
         <v>P1[30]</v>
       </c>
       <c r="P5" t="s">
@@ -10921,7 +10921,7 @@
         <v>426</v>
       </c>
       <c r="O6" t="str">
-        <f>I6</f>
+        <f t="shared" si="0"/>
         <v>P2[7]</v>
       </c>
       <c r="P6" t="s">
@@ -10958,7 +10958,7 @@
         <v>427</v>
       </c>
       <c r="O7" t="str">
-        <f>I7</f>
+        <f t="shared" si="0"/>
         <v>P2[6]</v>
       </c>
       <c r="P7" t="s">
@@ -10985,11 +10985,11 @@
       <c r="I8" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="K8" s="71"/>
-      <c r="L8" s="76"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="73"/>
       <c r="M8" t="s">
         <v>415</v>
       </c>
@@ -10997,7 +10997,7 @@
         <v>428</v>
       </c>
       <c r="O8" t="str">
-        <f>I8</f>
+        <f t="shared" si="0"/>
         <v>P2[5]</v>
       </c>
       <c r="P8" t="s">
@@ -11024,11 +11024,11 @@
       <c r="I9" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="J9" s="65" t="s">
+      <c r="J9" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="K9" s="71"/>
-      <c r="L9" s="76"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="73"/>
       <c r="M9" t="s">
         <v>416</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>429</v>
       </c>
       <c r="O9" t="str">
-        <f>I9</f>
+        <f t="shared" si="0"/>
         <v>P2[4]</v>
       </c>
       <c r="P9" t="s">
@@ -11073,7 +11073,7 @@
         <v>426</v>
       </c>
       <c r="O10" t="str">
-        <f>I10</f>
+        <f t="shared" si="0"/>
         <v>P1[21]</v>
       </c>
       <c r="P10" t="s">
@@ -11110,7 +11110,7 @@
         <v>427</v>
       </c>
       <c r="O11" t="str">
-        <f>I11</f>
+        <f t="shared" si="0"/>
         <v>P1[20]</v>
       </c>
       <c r="P11" t="s">
@@ -11137,9 +11137,9 @@
       <c r="I12" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="J12" s="68"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="78"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="75"/>
       <c r="M12" t="s">
         <v>415</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>428</v>
       </c>
       <c r="O12" t="str">
-        <f>I12</f>
+        <f t="shared" si="0"/>
         <v>P1[19]</v>
       </c>
       <c r="P12" t="s">
@@ -11174,9 +11174,9 @@
       <c r="I13" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="76"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="73"/>
       <c r="M13" t="s">
         <v>416</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>429</v>
       </c>
       <c r="O13" t="str">
-        <f>I13</f>
+        <f t="shared" si="0"/>
         <v>P1[18]</v>
       </c>
       <c r="P13" t="s">
@@ -11221,7 +11221,7 @@
         <v>426</v>
       </c>
       <c r="O14" t="str">
-        <f>I14</f>
+        <f t="shared" si="0"/>
         <v>P0[5]</v>
       </c>
       <c r="P14" t="s">
@@ -11258,7 +11258,7 @@
         <v>427</v>
       </c>
       <c r="O15" t="str">
-        <f>I15</f>
+        <f t="shared" si="0"/>
         <v>P0[4]</v>
       </c>
       <c r="P15" t="s">
@@ -11297,7 +11297,7 @@
         <v>428</v>
       </c>
       <c r="O16" t="str">
-        <f>I16</f>
+        <f t="shared" si="0"/>
         <v>P4[29]</v>
       </c>
       <c r="P16" t="s">
@@ -11336,7 +11336,7 @@
         <v>429</v>
       </c>
       <c r="O17" t="str">
-        <f>I17</f>
+        <f t="shared" si="0"/>
         <v>P4[28]</v>
       </c>
       <c r="P17" t="s">
@@ -11373,7 +11373,7 @@
         <v>426</v>
       </c>
       <c r="O18" t="str">
-        <f>I18</f>
+        <f t="shared" si="0"/>
         <v>P2[8]</v>
       </c>
       <c r="P18" t="s">
@@ -11410,7 +11410,7 @@
         <v>427</v>
       </c>
       <c r="O19" t="str">
-        <f>I19</f>
+        <f t="shared" si="0"/>
         <v>P3[26]</v>
       </c>
       <c r="P19" t="s">
@@ -11449,7 +11449,7 @@
         <v>428</v>
       </c>
       <c r="O20" t="str">
-        <f>I20</f>
+        <f t="shared" si="0"/>
         <v>P1[0]</v>
       </c>
       <c r="P20" t="s">
@@ -11488,7 +11488,7 @@
         <v>429</v>
       </c>
       <c r="O21" t="str">
-        <f>I21</f>
+        <f t="shared" si="0"/>
         <v>P1[1]</v>
       </c>
       <c r="P21" t="s">
@@ -11527,7 +11527,7 @@
         <v>426</v>
       </c>
       <c r="O22" t="str">
-        <f>I22</f>
+        <f t="shared" si="0"/>
         <v>P1[17]</v>
       </c>
       <c r="P22" t="s">
@@ -11566,7 +11566,7 @@
         <v>427</v>
       </c>
       <c r="O23" t="str">
-        <f>I23</f>
+        <f t="shared" si="0"/>
         <v>P1[16]</v>
       </c>
       <c r="P23" t="s">
@@ -11605,7 +11605,7 @@
         <v>428</v>
       </c>
       <c r="O24" t="str">
-        <f>I24</f>
+        <f t="shared" si="0"/>
         <v>P1[15]</v>
       </c>
       <c r="P24" t="s">
@@ -11644,7 +11644,7 @@
         <v>429</v>
       </c>
       <c r="O25" t="str">
-        <f>I25</f>
+        <f t="shared" si="0"/>
         <v>P1[14]</v>
       </c>
       <c r="P25" t="s">
@@ -11683,7 +11683,7 @@
         <v>426</v>
       </c>
       <c r="O26" t="str">
-        <f>I26</f>
+        <f t="shared" si="0"/>
         <v>P1[10]</v>
       </c>
       <c r="P26" t="s">
@@ -11722,7 +11722,7 @@
         <v>427</v>
       </c>
       <c r="O27" t="str">
-        <f>I27</f>
+        <f t="shared" si="0"/>
         <v>P1[9]</v>
       </c>
       <c r="P27" t="s">
@@ -11761,7 +11761,7 @@
         <v>428</v>
       </c>
       <c r="O28" t="str">
-        <f>I28</f>
+        <f t="shared" si="0"/>
         <v>P1[8]</v>
       </c>
       <c r="P28" t="s">
@@ -11800,7 +11800,7 @@
         <v>429</v>
       </c>
       <c r="O29" t="str">
-        <f>I29</f>
+        <f t="shared" si="0"/>
         <v>P1[4]</v>
       </c>
       <c r="P29" t="s">
@@ -11839,7 +11839,7 @@
         <v>426</v>
       </c>
       <c r="O30" t="str">
-        <f>I30</f>
+        <f t="shared" si="0"/>
         <v>P2[3]</v>
       </c>
       <c r="P30" t="s">
@@ -11878,7 +11878,7 @@
         <v>427</v>
       </c>
       <c r="O31" t="str">
-        <f>I31</f>
+        <f t="shared" si="0"/>
         <v>P2[2]</v>
       </c>
       <c r="P31" t="s">
@@ -11919,7 +11919,7 @@
         <v>428</v>
       </c>
       <c r="O32" t="str">
-        <f>I32</f>
+        <f t="shared" si="0"/>
         <v>P2[1]</v>
       </c>
       <c r="P32" t="s">
@@ -11960,7 +11960,7 @@
         <v>429</v>
       </c>
       <c r="O33" t="str">
-        <f>I33</f>
+        <f t="shared" si="0"/>
         <v>P2[0]</v>
       </c>
       <c r="P33" t="s">
@@ -11997,7 +11997,7 @@
         <v>426</v>
       </c>
       <c r="O34" t="str">
-        <f>I34</f>
+        <f t="shared" ref="O34:O61" si="1">I34</f>
         <v>P1[25]</v>
       </c>
       <c r="P34" t="s">
@@ -12036,7 +12036,7 @@
         <v>427</v>
       </c>
       <c r="O35" t="str">
-        <f>I35</f>
+        <f t="shared" si="1"/>
         <v>P1[24]</v>
       </c>
       <c r="P35" t="s">
@@ -12075,7 +12075,7 @@
         <v>428</v>
       </c>
       <c r="O36" t="str">
-        <f>I36</f>
+        <f t="shared" si="1"/>
         <v>P1[23]</v>
       </c>
       <c r="P36" t="s">
@@ -12112,7 +12112,7 @@
         <v>429</v>
       </c>
       <c r="O37" t="str">
-        <f>I37</f>
+        <f t="shared" si="1"/>
         <v>P1[22]</v>
       </c>
       <c r="P37" t="s">
@@ -12149,7 +12149,7 @@
         <v>426</v>
       </c>
       <c r="O38" t="str">
-        <f>I38</f>
+        <f t="shared" si="1"/>
         <v>P1[29]</v>
       </c>
       <c r="P38" t="s">
@@ -12186,7 +12186,7 @@
         <v>427</v>
       </c>
       <c r="O39" t="str">
-        <f>I39</f>
+        <f t="shared" si="1"/>
         <v>P1[28]</v>
       </c>
       <c r="P39" t="s">
@@ -12223,7 +12223,7 @@
         <v>428</v>
       </c>
       <c r="O40" t="str">
-        <f>I40</f>
+        <f t="shared" si="1"/>
         <v>P1[27]</v>
       </c>
       <c r="P40" t="s">
@@ -12260,7 +12260,7 @@
         <v>429</v>
       </c>
       <c r="O41" t="str">
-        <f>I41</f>
+        <f t="shared" si="1"/>
         <v>P1[26]</v>
       </c>
       <c r="P41" t="s">
@@ -12289,9 +12289,9 @@
       <c r="I42" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="J42" s="63"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="75"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="72"/>
       <c r="M42" t="s">
         <v>413</v>
       </c>
@@ -12299,7 +12299,7 @@
         <v>426</v>
       </c>
       <c r="O42" t="str">
-        <f>I42</f>
+        <f t="shared" si="1"/>
         <v>P0[0]</v>
       </c>
       <c r="P42" t="s">
@@ -12338,7 +12338,7 @@
         <v>427</v>
       </c>
       <c r="O43" t="str">
-        <f>I43</f>
+        <f t="shared" si="1"/>
         <v>P0[1]</v>
       </c>
       <c r="P43" t="s">
@@ -12381,7 +12381,7 @@
         <v>428</v>
       </c>
       <c r="O44" t="str">
-        <f>I44</f>
+        <f t="shared" si="1"/>
         <v>P0[11]</v>
       </c>
       <c r="P44" t="s">
@@ -12424,7 +12424,7 @@
         <v>429</v>
       </c>
       <c r="O45" t="str">
-        <f>I45</f>
+        <f t="shared" si="1"/>
         <v>P0[10]</v>
       </c>
       <c r="P45" t="s">
@@ -12461,7 +12461,7 @@
         <v>426</v>
       </c>
       <c r="O46" t="str">
-        <f>I46</f>
+        <f t="shared" si="1"/>
         <v>P2[13]</v>
       </c>
       <c r="P46" t="s">
@@ -12498,7 +12498,7 @@
         <v>427</v>
       </c>
       <c r="O47" t="str">
-        <f>I47</f>
+        <f t="shared" si="1"/>
         <v>P2[12]</v>
       </c>
       <c r="P47" t="s">
@@ -12535,7 +12535,7 @@
         <v>428</v>
       </c>
       <c r="O48" t="str">
-        <f>I48</f>
+        <f t="shared" si="1"/>
         <v>P2[11]</v>
       </c>
       <c r="P48" t="s">
@@ -12574,7 +12574,7 @@
         <v>429</v>
       </c>
       <c r="O49" t="str">
-        <f>I49</f>
+        <f t="shared" si="1"/>
         <v>P2[10]</v>
       </c>
       <c r="P49" t="s">
@@ -12611,7 +12611,7 @@
         <v>426</v>
       </c>
       <c r="O50" t="str">
-        <f>I50</f>
+        <f t="shared" si="1"/>
         <v>P0[22]</v>
       </c>
       <c r="P50" t="s">
@@ -12648,7 +12648,7 @@
         <v>427</v>
       </c>
       <c r="O51" t="str">
-        <f>I51</f>
+        <f t="shared" si="1"/>
         <v>P0[21]</v>
       </c>
       <c r="P51" t="s">
@@ -12677,11 +12677,11 @@
       <c r="I52" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="J52" s="67"/>
-      <c r="K52" s="72" t="s">
+      <c r="J52" s="64"/>
+      <c r="K52" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="L52" s="77"/>
+      <c r="L52" s="74"/>
       <c r="M52" t="s">
         <v>415</v>
       </c>
@@ -12689,7 +12689,7 @@
         <v>428</v>
       </c>
       <c r="O52" t="str">
-        <f>I52</f>
+        <f t="shared" si="1"/>
         <v>P0[20]</v>
       </c>
       <c r="P52" t="s">
@@ -12718,11 +12718,11 @@
       <c r="I53" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="J53" s="67"/>
-      <c r="K53" s="72" t="s">
+      <c r="J53" s="64"/>
+      <c r="K53" s="69" t="s">
         <v>290</v>
       </c>
-      <c r="L53" s="77"/>
+      <c r="L53" s="74"/>
       <c r="M53" t="s">
         <v>416</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>429</v>
       </c>
       <c r="O53" t="str">
-        <f>I53</f>
+        <f t="shared" si="1"/>
         <v>P0[19]</v>
       </c>
       <c r="P53" t="s">
@@ -12759,11 +12759,11 @@
       <c r="I54" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="J54" s="69" t="s">
+      <c r="J54" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="K54" s="74"/>
-      <c r="L54" s="79" t="s">
+      <c r="K54" s="71"/>
+      <c r="L54" s="76" t="s">
         <v>204</v>
       </c>
       <c r="M54" t="s">
@@ -12773,7 +12773,7 @@
         <v>426</v>
       </c>
       <c r="O54" t="str">
-        <f>I54</f>
+        <f t="shared" si="1"/>
         <v>P0[25]</v>
       </c>
       <c r="P54" t="s">
@@ -12802,13 +12802,13 @@
       <c r="I55" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="J55" s="69" t="s">
+      <c r="J55" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="K55" s="74" t="s">
+      <c r="K55" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="L55" s="79" t="s">
+      <c r="L55" s="76" t="s">
         <v>200</v>
       </c>
       <c r="M55" s="57" t="s">
@@ -12818,7 +12818,7 @@
         <v>427</v>
       </c>
       <c r="O55" t="str">
-        <f>I55</f>
+        <f t="shared" si="1"/>
         <v>P0[26]</v>
       </c>
       <c r="P55" t="s">
@@ -12861,7 +12861,7 @@
         <v>428</v>
       </c>
       <c r="O56" t="str">
-        <f>I56</f>
+        <f t="shared" si="1"/>
         <v>P0[3]</v>
       </c>
       <c r="P56" t="s">
@@ -12904,7 +12904,7 @@
         <v>429</v>
       </c>
       <c r="O57" t="str">
-        <f>I57</f>
+        <f t="shared" si="1"/>
         <v>P0[2]</v>
       </c>
       <c r="P57" t="s">
@@ -12945,7 +12945,7 @@
         <v>426</v>
       </c>
       <c r="O58" t="str">
-        <f>I58</f>
+        <f t="shared" si="1"/>
         <v>P0[18]</v>
       </c>
       <c r="P58" t="s">
@@ -12986,7 +12986,7 @@
         <v>427</v>
       </c>
       <c r="O59" t="str">
-        <f>I59</f>
+        <f t="shared" si="1"/>
         <v>P0[17]</v>
       </c>
       <c r="P59" t="s">
@@ -13029,7 +13029,7 @@
         <v>428</v>
       </c>
       <c r="O60" t="str">
-        <f>I60</f>
+        <f t="shared" si="1"/>
         <v>P0[16]</v>
       </c>
       <c r="P60" t="s">
@@ -13070,7 +13070,7 @@
         <v>429</v>
       </c>
       <c r="O61" t="str">
-        <f>I61</f>
+        <f t="shared" si="1"/>
         <v>P0[15]</v>
       </c>
       <c r="P61" t="s">
@@ -13124,11 +13124,11 @@
       <c r="I63" s="32" t="s">
         <v>367</v>
       </c>
-      <c r="J63" s="64" t="s">
+      <c r="J63" s="61" t="s">
         <v>403</v>
       </c>
-      <c r="K63" s="64"/>
-      <c r="L63" s="64"/>
+      <c r="K63" s="61"/>
+      <c r="L63" s="61"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
@@ -13150,11 +13150,11 @@
       <c r="I64" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="J64" s="64" t="s">
+      <c r="J64" s="61" t="s">
         <v>404</v>
       </c>
-      <c r="K64" s="64"/>
-      <c r="L64" s="64"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="61"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
@@ -13176,11 +13176,11 @@
       <c r="I65" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="J65" s="64" t="s">
+      <c r="J65" s="61" t="s">
         <v>401</v>
       </c>
-      <c r="K65" s="64"/>
-      <c r="L65" s="64"/>
+      <c r="K65" s="61"/>
+      <c r="L65" s="61"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
@@ -13202,11 +13202,11 @@
       <c r="I66" s="32" t="s">
         <v>376</v>
       </c>
-      <c r="J66" s="64" t="s">
+      <c r="J66" s="61" t="s">
         <v>402</v>
       </c>
-      <c r="K66" s="64"/>
-      <c r="L66" s="64"/>
+      <c r="K66" s="61"/>
+      <c r="L66" s="61"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="38" t="s">
@@ -13228,11 +13228,11 @@
       <c r="I67" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="J67" s="62" t="s">
+      <c r="J67" s="59" t="s">
         <v>400</v>
       </c>
-      <c r="K67" s="62"/>
-      <c r="L67" s="62"/>
+      <c r="K67" s="59"/>
+      <c r="L67" s="59"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="38" t="s">
@@ -13254,11 +13254,11 @@
       <c r="I68" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="J68" s="66" t="s">
+      <c r="J68" s="63" t="s">
         <v>405</v>
       </c>
-      <c r="K68" s="66"/>
-      <c r="L68" s="66"/>
+      <c r="K68" s="63"/>
+      <c r="L68" s="63"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="38" t="s">
@@ -13280,11 +13280,11 @@
       <c r="I69" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="J69" s="66" t="s">
+      <c r="J69" s="63" t="s">
         <v>406</v>
       </c>
-      <c r="K69" s="66"/>
-      <c r="L69" s="66"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="38" t="s">
@@ -13306,11 +13306,11 @@
       <c r="I70" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="J70" s="66" t="s">
+      <c r="J70" s="63" t="s">
         <v>407</v>
       </c>
-      <c r="K70" s="66"/>
-      <c r="L70" s="66"/>
+      <c r="K70" s="63"/>
+      <c r="L70" s="63"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="38" t="s">
@@ -13332,11 +13332,11 @@
       <c r="I71" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="J71" s="66" t="s">
+      <c r="J71" s="63" t="s">
         <v>408</v>
       </c>
-      <c r="K71" s="66"/>
-      <c r="L71" s="66"/>
+      <c r="K71" s="63"/>
+      <c r="L71" s="63"/>
     </row>
   </sheetData>
   <sortState ref="A2:P71">

</xml_diff>

<commit_message>
updated pinlist, MRESET and ISP0 are the same function now, this prevents interrupting any of the modules if the user pushes ISP0 button
</commit_message>
<xml_diff>
--- a/doc/LPC1769_pinmapping.xlsx
+++ b/doc/LPC1769_pinmapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="3"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LPC1769FBD100,551" sheetId="1" r:id="rId1"/>
     <sheet name="V1.0" sheetId="2" r:id="rId2"/>
     <sheet name="V1.1" sheetId="4" r:id="rId3"/>
-    <sheet name="Scrap" sheetId="5" r:id="rId4"/>
-    <sheet name="KiCAD" sheetId="3" r:id="rId5"/>
+    <sheet name="V1.2" sheetId="6" r:id="rId4"/>
+    <sheet name="Scrap" sheetId="5" r:id="rId5"/>
+    <sheet name="KiCAD" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">V1.0!$A$1:$O$101</definedName>
@@ -62,6 +63,29 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
+    <comment ref="O23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Note the reverse order of X3/X4</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
     <comment ref="M45" authorId="0">
       <text>
         <r>
@@ -80,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="476">
   <si>
     <t>Pin Name</t>
   </si>
@@ -1639,6 +1663,84 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>I2C0</t>
+  </si>
+  <si>
+    <t>J01</t>
+  </si>
+  <si>
+    <t>J08</t>
+  </si>
+  <si>
+    <t>J06</t>
+  </si>
+  <si>
+    <t>J03</t>
+  </si>
+  <si>
+    <t>J04</t>
+  </si>
+  <si>
+    <t>J05</t>
+  </si>
+  <si>
+    <t>J07</t>
+  </si>
+  <si>
+    <t>J09</t>
+  </si>
+  <si>
+    <t>J02</t>
+  </si>
+  <si>
+    <t>JNAME</t>
+  </si>
+  <si>
+    <t>XNAME</t>
+  </si>
+  <si>
+    <t>ANAME</t>
+  </si>
+  <si>
+    <t>USB DFU P</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>UART2/I2C2</t>
+  </si>
+  <si>
+    <t>I2C1</t>
+  </si>
+  <si>
+    <t>ADC/UART0</t>
+  </si>
+  <si>
+    <t>LED/GPIO</t>
+  </si>
+  <si>
+    <t>UART3</t>
+  </si>
+  <si>
+    <t>ENET0</t>
+  </si>
+  <si>
+    <t>ENET1</t>
+  </si>
+  <si>
+    <t>ENET2</t>
+  </si>
+  <si>
+    <t>ISP/MRESET</t>
+  </si>
+  <si>
+    <t>Juicy Function</t>
   </si>
 </sst>
 </file>
@@ -1939,7 +2041,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="149">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2089,8 +2191,72 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2195,15 +2361,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -2225,8 +2382,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="149">
+  <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2301,6 +2486,38 @@
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2375,6 +2592,38 @@
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7999,8 +8248,8 @@
       <c r="L2" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="59" t="s">
+      <c r="M2" s="79"/>
+      <c r="N2" s="78" t="s">
         <v>438</v>
       </c>
       <c r="O2" s="57" t="s">
@@ -8049,8 +8298,8 @@
       <c r="L3" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="M3" s="60"/>
-      <c r="N3" s="59"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="78"/>
       <c r="O3" t="s">
         <v>413</v>
       </c>
@@ -8095,8 +8344,8 @@
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="58" t="s">
+      <c r="M4" s="79"/>
+      <c r="N4" s="77" t="s">
         <v>435</v>
       </c>
       <c r="O4" t="s">
@@ -8149,8 +8398,8 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="58"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="77"/>
       <c r="O5" t="s">
         <v>414</v>
       </c>
@@ -8203,8 +8452,8 @@
         <v>207</v>
       </c>
       <c r="L6" s="16"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="58"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="77"/>
       <c r="O6" t="s">
         <v>415</v>
       </c>
@@ -8245,8 +8494,8 @@
         <v>211</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="58"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="77"/>
       <c r="O7" t="s">
         <v>416</v>
       </c>
@@ -8452,10 +8701,10 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
-      <c r="M14" s="60" t="s">
+      <c r="M14" s="79" t="s">
         <v>410</v>
       </c>
-      <c r="N14" s="58" t="s">
+      <c r="N14" s="77" t="s">
         <v>441</v>
       </c>
       <c r="O14" t="s">
@@ -8492,8 +8741,8 @@
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="58"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="77"/>
       <c r="O15" t="s">
         <v>415</v>
       </c>
@@ -8528,8 +8777,8 @@
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="58"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="77"/>
       <c r="O16" t="s">
         <v>414</v>
       </c>
@@ -8564,8 +8813,8 @@
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="58"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="77"/>
       <c r="O17" t="s">
         <v>413</v>
       </c>
@@ -8600,10 +8849,10 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="60" t="s">
+      <c r="M18" s="79" t="s">
         <v>412</v>
       </c>
-      <c r="N18" s="58" t="s">
+      <c r="N18" s="77" t="s">
         <v>433</v>
       </c>
       <c r="O18" t="s">
@@ -8642,8 +8891,8 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="58"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="77"/>
       <c r="O19" t="s">
         <v>415</v>
       </c>
@@ -8680,8 +8929,8 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="58"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="77"/>
       <c r="O20" t="s">
         <v>414</v>
       </c>
@@ -8716,8 +8965,8 @@
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="58"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="77"/>
       <c r="O21" t="s">
         <v>413</v>
       </c>
@@ -8752,10 +9001,10 @@
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
-      <c r="M22" s="60" t="s">
+      <c r="M22" s="79" t="s">
         <v>412</v>
       </c>
-      <c r="N22" s="58" t="s">
+      <c r="N22" s="77" t="s">
         <v>432</v>
       </c>
       <c r="O22" t="s">
@@ -8792,8 +9041,8 @@
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="58"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="77"/>
       <c r="O23" t="s">
         <v>415</v>
       </c>
@@ -8828,8 +9077,8 @@
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="58"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="77"/>
       <c r="O24" t="s">
         <v>414</v>
       </c>
@@ -8864,8 +9113,8 @@
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="58"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="77"/>
       <c r="O25" t="s">
         <v>413</v>
       </c>
@@ -8902,10 +9151,10 @@
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
-      <c r="M26" s="60" t="s">
+      <c r="M26" s="79" t="s">
         <v>424</v>
       </c>
-      <c r="N26" s="58" t="s">
+      <c r="N26" s="77" t="s">
         <v>431</v>
       </c>
       <c r="O26" t="s">
@@ -8944,8 +9193,8 @@
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="58"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="77"/>
       <c r="O27" t="s">
         <v>414</v>
       </c>
@@ -8986,8 +9235,8 @@
         <v>300</v>
       </c>
       <c r="L28" s="27"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="58"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="77"/>
       <c r="O28" s="56" t="s">
         <v>416</v>
       </c>
@@ -9028,8 +9277,8 @@
         <v>297</v>
       </c>
       <c r="L29" s="27"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="58"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="77"/>
       <c r="O29" s="56" t="s">
         <v>415</v>
       </c>
@@ -9064,7 +9313,7 @@
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29"/>
-      <c r="N30" s="58" t="s">
+      <c r="N30" s="77" t="s">
         <v>425</v>
       </c>
       <c r="O30" t="s">
@@ -9101,7 +9350,7 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="N31" s="58"/>
+      <c r="N31" s="77"/>
       <c r="O31" t="s">
         <v>414</v>
       </c>
@@ -9136,7 +9385,7 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="29"/>
-      <c r="N32" s="58"/>
+      <c r="N32" s="77"/>
       <c r="O32" t="s">
         <v>415</v>
       </c>
@@ -9173,7 +9422,7 @@
       </c>
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
-      <c r="N33" s="58"/>
+      <c r="N33" s="77"/>
       <c r="O33" t="s">
         <v>416</v>
       </c>
@@ -9208,7 +9457,7 @@
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
-      <c r="N34" s="58" t="s">
+      <c r="N34" s="77" t="s">
         <v>430</v>
       </c>
       <c r="O34" t="s">
@@ -9245,7 +9494,7 @@
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
-      <c r="N35" s="58"/>
+      <c r="N35" s="77"/>
       <c r="O35" t="s">
         <v>414</v>
       </c>
@@ -9284,7 +9533,7 @@
         <v>287</v>
       </c>
       <c r="L36" s="24"/>
-      <c r="N36" s="58"/>
+      <c r="N36" s="77"/>
       <c r="O36" t="s">
         <v>415</v>
       </c>
@@ -9323,7 +9572,7 @@
         <v>290</v>
       </c>
       <c r="L37" s="24"/>
-      <c r="N37" s="58"/>
+      <c r="N37" s="77"/>
       <c r="O37" t="s">
         <v>416</v>
       </c>
@@ -9362,7 +9611,7 @@
         <v>257</v>
       </c>
       <c r="L38" s="25"/>
-      <c r="N38" s="58" t="s">
+      <c r="N38" s="77" t="s">
         <v>439</v>
       </c>
       <c r="O38" t="s">
@@ -9403,7 +9652,7 @@
         <v>261</v>
       </c>
       <c r="L39" s="25"/>
-      <c r="N39" s="58"/>
+      <c r="N39" s="77"/>
       <c r="O39" t="s">
         <v>414</v>
       </c>
@@ -9442,7 +9691,7 @@
         <v>264</v>
       </c>
       <c r="L40" s="25"/>
-      <c r="N40" s="58"/>
+      <c r="N40" s="77"/>
       <c r="O40" s="56" t="s">
         <v>416</v>
       </c>
@@ -9483,7 +9732,7 @@
       <c r="L41" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="N41" s="58"/>
+      <c r="N41" s="77"/>
       <c r="O41" s="56" t="s">
         <v>415</v>
       </c>
@@ -9582,7 +9831,7 @@
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
-      <c r="N44" s="58" t="s">
+      <c r="N44" s="77" t="s">
         <v>440</v>
       </c>
       <c r="O44" t="s">
@@ -9619,7 +9868,7 @@
       <c r="J45" s="23"/>
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
-      <c r="N45" s="58"/>
+      <c r="N45" s="77"/>
       <c r="O45" t="s">
         <v>414</v>
       </c>
@@ -9656,7 +9905,7 @@
       </c>
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
-      <c r="N46" s="58"/>
+      <c r="N46" s="77"/>
       <c r="O46" t="s">
         <v>415</v>
       </c>
@@ -9693,7 +9942,7 @@
       </c>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
-      <c r="N47" s="58"/>
+      <c r="N47" s="77"/>
       <c r="O47" t="s">
         <v>416</v>
       </c>
@@ -9730,7 +9979,7 @@
       </c>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
-      <c r="N48" s="58" t="s">
+      <c r="N48" s="77" t="s">
         <v>434</v>
       </c>
       <c r="O48" t="s">
@@ -9769,7 +10018,7 @@
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
-      <c r="N49" s="58"/>
+      <c r="N49" s="77"/>
       <c r="O49" t="s">
         <v>414</v>
       </c>
@@ -9808,7 +10057,7 @@
         <v>241</v>
       </c>
       <c r="L50" s="23"/>
-      <c r="N50" s="58"/>
+      <c r="N50" s="77"/>
       <c r="O50" t="s">
         <v>415</v>
       </c>
@@ -9847,7 +10096,7 @@
         <v>245</v>
       </c>
       <c r="L51" s="23"/>
-      <c r="N51" s="58"/>
+      <c r="N51" s="77"/>
       <c r="O51" t="s">
         <v>416</v>
       </c>
@@ -9986,7 +10235,7 @@
       <c r="J56" s="24"/>
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
-      <c r="N56" s="58" t="s">
+      <c r="N56" s="77" t="s">
         <v>442</v>
       </c>
       <c r="O56" t="s">
@@ -10023,7 +10272,7 @@
       <c r="J57" s="24"/>
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
-      <c r="N57" s="58"/>
+      <c r="N57" s="77"/>
       <c r="O57" t="s">
         <v>414</v>
       </c>
@@ -10060,7 +10309,7 @@
       <c r="L58" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="N58" s="58"/>
+      <c r="N58" s="77"/>
       <c r="O58" s="56" t="s">
         <v>416</v>
       </c>
@@ -10097,7 +10346,7 @@
       <c r="L59" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="N59" s="58"/>
+      <c r="N59" s="77"/>
       <c r="O59" s="56" t="s">
         <v>415</v>
       </c>
@@ -10134,7 +10383,7 @@
       </c>
       <c r="K60" s="29"/>
       <c r="L60" s="29"/>
-      <c r="N60" s="58" t="s">
+      <c r="N60" s="77" t="s">
         <v>444</v>
       </c>
       <c r="O60" t="s">
@@ -10173,7 +10422,7 @@
       </c>
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
-      <c r="N61" s="58"/>
+      <c r="N61" s="77"/>
       <c r="O61" t="s">
         <v>414</v>
       </c>
@@ -10210,7 +10459,7 @@
       </c>
       <c r="K62" s="29"/>
       <c r="L62" s="29"/>
-      <c r="N62" s="58"/>
+      <c r="N62" s="77"/>
       <c r="O62" t="s">
         <v>415</v>
       </c>
@@ -10247,7 +10496,7 @@
       </c>
       <c r="K63" s="29"/>
       <c r="L63" s="29"/>
-      <c r="N63" s="58"/>
+      <c r="N63" s="77"/>
       <c r="O63" t="s">
         <v>416</v>
       </c>
@@ -10284,7 +10533,7 @@
       </c>
       <c r="K64" s="30"/>
       <c r="L64" s="30"/>
-      <c r="N64" s="58" t="s">
+      <c r="N64" s="77" t="s">
         <v>445</v>
       </c>
       <c r="O64" t="s">
@@ -10323,7 +10572,7 @@
       </c>
       <c r="K65" s="30"/>
       <c r="L65" s="30"/>
-      <c r="N65" s="58"/>
+      <c r="N65" s="77"/>
       <c r="O65" t="s">
         <v>414</v>
       </c>
@@ -10360,7 +10609,7 @@
       </c>
       <c r="K66" s="30"/>
       <c r="L66" s="30"/>
-      <c r="N66" s="58"/>
+      <c r="N66" s="77"/>
       <c r="O66" t="s">
         <v>415</v>
       </c>
@@ -10397,7 +10646,7 @@
       </c>
       <c r="K67" s="30"/>
       <c r="L67" s="30"/>
-      <c r="N67" s="58"/>
+      <c r="N67" s="77"/>
       <c r="O67" t="s">
         <v>416</v>
       </c>
@@ -10516,10 +10765,10 @@
         <v>219</v>
       </c>
       <c r="L70" s="13"/>
-      <c r="M70" s="60" t="s">
+      <c r="M70" s="79" t="s">
         <v>411</v>
       </c>
-      <c r="N70" s="58" t="s">
+      <c r="N70" s="77" t="s">
         <v>438</v>
       </c>
       <c r="O70" t="s">
@@ -10562,8 +10811,8 @@
         <v>215</v>
       </c>
       <c r="L71" s="13"/>
-      <c r="M71" s="60"/>
-      <c r="N71" s="58"/>
+      <c r="M71" s="79"/>
+      <c r="N71" s="77"/>
       <c r="O71" t="s">
         <v>415</v>
       </c>
@@ -10577,6 +10826,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="N60:N63"/>
+    <mergeCell ref="N64:N67"/>
+    <mergeCell ref="N38:N41"/>
+    <mergeCell ref="N48:N51"/>
+    <mergeCell ref="N56:N59"/>
+    <mergeCell ref="N44:N47"/>
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="N4:N7"/>
     <mergeCell ref="N2:N3"/>
@@ -10593,12 +10848,6 @@
     <mergeCell ref="M14:M17"/>
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N60:N63"/>
-    <mergeCell ref="N64:N67"/>
-    <mergeCell ref="N38:N41"/>
-    <mergeCell ref="N48:N51"/>
-    <mergeCell ref="N56:N59"/>
-    <mergeCell ref="N44:N47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -10608,10 +10857,2972 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="O73" sqref="O73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="36"/>
+    <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="142" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" s="82" t="s">
+        <v>475</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>461</v>
+      </c>
+      <c r="O1" s="58" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" s="58" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q1" s="58" t="s">
+        <v>446</v>
+      </c>
+      <c r="W1" t="s">
+        <v>222</v>
+      </c>
+      <c r="X1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="33">
+        <v>24</v>
+      </c>
+      <c r="C2" s="34">
+        <v>1</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="J2" s="61" t="s">
+        <v>403</v>
+      </c>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="V2" t="s">
+        <v>413</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="33">
+        <v>25</v>
+      </c>
+      <c r="C3" s="34">
+        <v>1</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>404</v>
+      </c>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="80" t="s">
+        <v>451</v>
+      </c>
+      <c r="V3" t="s">
+        <v>414</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17">
+        <v>8</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="N4" s="80" t="s">
+        <v>452</v>
+      </c>
+      <c r="O4" t="s">
+        <v>413</v>
+      </c>
+      <c r="P4" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q4" t="str">
+        <f>I4</f>
+        <v>P0[24]</v>
+      </c>
+      <c r="V4" t="s">
+        <v>415</v>
+      </c>
+      <c r="W4" t="s">
+        <v>417</v>
+      </c>
+      <c r="X4" t="s">
+        <v>419</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="17">
+        <v>9</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22">
+        <v>1</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="N5" s="80" t="s">
+        <v>452</v>
+      </c>
+      <c r="O5" t="s">
+        <v>414</v>
+      </c>
+      <c r="P5" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q5" t="str">
+        <f>I5</f>
+        <v>P0[23]</v>
+      </c>
+      <c r="V5" t="s">
+        <v>416</v>
+      </c>
+      <c r="W5" t="s">
+        <v>418</v>
+      </c>
+      <c r="X5" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="17">
+        <v>20</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="L6" s="16"/>
+      <c r="M6" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="N6" s="80" t="s">
+        <v>452</v>
+      </c>
+      <c r="O6" t="s">
+        <v>415</v>
+      </c>
+      <c r="P6" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q6" t="str">
+        <f>I6</f>
+        <v>P1[31]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="17">
+        <v>21</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="N7" s="80" t="s">
+        <v>452</v>
+      </c>
+      <c r="O7" t="s">
+        <v>416</v>
+      </c>
+      <c r="P7" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q7" t="str">
+        <f>I7</f>
+        <v>P1[30]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="17">
+        <v>70</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="J8" s="84" t="s">
+        <v>233</v>
+      </c>
+      <c r="K8" s="86"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="N8" s="80" t="s">
+        <v>460</v>
+      </c>
+      <c r="O8" t="s">
+        <v>413</v>
+      </c>
+      <c r="P8" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q8" t="str">
+        <f>I8</f>
+        <v>P2[3]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="17">
+        <v>73</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="J9" s="84" t="s">
+        <v>237</v>
+      </c>
+      <c r="K9" s="86"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="N9" s="80" t="s">
+        <v>460</v>
+      </c>
+      <c r="O9" t="s">
+        <v>414</v>
+      </c>
+      <c r="P9" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q9" t="str">
+        <f>I9</f>
+        <v>P2[2]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="17">
+        <v>74</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="L10" s="23"/>
+      <c r="M10" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="N10" s="80" t="s">
+        <v>460</v>
+      </c>
+      <c r="O10" t="s">
+        <v>415</v>
+      </c>
+      <c r="P10" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q10" t="str">
+        <f>I10</f>
+        <v>P2[1]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="17">
+        <v>75</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="L11" s="23"/>
+      <c r="M11" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="N11" s="80" t="s">
+        <v>460</v>
+      </c>
+      <c r="O11" t="s">
+        <v>416</v>
+      </c>
+      <c r="P11" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q11" t="str">
+        <f>I11</f>
+        <v>P2[0]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="17">
+        <v>39</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="J12" s="93"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N12" s="80" t="s">
+        <v>455</v>
+      </c>
+      <c r="O12" t="s">
+        <v>413</v>
+      </c>
+      <c r="P12" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q12" t="str">
+        <f>I12</f>
+        <v>P1[25]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="17">
+        <v>38</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="J13" s="93"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N13" s="80" t="s">
+        <v>455</v>
+      </c>
+      <c r="O13" t="s">
+        <v>414</v>
+      </c>
+      <c r="P13" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q13" t="str">
+        <f>I13</f>
+        <v>P1[24]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="17">
+        <v>37</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N14" s="80" t="s">
+        <v>455</v>
+      </c>
+      <c r="O14" t="s">
+        <v>415</v>
+      </c>
+      <c r="P14" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q14" t="str">
+        <f>I14</f>
+        <v>P1[23]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="17">
+        <v>36</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N15" s="80" t="s">
+        <v>455</v>
+      </c>
+      <c r="O15" t="s">
+        <v>416</v>
+      </c>
+      <c r="P15" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q15" t="str">
+        <f>I15</f>
+        <v>P1[22]</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="17">
+        <v>45</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N16" s="80" t="s">
+        <v>456</v>
+      </c>
+      <c r="O16" t="s">
+        <v>413</v>
+      </c>
+      <c r="P16" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>I16</f>
+        <v>P1[29]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="17">
+        <v>44</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N17" s="80" t="s">
+        <v>456</v>
+      </c>
+      <c r="O17" t="s">
+        <v>414</v>
+      </c>
+      <c r="P17" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q17" t="str">
+        <f>I17</f>
+        <v>P1[28]</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="B18" s="17">
+        <v>43</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N18" s="80" t="s">
+        <v>456</v>
+      </c>
+      <c r="O18" t="s">
+        <v>415</v>
+      </c>
+      <c r="P18" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q18" t="str">
+        <f>I18</f>
+        <v>P1[27]</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="17">
+        <v>40</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N19" s="80" t="s">
+        <v>456</v>
+      </c>
+      <c r="O19" t="s">
+        <v>416</v>
+      </c>
+      <c r="P19" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q19" t="str">
+        <f>I19</f>
+        <v>P1[26]</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="17">
+        <v>46</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="22">
+        <v>1</v>
+      </c>
+      <c r="G20" s="22"/>
+      <c r="H20" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="N20" s="80" t="s">
+        <v>457</v>
+      </c>
+      <c r="O20" t="s">
+        <v>413</v>
+      </c>
+      <c r="P20" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q20" t="str">
+        <f>I20</f>
+        <v>P0[0]</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="17">
+        <v>47</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="22">
+        <v>1</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="N21" s="80" t="s">
+        <v>457</v>
+      </c>
+      <c r="O21" t="s">
+        <v>414</v>
+      </c>
+      <c r="P21" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q21" t="str">
+        <f>I21</f>
+        <v>P0[1]</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="17">
+        <v>49</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="22"/>
+      <c r="H22" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="L22" s="27"/>
+      <c r="M22" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="N22" s="80" t="s">
+        <v>457</v>
+      </c>
+      <c r="O22" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="P22" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q22" t="str">
+        <f>I22</f>
+        <v>P0[11]</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="17">
+        <v>48</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="22">
+        <v>1</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="H23" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="L23" s="27"/>
+      <c r="M23" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="N23" s="80" t="s">
+        <v>457</v>
+      </c>
+      <c r="O23" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="P23" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q23" t="str">
+        <f>I23</f>
+        <v>P0[10]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="17">
+        <v>50</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N24" s="80" t="s">
+        <v>454</v>
+      </c>
+      <c r="O24" t="s">
+        <v>413</v>
+      </c>
+      <c r="P24" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q24" t="str">
+        <f>I24</f>
+        <v>P2[13]</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="17">
+        <v>51</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N25" s="80" t="s">
+        <v>454</v>
+      </c>
+      <c r="O25" t="s">
+        <v>414</v>
+      </c>
+      <c r="P25" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q25" t="str">
+        <f>I25</f>
+        <v>P2[12]</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="17">
+        <v>52</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N26" s="80" t="s">
+        <v>454</v>
+      </c>
+      <c r="O26" t="s">
+        <v>415</v>
+      </c>
+      <c r="P26" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q26" t="str">
+        <f>I26</f>
+        <v>P2[11]</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="17">
+        <v>27</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N27" s="80" t="s">
+        <v>454</v>
+      </c>
+      <c r="O27" t="s">
+        <v>416</v>
+      </c>
+      <c r="P27" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q27" t="str">
+        <f>I27</f>
+        <v>P3[25]</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="17">
+        <v>56</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="90" t="s">
+        <v>467</v>
+      </c>
+      <c r="N28" s="80" t="s">
+        <v>458</v>
+      </c>
+      <c r="O28" t="s">
+        <v>413</v>
+      </c>
+      <c r="P28" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q28" t="str">
+        <f>I28</f>
+        <v>P0[22]</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="17">
+        <v>57</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="90" t="s">
+        <v>467</v>
+      </c>
+      <c r="N29" s="80" t="s">
+        <v>458</v>
+      </c>
+      <c r="O29" t="s">
+        <v>414</v>
+      </c>
+      <c r="P29" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q29" t="str">
+        <f>I29</f>
+        <v>P0[21]</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="17">
+        <v>58</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22">
+        <v>1</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="22">
+        <v>1</v>
+      </c>
+      <c r="G30" s="22"/>
+      <c r="H30" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="L30" s="24"/>
+      <c r="M30" s="90" t="s">
+        <v>467</v>
+      </c>
+      <c r="N30" s="80" t="s">
+        <v>458</v>
+      </c>
+      <c r="O30" t="s">
+        <v>415</v>
+      </c>
+      <c r="P30" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q30" t="str">
+        <f>I30</f>
+        <v>P0[20]</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="17">
+        <v>59</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22">
+        <v>1</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="22">
+        <v>1</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="L31" s="24"/>
+      <c r="M31" s="90" t="s">
+        <v>467</v>
+      </c>
+      <c r="N31" s="80" t="s">
+        <v>458</v>
+      </c>
+      <c r="O31" t="s">
+        <v>416</v>
+      </c>
+      <c r="P31" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q31" t="str">
+        <f>I31</f>
+        <v>P0[19]</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="17">
+        <v>7</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22">
+        <v>1</v>
+      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="M32" s="96" t="s">
+        <v>468</v>
+      </c>
+      <c r="N32" s="81" t="s">
+        <v>453</v>
+      </c>
+      <c r="O32" t="s">
+        <v>413</v>
+      </c>
+      <c r="P32" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q32" t="str">
+        <f>I32</f>
+        <v>P0[25]</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="17">
+        <v>6</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22">
+        <v>1</v>
+      </c>
+      <c r="E33" s="22">
+        <v>1</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="M33" s="96" t="s">
+        <v>468</v>
+      </c>
+      <c r="N33" s="81" t="s">
+        <v>453</v>
+      </c>
+      <c r="O33" s="57" t="s">
+        <v>414</v>
+      </c>
+      <c r="P33" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q33" t="str">
+        <f>I33</f>
+        <v>P0[26]</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="17">
+        <v>99</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22">
+        <v>1</v>
+      </c>
+      <c r="E34" s="22">
+        <v>1</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="L34" s="13"/>
+      <c r="M34" s="96" t="s">
+        <v>468</v>
+      </c>
+      <c r="N34" s="80" t="s">
+        <v>453</v>
+      </c>
+      <c r="O34" t="s">
+        <v>415</v>
+      </c>
+      <c r="P34" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q34" t="str">
+        <f>I34</f>
+        <v>P0[3]</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="17">
+        <v>98</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22">
+        <v>1</v>
+      </c>
+      <c r="E35" s="22">
+        <v>1</v>
+      </c>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="L35" s="13"/>
+      <c r="M35" s="96" t="s">
+        <v>468</v>
+      </c>
+      <c r="N35" s="80" t="s">
+        <v>453</v>
+      </c>
+      <c r="O35" t="s">
+        <v>416</v>
+      </c>
+      <c r="P35" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q35" t="str">
+        <f>I35</f>
+        <v>P0[2]</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="17">
+        <v>60</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22">
+        <v>1</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22">
+        <v>1</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="L36" s="25"/>
+      <c r="M36" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="N36" s="80" t="s">
+        <v>459</v>
+      </c>
+      <c r="O36" t="s">
+        <v>413</v>
+      </c>
+      <c r="P36" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q36" t="str">
+        <f>I36</f>
+        <v>P0[18]</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="17">
+        <v>61</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22">
+        <v>1</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22">
+        <v>1</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="L37" s="25"/>
+      <c r="M37" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="N37" s="80" t="s">
+        <v>459</v>
+      </c>
+      <c r="O37" t="s">
+        <v>414</v>
+      </c>
+      <c r="P37" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q37" t="str">
+        <f>I37</f>
+        <v>P0[17]</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="17">
+        <v>63</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22">
+        <v>1</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="L38" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="M38" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="N38" s="80" t="s">
+        <v>459</v>
+      </c>
+      <c r="O38" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="P38" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q38" t="str">
+        <f>I38</f>
+        <v>P0[16]</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="17">
+        <v>62</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22">
+        <v>1</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22">
+        <v>1</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="L39" s="25"/>
+      <c r="M39" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="N39" s="80" t="s">
+        <v>459</v>
+      </c>
+      <c r="O39" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="P39" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q39" t="str">
+        <f>I39</f>
+        <v>P0[15]</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="17">
+        <v>66</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22">
+        <v>1</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N40" s="80" t="s">
+        <v>440</v>
+      </c>
+      <c r="O40" t="s">
+        <v>413</v>
+      </c>
+      <c r="P40" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q40" t="str">
+        <f>I40</f>
+        <v>P2[7]</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="17">
+        <v>67</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N41" s="80" t="s">
+        <v>440</v>
+      </c>
+      <c r="O41" t="s">
+        <v>414</v>
+      </c>
+      <c r="P41" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q41" t="str">
+        <f>I41</f>
+        <v>P2[6]</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="17">
+        <v>68</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22">
+        <v>1</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="J42" s="62" t="s">
+        <v>276</v>
+      </c>
+      <c r="K42" s="68"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N42" s="80" t="s">
+        <v>440</v>
+      </c>
+      <c r="O42" t="s">
+        <v>415</v>
+      </c>
+      <c r="P42" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q42" t="str">
+        <f>I42</f>
+        <v>P2[5]</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="17">
+        <v>69</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22">
+        <v>1</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="96" t="s">
+        <v>303</v>
+      </c>
+      <c r="N43" s="80" t="s">
+        <v>440</v>
+      </c>
+      <c r="O43" t="s">
+        <v>416</v>
+      </c>
+      <c r="P43" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q43" t="str">
+        <f>I43</f>
+        <v>P2[4]</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="17">
+        <v>35</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I44" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
+      <c r="L44" s="30"/>
+      <c r="M44" s="96" t="s">
+        <v>469</v>
+      </c>
+      <c r="N44" s="80" t="s">
+        <v>441</v>
+      </c>
+      <c r="O44" t="s">
+        <v>413</v>
+      </c>
+      <c r="P44" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q44" t="str">
+        <f>I44</f>
+        <v>P1[21]</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="17">
+        <v>34</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22">
+        <v>1</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="96" t="s">
+        <v>469</v>
+      </c>
+      <c r="N45" s="80" t="s">
+        <v>441</v>
+      </c>
+      <c r="O45" t="s">
+        <v>414</v>
+      </c>
+      <c r="P45" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q45" t="str">
+        <f>I45</f>
+        <v>P1[20]</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B46" s="17">
+        <v>33</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22">
+        <v>1</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I46" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="96" t="s">
+        <v>469</v>
+      </c>
+      <c r="N46" s="80" t="s">
+        <v>441</v>
+      </c>
+      <c r="O46" t="s">
+        <v>415</v>
+      </c>
+      <c r="P46" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q46" t="str">
+        <f>I46</f>
+        <v>P1[19]</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="17">
+        <v>32</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22">
+        <v>1</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="96" t="s">
+        <v>469</v>
+      </c>
+      <c r="N47" s="80" t="s">
+        <v>441</v>
+      </c>
+      <c r="O47" t="s">
+        <v>416</v>
+      </c>
+      <c r="P47" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q47" t="str">
+        <f>I47</f>
+        <v>P1[18]</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="17">
+        <v>80</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22">
+        <v>1</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="96" t="s">
+        <v>470</v>
+      </c>
+      <c r="N48" s="80" t="s">
+        <v>442</v>
+      </c>
+      <c r="O48" t="s">
+        <v>413</v>
+      </c>
+      <c r="P48" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q48" t="str">
+        <f>I48</f>
+        <v>P0[5]</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="17">
+        <v>81</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22">
+        <v>1</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="96" t="s">
+        <v>470</v>
+      </c>
+      <c r="N49" s="80" t="s">
+        <v>442</v>
+      </c>
+      <c r="O49" t="s">
+        <v>414</v>
+      </c>
+      <c r="P49" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q49" t="str">
+        <f>I49</f>
+        <v>P0[4]</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="17">
+        <v>85</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22">
+        <v>1</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="M50" s="96" t="s">
+        <v>470</v>
+      </c>
+      <c r="N50" s="80" t="s">
+        <v>442</v>
+      </c>
+      <c r="O50" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="P50" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q50" t="str">
+        <f>I50</f>
+        <v>P4[29]</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="17">
+        <v>82</v>
+      </c>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22">
+        <v>1</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="M51" s="96" t="s">
+        <v>470</v>
+      </c>
+      <c r="N51" s="80" t="s">
+        <v>442</v>
+      </c>
+      <c r="O51" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="P51" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q51" t="str">
+        <f>I51</f>
+        <v>P4[28]</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="17">
+        <v>65</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22">
+        <v>1</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" s="84"/>
+      <c r="K52" s="86"/>
+      <c r="L52" s="88"/>
+      <c r="M52" s="96" t="s">
+        <v>471</v>
+      </c>
+      <c r="N52" t="s">
+        <v>443</v>
+      </c>
+      <c r="O52" t="s">
+        <v>413</v>
+      </c>
+      <c r="P52" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q52" t="str">
+        <f>I52</f>
+        <v>P2[8]</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="17">
+        <v>26</v>
+      </c>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22">
+        <v>1</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="J53" s="65"/>
+      <c r="K53" s="70"/>
+      <c r="L53" s="75"/>
+      <c r="M53" s="96" t="s">
+        <v>471</v>
+      </c>
+      <c r="N53" t="s">
+        <v>443</v>
+      </c>
+      <c r="O53" t="s">
+        <v>414</v>
+      </c>
+      <c r="P53" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q53" t="str">
+        <f>I53</f>
+        <v>P3[26]</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="17">
+        <v>95</v>
+      </c>
+      <c r="C54" s="22">
+        <v>1</v>
+      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="J54" s="85" t="s">
+        <v>383</v>
+      </c>
+      <c r="K54" s="87"/>
+      <c r="L54" s="89"/>
+      <c r="M54" s="96" t="s">
+        <v>471</v>
+      </c>
+      <c r="N54" t="s">
+        <v>443</v>
+      </c>
+      <c r="O54" t="s">
+        <v>415</v>
+      </c>
+      <c r="P54" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q54" t="str">
+        <f>I54</f>
+        <v>P1[0]</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="17">
+        <v>94</v>
+      </c>
+      <c r="C55" s="22">
+        <v>1</v>
+      </c>
+      <c r="D55" s="22"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="J55" s="85" t="s">
+        <v>381</v>
+      </c>
+      <c r="K55" s="87"/>
+      <c r="L55" s="89"/>
+      <c r="M55" s="96" t="s">
+        <v>471</v>
+      </c>
+      <c r="N55" t="s">
+        <v>443</v>
+      </c>
+      <c r="O55" t="s">
+        <v>416</v>
+      </c>
+      <c r="P55" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q55" t="str">
+        <f>I55</f>
+        <v>P1[1]</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="17">
+        <v>86</v>
+      </c>
+      <c r="C56" s="22">
+        <v>1</v>
+      </c>
+      <c r="D56" s="22"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="J56" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="K56" s="29"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="96" t="s">
+        <v>472</v>
+      </c>
+      <c r="N56" s="80" t="s">
+        <v>444</v>
+      </c>
+      <c r="O56" t="s">
+        <v>413</v>
+      </c>
+      <c r="P56" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q56" t="str">
+        <f>I56</f>
+        <v>P1[17]</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" s="17">
+        <v>87</v>
+      </c>
+      <c r="C57" s="22">
+        <v>1</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="J57" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="K57" s="29"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="96" t="s">
+        <v>472</v>
+      </c>
+      <c r="N57" s="80" t="s">
+        <v>444</v>
+      </c>
+      <c r="O57" t="s">
+        <v>414</v>
+      </c>
+      <c r="P57" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q57" t="str">
+        <f>I57</f>
+        <v>P1[16]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" s="17">
+        <v>88</v>
+      </c>
+      <c r="C58" s="22">
+        <v>1</v>
+      </c>
+      <c r="D58" s="22"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="J58" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="K58" s="29"/>
+      <c r="L58" s="29"/>
+      <c r="M58" s="96" t="s">
+        <v>472</v>
+      </c>
+      <c r="N58" s="80" t="s">
+        <v>444</v>
+      </c>
+      <c r="O58" t="s">
+        <v>415</v>
+      </c>
+      <c r="P58" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q58" t="str">
+        <f>I58</f>
+        <v>P1[15]</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="17">
+        <v>89</v>
+      </c>
+      <c r="C59" s="22">
+        <v>1</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="J59" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="K59" s="29"/>
+      <c r="L59" s="29"/>
+      <c r="M59" s="96" t="s">
+        <v>472</v>
+      </c>
+      <c r="N59" s="80" t="s">
+        <v>444</v>
+      </c>
+      <c r="O59" t="s">
+        <v>416</v>
+      </c>
+      <c r="P59" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q59" t="str">
+        <f>I59</f>
+        <v>P1[14]</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" s="17">
+        <v>90</v>
+      </c>
+      <c r="C60" s="22">
+        <v>1</v>
+      </c>
+      <c r="D60" s="22"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="J60" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="K60" s="30"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="96" t="s">
+        <v>473</v>
+      </c>
+      <c r="N60" s="80" t="s">
+        <v>445</v>
+      </c>
+      <c r="O60" t="s">
+        <v>413</v>
+      </c>
+      <c r="P60" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q60" t="str">
+        <f>I60</f>
+        <v>P1[10]</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" s="17">
+        <v>91</v>
+      </c>
+      <c r="C61" s="22">
+        <v>1</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="J61" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="K61" s="30"/>
+      <c r="L61" s="30"/>
+      <c r="M61" s="96" t="s">
+        <v>473</v>
+      </c>
+      <c r="N61" s="80" t="s">
+        <v>445</v>
+      </c>
+      <c r="O61" t="s">
+        <v>414</v>
+      </c>
+      <c r="P61" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q61" t="str">
+        <f>I61</f>
+        <v>P1[9]</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="17">
+        <v>92</v>
+      </c>
+      <c r="C62" s="22">
+        <v>1</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="J62" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="K62" s="30"/>
+      <c r="L62" s="30"/>
+      <c r="M62" s="96" t="s">
+        <v>473</v>
+      </c>
+      <c r="N62" s="80" t="s">
+        <v>445</v>
+      </c>
+      <c r="O62" t="s">
+        <v>415</v>
+      </c>
+      <c r="P62" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q62" t="str">
+        <f>I62</f>
+        <v>P1[8]</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" s="17">
+        <v>93</v>
+      </c>
+      <c r="C63" s="22">
+        <v>1</v>
+      </c>
+      <c r="D63" s="22"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="J63" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="K63" s="30"/>
+      <c r="L63" s="30"/>
+      <c r="M63" s="96" t="s">
+        <v>473</v>
+      </c>
+      <c r="N63" s="80" t="s">
+        <v>445</v>
+      </c>
+      <c r="O63" t="s">
+        <v>416</v>
+      </c>
+      <c r="P63" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q63" t="str">
+        <f>I63</f>
+        <v>P1[4]</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="52">
+        <v>53</v>
+      </c>
+      <c r="C64" s="53"/>
+      <c r="D64" s="53">
+        <v>1</v>
+      </c>
+      <c r="E64" s="51"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="I64" s="51" t="s">
+        <v>309</v>
+      </c>
+      <c r="J64" s="55" t="s">
+        <v>409</v>
+      </c>
+      <c r="K64" s="55"/>
+      <c r="L64" s="55"/>
+      <c r="M64" s="96" t="s">
+        <v>474</v>
+      </c>
+      <c r="N64" s="80" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="39">
+        <v>76</v>
+      </c>
+      <c r="C65" s="40">
+        <v>1</v>
+      </c>
+      <c r="D65" s="40"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I65" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J65" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="K65" s="63"/>
+      <c r="L65" s="63"/>
+      <c r="N65" s="80" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="39">
+        <v>77</v>
+      </c>
+      <c r="C66" s="40">
+        <v>1</v>
+      </c>
+      <c r="D66" s="40"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I66" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="J66" s="63" t="s">
+        <v>406</v>
+      </c>
+      <c r="K66" s="63"/>
+      <c r="L66" s="63"/>
+      <c r="N66" s="80" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="39">
+        <v>78</v>
+      </c>
+      <c r="C67" s="40">
+        <v>1</v>
+      </c>
+      <c r="D67" s="40"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I67" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="J67" s="63" t="s">
+        <v>407</v>
+      </c>
+      <c r="K67" s="63"/>
+      <c r="L67" s="63"/>
+      <c r="N67" s="80" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="39">
+        <v>79</v>
+      </c>
+      <c r="C68" s="40">
+        <v>1</v>
+      </c>
+      <c r="D68" s="40"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="40"/>
+      <c r="H68" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I68" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="J68" s="63" t="s">
+        <v>408</v>
+      </c>
+      <c r="K68" s="63"/>
+      <c r="L68" s="63"/>
+      <c r="N68" s="80" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="33">
+        <v>29</v>
+      </c>
+      <c r="C69" s="34">
+        <v>1</v>
+      </c>
+      <c r="D69" s="34"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I69" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="J69" s="61" t="s">
+        <v>401</v>
+      </c>
+      <c r="K69" s="61"/>
+      <c r="L69" s="61"/>
+      <c r="M69" s="91"/>
+      <c r="N69" s="80" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="33">
+        <v>30</v>
+      </c>
+      <c r="C70" s="34">
+        <v>1</v>
+      </c>
+      <c r="D70" s="34"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
+      <c r="H70" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I70" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="J70" s="61" t="s">
+        <v>402</v>
+      </c>
+      <c r="K70" s="61"/>
+      <c r="L70" s="61"/>
+      <c r="M70" s="90"/>
+      <c r="N70" s="80" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="39">
+        <v>64</v>
+      </c>
+      <c r="C71" s="40">
+        <v>1</v>
+      </c>
+      <c r="D71" s="40"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="40"/>
+      <c r="H71" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I71" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="J71" s="59" t="s">
+        <v>400</v>
+      </c>
+      <c r="K71" s="59"/>
+      <c r="L71" s="59"/>
+      <c r="M71" s="92"/>
+      <c r="N71" s="80" t="s">
+        <v>464</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:Q71">
+    <sortCondition ref="N2:N71"/>
+    <sortCondition ref="O2:O71"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26:O29"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10628,7 +13839,7 @@
     <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="142" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="141" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -10665,7 +13876,7 @@
       <c r="L1" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="58" t="s">
         <v>448</v>
       </c>
       <c r="N1" t="s">
@@ -10674,7 +13885,7 @@
       <c r="O1" t="s">
         <v>446</v>
       </c>
-      <c r="P1" s="61" t="s">
+      <c r="P1" s="58" t="s">
         <v>449</v>
       </c>
       <c r="U1" t="s">
@@ -10721,7 +13932,7 @@
         <v>426</v>
       </c>
       <c r="O2" t="str">
-        <f>I2</f>
+        <f t="shared" ref="O2:O33" si="0">I2</f>
         <v>P0[24]</v>
       </c>
       <c r="P2" t="s">
@@ -10768,7 +13979,7 @@
         <v>427</v>
       </c>
       <c r="O3" t="str">
-        <f>I3</f>
+        <f t="shared" si="0"/>
         <v>P0[23]</v>
       </c>
       <c r="P3" t="s">
@@ -10817,7 +14028,7 @@
         <v>428</v>
       </c>
       <c r="O4" t="str">
-        <f>I4</f>
+        <f t="shared" si="0"/>
         <v>P1[31]</v>
       </c>
       <c r="P4" t="s">
@@ -10872,7 +14083,7 @@
         <v>429</v>
       </c>
       <c r="O5" t="str">
-        <f>I5</f>
+        <f t="shared" si="0"/>
         <v>P1[30]</v>
       </c>
       <c r="P5" t="s">
@@ -10921,7 +14132,7 @@
         <v>426</v>
       </c>
       <c r="O6" t="str">
-        <f>I6</f>
+        <f t="shared" si="0"/>
         <v>P2[7]</v>
       </c>
       <c r="P6" t="s">
@@ -10958,7 +14169,7 @@
         <v>427</v>
       </c>
       <c r="O7" t="str">
-        <f>I7</f>
+        <f t="shared" si="0"/>
         <v>P2[6]</v>
       </c>
       <c r="P7" t="s">
@@ -10985,11 +14196,11 @@
       <c r="I8" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="K8" s="71"/>
-      <c r="L8" s="76"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="73"/>
       <c r="M8" t="s">
         <v>415</v>
       </c>
@@ -10997,7 +14208,7 @@
         <v>428</v>
       </c>
       <c r="O8" t="str">
-        <f>I8</f>
+        <f t="shared" si="0"/>
         <v>P2[5]</v>
       </c>
       <c r="P8" t="s">
@@ -11024,11 +14235,11 @@
       <c r="I9" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="J9" s="65" t="s">
+      <c r="J9" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="K9" s="71"/>
-      <c r="L9" s="76"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="73"/>
       <c r="M9" t="s">
         <v>416</v>
       </c>
@@ -11036,7 +14247,7 @@
         <v>429</v>
       </c>
       <c r="O9" t="str">
-        <f>I9</f>
+        <f t="shared" si="0"/>
         <v>P2[4]</v>
       </c>
       <c r="P9" t="s">
@@ -11073,7 +14284,7 @@
         <v>426</v>
       </c>
       <c r="O10" t="str">
-        <f>I10</f>
+        <f t="shared" si="0"/>
         <v>P1[21]</v>
       </c>
       <c r="P10" t="s">
@@ -11110,7 +14321,7 @@
         <v>427</v>
       </c>
       <c r="O11" t="str">
-        <f>I11</f>
+        <f t="shared" si="0"/>
         <v>P1[20]</v>
       </c>
       <c r="P11" t="s">
@@ -11137,9 +14348,9 @@
       <c r="I12" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="J12" s="68"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="78"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="75"/>
       <c r="M12" t="s">
         <v>415</v>
       </c>
@@ -11147,7 +14358,7 @@
         <v>428</v>
       </c>
       <c r="O12" t="str">
-        <f>I12</f>
+        <f t="shared" si="0"/>
         <v>P1[19]</v>
       </c>
       <c r="P12" t="s">
@@ -11174,9 +14385,9 @@
       <c r="I13" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="76"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="73"/>
       <c r="M13" t="s">
         <v>416</v>
       </c>
@@ -11184,7 +14395,7 @@
         <v>429</v>
       </c>
       <c r="O13" t="str">
-        <f>I13</f>
+        <f t="shared" si="0"/>
         <v>P1[18]</v>
       </c>
       <c r="P13" t="s">
@@ -11221,7 +14432,7 @@
         <v>426</v>
       </c>
       <c r="O14" t="str">
-        <f>I14</f>
+        <f t="shared" si="0"/>
         <v>P0[5]</v>
       </c>
       <c r="P14" t="s">
@@ -11258,7 +14469,7 @@
         <v>427</v>
       </c>
       <c r="O15" t="str">
-        <f>I15</f>
+        <f t="shared" si="0"/>
         <v>P0[4]</v>
       </c>
       <c r="P15" t="s">
@@ -11297,7 +14508,7 @@
         <v>428</v>
       </c>
       <c r="O16" t="str">
-        <f>I16</f>
+        <f t="shared" si="0"/>
         <v>P4[29]</v>
       </c>
       <c r="P16" t="s">
@@ -11336,7 +14547,7 @@
         <v>429</v>
       </c>
       <c r="O17" t="str">
-        <f>I17</f>
+        <f t="shared" si="0"/>
         <v>P4[28]</v>
       </c>
       <c r="P17" t="s">
@@ -11373,7 +14584,7 @@
         <v>426</v>
       </c>
       <c r="O18" t="str">
-        <f>I18</f>
+        <f t="shared" si="0"/>
         <v>P2[8]</v>
       </c>
       <c r="P18" t="s">
@@ -11410,7 +14621,7 @@
         <v>427</v>
       </c>
       <c r="O19" t="str">
-        <f>I19</f>
+        <f t="shared" si="0"/>
         <v>P3[26]</v>
       </c>
       <c r="P19" t="s">
@@ -11449,7 +14660,7 @@
         <v>428</v>
       </c>
       <c r="O20" t="str">
-        <f>I20</f>
+        <f t="shared" si="0"/>
         <v>P1[0]</v>
       </c>
       <c r="P20" t="s">
@@ -11488,7 +14699,7 @@
         <v>429</v>
       </c>
       <c r="O21" t="str">
-        <f>I21</f>
+        <f t="shared" si="0"/>
         <v>P1[1]</v>
       </c>
       <c r="P21" t="s">
@@ -11527,7 +14738,7 @@
         <v>426</v>
       </c>
       <c r="O22" t="str">
-        <f>I22</f>
+        <f t="shared" si="0"/>
         <v>P1[17]</v>
       </c>
       <c r="P22" t="s">
@@ -11566,7 +14777,7 @@
         <v>427</v>
       </c>
       <c r="O23" t="str">
-        <f>I23</f>
+        <f t="shared" si="0"/>
         <v>P1[16]</v>
       </c>
       <c r="P23" t="s">
@@ -11605,7 +14816,7 @@
         <v>428</v>
       </c>
       <c r="O24" t="str">
-        <f>I24</f>
+        <f t="shared" si="0"/>
         <v>P1[15]</v>
       </c>
       <c r="P24" t="s">
@@ -11644,7 +14855,7 @@
         <v>429</v>
       </c>
       <c r="O25" t="str">
-        <f>I25</f>
+        <f t="shared" si="0"/>
         <v>P1[14]</v>
       </c>
       <c r="P25" t="s">
@@ -11683,7 +14894,7 @@
         <v>426</v>
       </c>
       <c r="O26" t="str">
-        <f>I26</f>
+        <f t="shared" si="0"/>
         <v>P1[10]</v>
       </c>
       <c r="P26" t="s">
@@ -11722,7 +14933,7 @@
         <v>427</v>
       </c>
       <c r="O27" t="str">
-        <f>I27</f>
+        <f t="shared" si="0"/>
         <v>P1[9]</v>
       </c>
       <c r="P27" t="s">
@@ -11761,7 +14972,7 @@
         <v>428</v>
       </c>
       <c r="O28" t="str">
-        <f>I28</f>
+        <f t="shared" si="0"/>
         <v>P1[8]</v>
       </c>
       <c r="P28" t="s">
@@ -11800,7 +15011,7 @@
         <v>429</v>
       </c>
       <c r="O29" t="str">
-        <f>I29</f>
+        <f t="shared" si="0"/>
         <v>P1[4]</v>
       </c>
       <c r="P29" t="s">
@@ -11839,7 +15050,7 @@
         <v>426</v>
       </c>
       <c r="O30" t="str">
-        <f>I30</f>
+        <f t="shared" si="0"/>
         <v>P2[3]</v>
       </c>
       <c r="P30" t="s">
@@ -11878,7 +15089,7 @@
         <v>427</v>
       </c>
       <c r="O31" t="str">
-        <f>I31</f>
+        <f t="shared" si="0"/>
         <v>P2[2]</v>
       </c>
       <c r="P31" t="s">
@@ -11919,7 +15130,7 @@
         <v>428</v>
       </c>
       <c r="O32" t="str">
-        <f>I32</f>
+        <f t="shared" si="0"/>
         <v>P2[1]</v>
       </c>
       <c r="P32" t="s">
@@ -11960,7 +15171,7 @@
         <v>429</v>
       </c>
       <c r="O33" t="str">
-        <f>I33</f>
+        <f t="shared" si="0"/>
         <v>P2[0]</v>
       </c>
       <c r="P33" t="s">
@@ -11997,7 +15208,7 @@
         <v>426</v>
       </c>
       <c r="O34" t="str">
-        <f>I34</f>
+        <f t="shared" ref="O34:O61" si="1">I34</f>
         <v>P1[25]</v>
       </c>
       <c r="P34" t="s">
@@ -12036,7 +15247,7 @@
         <v>427</v>
       </c>
       <c r="O35" t="str">
-        <f>I35</f>
+        <f t="shared" si="1"/>
         <v>P1[24]</v>
       </c>
       <c r="P35" t="s">
@@ -12075,7 +15286,7 @@
         <v>428</v>
       </c>
       <c r="O36" t="str">
-        <f>I36</f>
+        <f t="shared" si="1"/>
         <v>P1[23]</v>
       </c>
       <c r="P36" t="s">
@@ -12112,7 +15323,7 @@
         <v>429</v>
       </c>
       <c r="O37" t="str">
-        <f>I37</f>
+        <f t="shared" si="1"/>
         <v>P1[22]</v>
       </c>
       <c r="P37" t="s">
@@ -12149,7 +15360,7 @@
         <v>426</v>
       </c>
       <c r="O38" t="str">
-        <f>I38</f>
+        <f t="shared" si="1"/>
         <v>P1[29]</v>
       </c>
       <c r="P38" t="s">
@@ -12186,7 +15397,7 @@
         <v>427</v>
       </c>
       <c r="O39" t="str">
-        <f>I39</f>
+        <f t="shared" si="1"/>
         <v>P1[28]</v>
       </c>
       <c r="P39" t="s">
@@ -12223,7 +15434,7 @@
         <v>428</v>
       </c>
       <c r="O40" t="str">
-        <f>I40</f>
+        <f t="shared" si="1"/>
         <v>P1[27]</v>
       </c>
       <c r="P40" t="s">
@@ -12260,7 +15471,7 @@
         <v>429</v>
       </c>
       <c r="O41" t="str">
-        <f>I41</f>
+        <f t="shared" si="1"/>
         <v>P1[26]</v>
       </c>
       <c r="P41" t="s">
@@ -12289,9 +15500,9 @@
       <c r="I42" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="J42" s="63"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="75"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="72"/>
       <c r="M42" t="s">
         <v>413</v>
       </c>
@@ -12299,7 +15510,7 @@
         <v>426</v>
       </c>
       <c r="O42" t="str">
-        <f>I42</f>
+        <f t="shared" si="1"/>
         <v>P0[0]</v>
       </c>
       <c r="P42" t="s">
@@ -12338,7 +15549,7 @@
         <v>427</v>
       </c>
       <c r="O43" t="str">
-        <f>I43</f>
+        <f t="shared" si="1"/>
         <v>P0[1]</v>
       </c>
       <c r="P43" t="s">
@@ -12381,7 +15592,7 @@
         <v>428</v>
       </c>
       <c r="O44" t="str">
-        <f>I44</f>
+        <f t="shared" si="1"/>
         <v>P0[11]</v>
       </c>
       <c r="P44" t="s">
@@ -12424,7 +15635,7 @@
         <v>429</v>
       </c>
       <c r="O45" t="str">
-        <f>I45</f>
+        <f t="shared" si="1"/>
         <v>P0[10]</v>
       </c>
       <c r="P45" t="s">
@@ -12461,7 +15672,7 @@
         <v>426</v>
       </c>
       <c r="O46" t="str">
-        <f>I46</f>
+        <f t="shared" si="1"/>
         <v>P2[13]</v>
       </c>
       <c r="P46" t="s">
@@ -12498,7 +15709,7 @@
         <v>427</v>
       </c>
       <c r="O47" t="str">
-        <f>I47</f>
+        <f t="shared" si="1"/>
         <v>P2[12]</v>
       </c>
       <c r="P47" t="s">
@@ -12535,7 +15746,7 @@
         <v>428</v>
       </c>
       <c r="O48" t="str">
-        <f>I48</f>
+        <f t="shared" si="1"/>
         <v>P2[11]</v>
       </c>
       <c r="P48" t="s">
@@ -12574,7 +15785,7 @@
         <v>429</v>
       </c>
       <c r="O49" t="str">
-        <f>I49</f>
+        <f t="shared" si="1"/>
         <v>P2[10]</v>
       </c>
       <c r="P49" t="s">
@@ -12611,7 +15822,7 @@
         <v>426</v>
       </c>
       <c r="O50" t="str">
-        <f>I50</f>
+        <f t="shared" si="1"/>
         <v>P0[22]</v>
       </c>
       <c r="P50" t="s">
@@ -12648,7 +15859,7 @@
         <v>427</v>
       </c>
       <c r="O51" t="str">
-        <f>I51</f>
+        <f t="shared" si="1"/>
         <v>P0[21]</v>
       </c>
       <c r="P51" t="s">
@@ -12677,11 +15888,11 @@
       <c r="I52" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="J52" s="67"/>
-      <c r="K52" s="72" t="s">
+      <c r="J52" s="64"/>
+      <c r="K52" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="L52" s="77"/>
+      <c r="L52" s="74"/>
       <c r="M52" t="s">
         <v>415</v>
       </c>
@@ -12689,7 +15900,7 @@
         <v>428</v>
       </c>
       <c r="O52" t="str">
-        <f>I52</f>
+        <f t="shared" si="1"/>
         <v>P0[20]</v>
       </c>
       <c r="P52" t="s">
@@ -12718,11 +15929,11 @@
       <c r="I53" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="J53" s="67"/>
-      <c r="K53" s="72" t="s">
+      <c r="J53" s="64"/>
+      <c r="K53" s="69" t="s">
         <v>290</v>
       </c>
-      <c r="L53" s="77"/>
+      <c r="L53" s="74"/>
       <c r="M53" t="s">
         <v>416</v>
       </c>
@@ -12730,7 +15941,7 @@
         <v>429</v>
       </c>
       <c r="O53" t="str">
-        <f>I53</f>
+        <f t="shared" si="1"/>
         <v>P0[19]</v>
       </c>
       <c r="P53" t="s">
@@ -12759,11 +15970,11 @@
       <c r="I54" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="J54" s="69" t="s">
+      <c r="J54" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="K54" s="74"/>
-      <c r="L54" s="79" t="s">
+      <c r="K54" s="71"/>
+      <c r="L54" s="76" t="s">
         <v>204</v>
       </c>
       <c r="M54" t="s">
@@ -12773,7 +15984,7 @@
         <v>426</v>
       </c>
       <c r="O54" t="str">
-        <f>I54</f>
+        <f t="shared" si="1"/>
         <v>P0[25]</v>
       </c>
       <c r="P54" t="s">
@@ -12802,13 +16013,13 @@
       <c r="I55" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="J55" s="69" t="s">
+      <c r="J55" s="66" t="s">
         <v>198</v>
       </c>
-      <c r="K55" s="74" t="s">
+      <c r="K55" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="L55" s="79" t="s">
+      <c r="L55" s="76" t="s">
         <v>200</v>
       </c>
       <c r="M55" s="57" t="s">
@@ -12818,7 +16029,7 @@
         <v>427</v>
       </c>
       <c r="O55" t="str">
-        <f>I55</f>
+        <f t="shared" si="1"/>
         <v>P0[26]</v>
       </c>
       <c r="P55" t="s">
@@ -12861,7 +16072,7 @@
         <v>428</v>
       </c>
       <c r="O56" t="str">
-        <f>I56</f>
+        <f t="shared" si="1"/>
         <v>P0[3]</v>
       </c>
       <c r="P56" t="s">
@@ -12904,7 +16115,7 @@
         <v>429</v>
       </c>
       <c r="O57" t="str">
-        <f>I57</f>
+        <f t="shared" si="1"/>
         <v>P0[2]</v>
       </c>
       <c r="P57" t="s">
@@ -12945,7 +16156,7 @@
         <v>426</v>
       </c>
       <c r="O58" t="str">
-        <f>I58</f>
+        <f t="shared" si="1"/>
         <v>P0[18]</v>
       </c>
       <c r="P58" t="s">
@@ -12986,7 +16197,7 @@
         <v>427</v>
       </c>
       <c r="O59" t="str">
-        <f>I59</f>
+        <f t="shared" si="1"/>
         <v>P0[17]</v>
       </c>
       <c r="P59" t="s">
@@ -13029,7 +16240,7 @@
         <v>428</v>
       </c>
       <c r="O60" t="str">
-        <f>I60</f>
+        <f t="shared" si="1"/>
         <v>P0[16]</v>
       </c>
       <c r="P60" t="s">
@@ -13070,7 +16281,7 @@
         <v>429</v>
       </c>
       <c r="O61" t="str">
-        <f>I61</f>
+        <f t="shared" si="1"/>
         <v>P0[15]</v>
       </c>
       <c r="P61" t="s">
@@ -13124,11 +16335,11 @@
       <c r="I63" s="32" t="s">
         <v>367</v>
       </c>
-      <c r="J63" s="64" t="s">
+      <c r="J63" s="61" t="s">
         <v>403</v>
       </c>
-      <c r="K63" s="64"/>
-      <c r="L63" s="64"/>
+      <c r="K63" s="61"/>
+      <c r="L63" s="61"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
@@ -13150,11 +16361,11 @@
       <c r="I64" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="J64" s="64" t="s">
+      <c r="J64" s="61" t="s">
         <v>404</v>
       </c>
-      <c r="K64" s="64"/>
-      <c r="L64" s="64"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="61"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
@@ -13176,11 +16387,11 @@
       <c r="I65" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="J65" s="64" t="s">
+      <c r="J65" s="61" t="s">
         <v>401</v>
       </c>
-      <c r="K65" s="64"/>
-      <c r="L65" s="64"/>
+      <c r="K65" s="61"/>
+      <c r="L65" s="61"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
@@ -13202,11 +16413,11 @@
       <c r="I66" s="32" t="s">
         <v>376</v>
       </c>
-      <c r="J66" s="64" t="s">
+      <c r="J66" s="61" t="s">
         <v>402</v>
       </c>
-      <c r="K66" s="64"/>
-      <c r="L66" s="64"/>
+      <c r="K66" s="61"/>
+      <c r="L66" s="61"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="38" t="s">
@@ -13228,11 +16439,11 @@
       <c r="I67" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="J67" s="62" t="s">
+      <c r="J67" s="59" t="s">
         <v>400</v>
       </c>
-      <c r="K67" s="62"/>
-      <c r="L67" s="62"/>
+      <c r="K67" s="59"/>
+      <c r="L67" s="59"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="38" t="s">
@@ -13254,11 +16465,11 @@
       <c r="I68" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="J68" s="66" t="s">
+      <c r="J68" s="63" t="s">
         <v>405</v>
       </c>
-      <c r="K68" s="66"/>
-      <c r="L68" s="66"/>
+      <c r="K68" s="63"/>
+      <c r="L68" s="63"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="38" t="s">
@@ -13280,11 +16491,11 @@
       <c r="I69" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="J69" s="66" t="s">
+      <c r="J69" s="63" t="s">
         <v>406</v>
       </c>
-      <c r="K69" s="66"/>
-      <c r="L69" s="66"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="38" t="s">
@@ -13306,11 +16517,11 @@
       <c r="I70" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="J70" s="66" t="s">
+      <c r="J70" s="63" t="s">
         <v>407</v>
       </c>
-      <c r="K70" s="66"/>
-      <c r="L70" s="66"/>
+      <c r="K70" s="63"/>
+      <c r="L70" s="63"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="38" t="s">
@@ -13332,11 +16543,11 @@
       <c r="I71" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="J71" s="66" t="s">
+      <c r="J71" s="63" t="s">
         <v>408</v>
       </c>
-      <c r="K71" s="66"/>
-      <c r="L71" s="66"/>
+      <c r="K71" s="63"/>
+      <c r="L71" s="63"/>
     </row>
   </sheetData>
   <sortState ref="A2:P71">
@@ -13349,7 +16560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>

</xml_diff>

<commit_message>
added sheet for documentation
</commit_message>
<xml_diff>
--- a/doc/LPC1769_pinmapping.xlsx
+++ b/doc/LPC1769_pinmapping.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherifeid/plugge_git/R1000A/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherifeid/plugge_git/R1000AX/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="994" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LPC1769FBD100,551" sheetId="1" r:id="rId1"/>
     <sheet name="V1.0" sheetId="2" r:id="rId2"/>
     <sheet name="V1.1" sheetId="4" r:id="rId3"/>
     <sheet name="V1.2" sheetId="6" r:id="rId4"/>
-    <sheet name="Scrap" sheetId="5" r:id="rId5"/>
-    <sheet name="KiCAD" sheetId="3" r:id="rId6"/>
+    <sheet name="V1.2 Display" sheetId="7" r:id="rId5"/>
+    <sheet name="Scrap" sheetId="5" r:id="rId6"/>
+    <sheet name="KiCAD" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">V1.0!$A$1:$O$101</definedName>
@@ -86,6 +87,29 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
+    <comment ref="I23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Note the reverse order of X3/X4</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
     <comment ref="M45" authorId="0">
       <text>
         <r>
@@ -104,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="479">
   <si>
     <t>Pin Name</t>
   </si>
@@ -1741,6 +1765,15 @@
   </si>
   <si>
     <t>Juicy Function</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>Socket Number</t>
+  </si>
+  <si>
+    <t>Pin Order in Socket</t>
   </si>
 </sst>
 </file>
@@ -2041,7 +2074,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="213">
+  <cellStyleXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2255,8 +2288,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2382,15 +2423,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2410,8 +2442,23 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="213">
+  <cellStyles count="221">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2518,6 +2565,10 @@
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2624,6 +2675,10 @@
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4822,7 +4877,7 @@
     <col min="15" max="15" width="11" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="141" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="142" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -8170,7 +8225,7 @@
     <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="141" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="142" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -8248,8 +8303,8 @@
       <c r="L2" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="78" t="s">
+      <c r="M2" s="96"/>
+      <c r="N2" s="95" t="s">
         <v>438</v>
       </c>
       <c r="O2" s="57" t="s">
@@ -8298,8 +8353,8 @@
       <c r="L3" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="M3" s="79"/>
-      <c r="N3" s="78"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="95"/>
       <c r="O3" t="s">
         <v>413</v>
       </c>
@@ -8344,8 +8399,8 @@
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="77" t="s">
+      <c r="M4" s="96"/>
+      <c r="N4" s="94" t="s">
         <v>435</v>
       </c>
       <c r="O4" t="s">
@@ -8398,8 +8453,8 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="77"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="94"/>
       <c r="O5" t="s">
         <v>414</v>
       </c>
@@ -8452,8 +8507,8 @@
         <v>207</v>
       </c>
       <c r="L6" s="16"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="77"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="94"/>
       <c r="O6" t="s">
         <v>415</v>
       </c>
@@ -8494,8 +8549,8 @@
         <v>211</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="77"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="94"/>
       <c r="O7" t="s">
         <v>416</v>
       </c>
@@ -8701,10 +8756,10 @@
       <c r="J14" s="26"/>
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
-      <c r="M14" s="79" t="s">
+      <c r="M14" s="96" t="s">
         <v>410</v>
       </c>
-      <c r="N14" s="77" t="s">
+      <c r="N14" s="94" t="s">
         <v>441</v>
       </c>
       <c r="O14" t="s">
@@ -8741,8 +8796,8 @@
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="77"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="94"/>
       <c r="O15" t="s">
         <v>415</v>
       </c>
@@ -8777,8 +8832,8 @@
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="77"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="94"/>
       <c r="O16" t="s">
         <v>414</v>
       </c>
@@ -8813,8 +8868,8 @@
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="77"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="94"/>
       <c r="O17" t="s">
         <v>413</v>
       </c>
@@ -8849,10 +8904,10 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
-      <c r="M18" s="79" t="s">
+      <c r="M18" s="96" t="s">
         <v>412</v>
       </c>
-      <c r="N18" s="77" t="s">
+      <c r="N18" s="94" t="s">
         <v>433</v>
       </c>
       <c r="O18" t="s">
@@ -8891,8 +8946,8 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="77"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="94"/>
       <c r="O19" t="s">
         <v>415</v>
       </c>
@@ -8929,8 +8984,8 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="77"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="94"/>
       <c r="O20" t="s">
         <v>414</v>
       </c>
@@ -8965,8 +9020,8 @@
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="77"/>
+      <c r="M21" s="96"/>
+      <c r="N21" s="94"/>
       <c r="O21" t="s">
         <v>413</v>
       </c>
@@ -9001,10 +9056,10 @@
       <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
-      <c r="M22" s="79" t="s">
+      <c r="M22" s="96" t="s">
         <v>412</v>
       </c>
-      <c r="N22" s="77" t="s">
+      <c r="N22" s="94" t="s">
         <v>432</v>
       </c>
       <c r="O22" t="s">
@@ -9041,8 +9096,8 @@
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="77"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="94"/>
       <c r="O23" t="s">
         <v>415</v>
       </c>
@@ -9077,8 +9132,8 @@
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="77"/>
+      <c r="M24" s="96"/>
+      <c r="N24" s="94"/>
       <c r="O24" t="s">
         <v>414</v>
       </c>
@@ -9113,8 +9168,8 @@
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="77"/>
+      <c r="M25" s="96"/>
+      <c r="N25" s="94"/>
       <c r="O25" t="s">
         <v>413</v>
       </c>
@@ -9151,10 +9206,10 @@
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
       <c r="L26" s="27"/>
-      <c r="M26" s="79" t="s">
+      <c r="M26" s="96" t="s">
         <v>424</v>
       </c>
-      <c r="N26" s="77" t="s">
+      <c r="N26" s="94" t="s">
         <v>431</v>
       </c>
       <c r="O26" t="s">
@@ -9193,8 +9248,8 @@
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="77"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="94"/>
       <c r="O27" t="s">
         <v>414</v>
       </c>
@@ -9235,8 +9290,8 @@
         <v>300</v>
       </c>
       <c r="L28" s="27"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="77"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="94"/>
       <c r="O28" s="56" t="s">
         <v>416</v>
       </c>
@@ -9277,8 +9332,8 @@
         <v>297</v>
       </c>
       <c r="L29" s="27"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="77"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="94"/>
       <c r="O29" s="56" t="s">
         <v>415</v>
       </c>
@@ -9313,7 +9368,7 @@
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29"/>
-      <c r="N30" s="77" t="s">
+      <c r="N30" s="94" t="s">
         <v>425</v>
       </c>
       <c r="O30" t="s">
@@ -9350,7 +9405,7 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="N31" s="77"/>
+      <c r="N31" s="94"/>
       <c r="O31" t="s">
         <v>414</v>
       </c>
@@ -9385,7 +9440,7 @@
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="29"/>
-      <c r="N32" s="77"/>
+      <c r="N32" s="94"/>
       <c r="O32" t="s">
         <v>415</v>
       </c>
@@ -9422,7 +9477,7 @@
       </c>
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
-      <c r="N33" s="77"/>
+      <c r="N33" s="94"/>
       <c r="O33" t="s">
         <v>416</v>
       </c>
@@ -9457,7 +9512,7 @@
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
-      <c r="N34" s="77" t="s">
+      <c r="N34" s="94" t="s">
         <v>430</v>
       </c>
       <c r="O34" t="s">
@@ -9494,7 +9549,7 @@
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
-      <c r="N35" s="77"/>
+      <c r="N35" s="94"/>
       <c r="O35" t="s">
         <v>414</v>
       </c>
@@ -9533,7 +9588,7 @@
         <v>287</v>
       </c>
       <c r="L36" s="24"/>
-      <c r="N36" s="77"/>
+      <c r="N36" s="94"/>
       <c r="O36" t="s">
         <v>415</v>
       </c>
@@ -9572,7 +9627,7 @@
         <v>290</v>
       </c>
       <c r="L37" s="24"/>
-      <c r="N37" s="77"/>
+      <c r="N37" s="94"/>
       <c r="O37" t="s">
         <v>416</v>
       </c>
@@ -9611,7 +9666,7 @@
         <v>257</v>
       </c>
       <c r="L38" s="25"/>
-      <c r="N38" s="77" t="s">
+      <c r="N38" s="94" t="s">
         <v>439</v>
       </c>
       <c r="O38" t="s">
@@ -9652,7 +9707,7 @@
         <v>261</v>
       </c>
       <c r="L39" s="25"/>
-      <c r="N39" s="77"/>
+      <c r="N39" s="94"/>
       <c r="O39" t="s">
         <v>414</v>
       </c>
@@ -9691,7 +9746,7 @@
         <v>264</v>
       </c>
       <c r="L40" s="25"/>
-      <c r="N40" s="77"/>
+      <c r="N40" s="94"/>
       <c r="O40" s="56" t="s">
         <v>416</v>
       </c>
@@ -9732,7 +9787,7 @@
       <c r="L41" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="N41" s="77"/>
+      <c r="N41" s="94"/>
       <c r="O41" s="56" t="s">
         <v>415</v>
       </c>
@@ -9831,7 +9886,7 @@
       <c r="J44" s="23"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
-      <c r="N44" s="77" t="s">
+      <c r="N44" s="94" t="s">
         <v>440</v>
       </c>
       <c r="O44" t="s">
@@ -9868,7 +9923,7 @@
       <c r="J45" s="23"/>
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
-      <c r="N45" s="77"/>
+      <c r="N45" s="94"/>
       <c r="O45" t="s">
         <v>414</v>
       </c>
@@ -9905,7 +9960,7 @@
       </c>
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
-      <c r="N46" s="77"/>
+      <c r="N46" s="94"/>
       <c r="O46" t="s">
         <v>415</v>
       </c>
@@ -9942,7 +9997,7 @@
       </c>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
-      <c r="N47" s="77"/>
+      <c r="N47" s="94"/>
       <c r="O47" t="s">
         <v>416</v>
       </c>
@@ -9979,7 +10034,7 @@
       </c>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
-      <c r="N48" s="77" t="s">
+      <c r="N48" s="94" t="s">
         <v>434</v>
       </c>
       <c r="O48" t="s">
@@ -10018,7 +10073,7 @@
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
-      <c r="N49" s="77"/>
+      <c r="N49" s="94"/>
       <c r="O49" t="s">
         <v>414</v>
       </c>
@@ -10057,7 +10112,7 @@
         <v>241</v>
       </c>
       <c r="L50" s="23"/>
-      <c r="N50" s="77"/>
+      <c r="N50" s="94"/>
       <c r="O50" t="s">
         <v>415</v>
       </c>
@@ -10096,7 +10151,7 @@
         <v>245</v>
       </c>
       <c r="L51" s="23"/>
-      <c r="N51" s="77"/>
+      <c r="N51" s="94"/>
       <c r="O51" t="s">
         <v>416</v>
       </c>
@@ -10235,7 +10290,7 @@
       <c r="J56" s="24"/>
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
-      <c r="N56" s="77" t="s">
+      <c r="N56" s="94" t="s">
         <v>442</v>
       </c>
       <c r="O56" t="s">
@@ -10272,7 +10327,7 @@
       <c r="J57" s="24"/>
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
-      <c r="N57" s="77"/>
+      <c r="N57" s="94"/>
       <c r="O57" t="s">
         <v>414</v>
       </c>
@@ -10309,7 +10364,7 @@
       <c r="L58" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="N58" s="77"/>
+      <c r="N58" s="94"/>
       <c r="O58" s="56" t="s">
         <v>416</v>
       </c>
@@ -10346,7 +10401,7 @@
       <c r="L59" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="N59" s="77"/>
+      <c r="N59" s="94"/>
       <c r="O59" s="56" t="s">
         <v>415</v>
       </c>
@@ -10383,7 +10438,7 @@
       </c>
       <c r="K60" s="29"/>
       <c r="L60" s="29"/>
-      <c r="N60" s="77" t="s">
+      <c r="N60" s="94" t="s">
         <v>444</v>
       </c>
       <c r="O60" t="s">
@@ -10422,7 +10477,7 @@
       </c>
       <c r="K61" s="29"/>
       <c r="L61" s="29"/>
-      <c r="N61" s="77"/>
+      <c r="N61" s="94"/>
       <c r="O61" t="s">
         <v>414</v>
       </c>
@@ -10459,7 +10514,7 @@
       </c>
       <c r="K62" s="29"/>
       <c r="L62" s="29"/>
-      <c r="N62" s="77"/>
+      <c r="N62" s="94"/>
       <c r="O62" t="s">
         <v>415</v>
       </c>
@@ -10496,7 +10551,7 @@
       </c>
       <c r="K63" s="29"/>
       <c r="L63" s="29"/>
-      <c r="N63" s="77"/>
+      <c r="N63" s="94"/>
       <c r="O63" t="s">
         <v>416</v>
       </c>
@@ -10533,7 +10588,7 @@
       </c>
       <c r="K64" s="30"/>
       <c r="L64" s="30"/>
-      <c r="N64" s="77" t="s">
+      <c r="N64" s="94" t="s">
         <v>445</v>
       </c>
       <c r="O64" t="s">
@@ -10572,7 +10627,7 @@
       </c>
       <c r="K65" s="30"/>
       <c r="L65" s="30"/>
-      <c r="N65" s="77"/>
+      <c r="N65" s="94"/>
       <c r="O65" t="s">
         <v>414</v>
       </c>
@@ -10609,7 +10664,7 @@
       </c>
       <c r="K66" s="30"/>
       <c r="L66" s="30"/>
-      <c r="N66" s="77"/>
+      <c r="N66" s="94"/>
       <c r="O66" t="s">
         <v>415</v>
       </c>
@@ -10646,7 +10701,7 @@
       </c>
       <c r="K67" s="30"/>
       <c r="L67" s="30"/>
-      <c r="N67" s="77"/>
+      <c r="N67" s="94"/>
       <c r="O67" t="s">
         <v>416</v>
       </c>
@@ -10765,10 +10820,10 @@
         <v>219</v>
       </c>
       <c r="L70" s="13"/>
-      <c r="M70" s="79" t="s">
+      <c r="M70" s="96" t="s">
         <v>411</v>
       </c>
-      <c r="N70" s="77" t="s">
+      <c r="N70" s="94" t="s">
         <v>438</v>
       </c>
       <c r="O70" t="s">
@@ -10811,8 +10866,8 @@
         <v>215</v>
       </c>
       <c r="L71" s="13"/>
-      <c r="M71" s="79"/>
-      <c r="N71" s="77"/>
+      <c r="M71" s="96"/>
+      <c r="N71" s="94"/>
       <c r="O71" t="s">
         <v>415</v>
       </c>
@@ -10826,12 +10881,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="N60:N63"/>
-    <mergeCell ref="N64:N67"/>
-    <mergeCell ref="N38:N41"/>
-    <mergeCell ref="N48:N51"/>
-    <mergeCell ref="N56:N59"/>
-    <mergeCell ref="N44:N47"/>
     <mergeCell ref="N14:N17"/>
     <mergeCell ref="N4:N7"/>
     <mergeCell ref="N2:N3"/>
@@ -10848,6 +10897,12 @@
     <mergeCell ref="M14:M17"/>
     <mergeCell ref="M2:M5"/>
     <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N60:N63"/>
+    <mergeCell ref="N64:N67"/>
+    <mergeCell ref="N38:N41"/>
+    <mergeCell ref="N48:N51"/>
+    <mergeCell ref="N56:N59"/>
+    <mergeCell ref="N44:N47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -10859,8 +10914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="O73" sqref="O73"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10876,6 +10931,7 @@
     <col min="11" max="11" width="8.83203125" style="36"/>
     <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="142" x14ac:dyDescent="0.2">
@@ -10915,7 +10971,7 @@
       <c r="L1" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="82" t="s">
+      <c r="M1" s="79" t="s">
         <v>475</v>
       </c>
       <c r="N1" s="58" t="s">
@@ -10965,8 +11021,8 @@
       </c>
       <c r="K2" s="61"/>
       <c r="L2" s="61"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="80" t="s">
+      <c r="M2" s="87"/>
+      <c r="N2" s="77" t="s">
         <v>451</v>
       </c>
       <c r="V2" t="s">
@@ -11001,8 +11057,8 @@
       </c>
       <c r="K3" s="61"/>
       <c r="L3" s="61"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="80" t="s">
+      <c r="M3" s="87"/>
+      <c r="N3" s="77" t="s">
         <v>451</v>
       </c>
       <c r="V3" t="s">
@@ -11039,10 +11095,10 @@
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
-      <c r="M4" s="83" t="s">
+      <c r="M4" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N4" s="80" t="s">
+      <c r="N4" s="77" t="s">
         <v>452</v>
       </c>
       <c r="O4" t="s">
@@ -11052,7 +11108,7 @@
         <v>426</v>
       </c>
       <c r="Q4" t="str">
-        <f>I4</f>
+        <f t="shared" ref="Q4:Q35" si="0">I4</f>
         <v>P0[24]</v>
       </c>
       <c r="V4" t="s">
@@ -11095,10 +11151,10 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="83" t="s">
+      <c r="M5" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N5" s="80" t="s">
+      <c r="N5" s="77" t="s">
         <v>452</v>
       </c>
       <c r="O5" t="s">
@@ -11108,7 +11164,7 @@
         <v>427</v>
       </c>
       <c r="Q5" t="str">
-        <f>I5</f>
+        <f t="shared" si="0"/>
         <v>P0[23]</v>
       </c>
       <c r="V5" t="s">
@@ -11153,10 +11209,10 @@
         <v>207</v>
       </c>
       <c r="L6" s="16"/>
-      <c r="M6" s="83" t="s">
+      <c r="M6" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N6" s="80" t="s">
+      <c r="N6" s="77" t="s">
         <v>452</v>
       </c>
       <c r="O6" t="s">
@@ -11166,7 +11222,7 @@
         <v>428</v>
       </c>
       <c r="Q6" t="str">
-        <f>I6</f>
+        <f t="shared" si="0"/>
         <v>P1[31]</v>
       </c>
     </row>
@@ -11199,10 +11255,10 @@
         <v>211</v>
       </c>
       <c r="L7" s="16"/>
-      <c r="M7" s="83" t="s">
+      <c r="M7" s="80" t="s">
         <v>465</v>
       </c>
-      <c r="N7" s="80" t="s">
+      <c r="N7" s="77" t="s">
         <v>452</v>
       </c>
       <c r="O7" t="s">
@@ -11212,7 +11268,7 @@
         <v>429</v>
       </c>
       <c r="Q7" t="str">
-        <f>I7</f>
+        <f t="shared" si="0"/>
         <v>P1[30]</v>
       </c>
     </row>
@@ -11236,15 +11292,15 @@
       <c r="I8" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="81" t="s">
         <v>233</v>
       </c>
-      <c r="K8" s="86"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="96" t="s">
+      <c r="K8" s="83"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="N8" s="80" t="s">
+      <c r="N8" s="77" t="s">
         <v>460</v>
       </c>
       <c r="O8" t="s">
@@ -11254,7 +11310,7 @@
         <v>426</v>
       </c>
       <c r="Q8" t="str">
-        <f>I8</f>
+        <f t="shared" si="0"/>
         <v>P2[3]</v>
       </c>
     </row>
@@ -11278,15 +11334,15 @@
       <c r="I9" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="J9" s="84" t="s">
+      <c r="J9" s="81" t="s">
         <v>237</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="96" t="s">
+      <c r="K9" s="83"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="N9" s="80" t="s">
+      <c r="N9" s="77" t="s">
         <v>460</v>
       </c>
       <c r="O9" t="s">
@@ -11296,7 +11352,7 @@
         <v>427</v>
       </c>
       <c r="Q9" t="str">
-        <f>I9</f>
+        <f t="shared" si="0"/>
         <v>P2[2]</v>
       </c>
     </row>
@@ -11327,10 +11383,10 @@
         <v>241</v>
       </c>
       <c r="L10" s="23"/>
-      <c r="M10" s="96" t="s">
+      <c r="M10" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="N10" s="80" t="s">
+      <c r="N10" s="77" t="s">
         <v>460</v>
       </c>
       <c r="O10" t="s">
@@ -11340,7 +11396,7 @@
         <v>428</v>
       </c>
       <c r="Q10" t="str">
-        <f>I10</f>
+        <f t="shared" si="0"/>
         <v>P2[1]</v>
       </c>
     </row>
@@ -11371,10 +11427,10 @@
         <v>245</v>
       </c>
       <c r="L11" s="23"/>
-      <c r="M11" s="96" t="s">
+      <c r="M11" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="N11" s="80" t="s">
+      <c r="N11" s="77" t="s">
         <v>460</v>
       </c>
       <c r="O11" t="s">
@@ -11384,7 +11440,7 @@
         <v>429</v>
       </c>
       <c r="Q11" t="str">
-        <f>I11</f>
+        <f t="shared" si="0"/>
         <v>P2[0]</v>
       </c>
     </row>
@@ -11408,13 +11464,13 @@
       <c r="I12" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="J12" s="93"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="95"/>
-      <c r="M12" s="96" t="s">
+      <c r="J12" s="90"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N12" s="80" t="s">
+      <c r="N12" s="77" t="s">
         <v>455</v>
       </c>
       <c r="O12" t="s">
@@ -11424,7 +11480,7 @@
         <v>426</v>
       </c>
       <c r="Q12" t="str">
-        <f>I12</f>
+        <f t="shared" si="0"/>
         <v>P1[25]</v>
       </c>
     </row>
@@ -11450,13 +11506,13 @@
       <c r="I13" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="J13" s="93"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="95"/>
-      <c r="M13" s="96" t="s">
+      <c r="J13" s="90"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N13" s="80" t="s">
+      <c r="N13" s="77" t="s">
         <v>455</v>
       </c>
       <c r="O13" t="s">
@@ -11466,7 +11522,7 @@
         <v>427</v>
       </c>
       <c r="Q13" t="str">
-        <f>I13</f>
+        <f t="shared" si="0"/>
         <v>P1[24]</v>
       </c>
     </row>
@@ -11495,10 +11551,10 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="96" t="s">
+      <c r="M14" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N14" s="80" t="s">
+      <c r="N14" s="77" t="s">
         <v>455</v>
       </c>
       <c r="O14" t="s">
@@ -11508,7 +11564,7 @@
         <v>428</v>
       </c>
       <c r="Q14" t="str">
-        <f>I14</f>
+        <f t="shared" si="0"/>
         <v>P1[23]</v>
       </c>
     </row>
@@ -11535,10 +11591,10 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
-      <c r="M15" s="96" t="s">
+      <c r="M15" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N15" s="80" t="s">
+      <c r="N15" s="77" t="s">
         <v>455</v>
       </c>
       <c r="O15" t="s">
@@ -11548,7 +11604,7 @@
         <v>429</v>
       </c>
       <c r="Q15" t="str">
-        <f>I15</f>
+        <f t="shared" si="0"/>
         <v>P1[22]</v>
       </c>
     </row>
@@ -11575,10 +11631,10 @@
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N16" s="80" t="s">
+      <c r="N16" s="77" t="s">
         <v>456</v>
       </c>
       <c r="O16" t="s">
@@ -11588,7 +11644,7 @@
         <v>426</v>
       </c>
       <c r="Q16" t="str">
-        <f>I16</f>
+        <f t="shared" si="0"/>
         <v>P1[29]</v>
       </c>
     </row>
@@ -11615,10 +11671,10 @@
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
-      <c r="M17" s="96" t="s">
+      <c r="M17" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N17" s="80" t="s">
+      <c r="N17" s="77" t="s">
         <v>456</v>
       </c>
       <c r="O17" t="s">
@@ -11628,7 +11684,7 @@
         <v>427</v>
       </c>
       <c r="Q17" t="str">
-        <f>I17</f>
+        <f t="shared" si="0"/>
         <v>P1[28]</v>
       </c>
     </row>
@@ -11655,10 +11711,10 @@
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
-      <c r="M18" s="96" t="s">
+      <c r="M18" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N18" s="80" t="s">
+      <c r="N18" s="77" t="s">
         <v>456</v>
       </c>
       <c r="O18" t="s">
@@ -11668,7 +11724,7 @@
         <v>428</v>
       </c>
       <c r="Q18" t="str">
-        <f>I18</f>
+        <f t="shared" si="0"/>
         <v>P1[27]</v>
       </c>
     </row>
@@ -11695,10 +11751,10 @@
       <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
-      <c r="M19" s="96" t="s">
+      <c r="M19" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N19" s="80" t="s">
+      <c r="N19" s="77" t="s">
         <v>456</v>
       </c>
       <c r="O19" t="s">
@@ -11708,7 +11764,7 @@
         <v>429</v>
       </c>
       <c r="Q19" t="str">
-        <f>I19</f>
+        <f t="shared" si="0"/>
         <v>P1[26]</v>
       </c>
     </row>
@@ -11737,10 +11793,10 @@
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
-      <c r="M20" s="83" t="s">
+      <c r="M20" s="80" t="s">
         <v>466</v>
       </c>
-      <c r="N20" s="80" t="s">
+      <c r="N20" s="77" t="s">
         <v>457</v>
       </c>
       <c r="O20" t="s">
@@ -11750,7 +11806,7 @@
         <v>426</v>
       </c>
       <c r="Q20" t="str">
-        <f>I20</f>
+        <f t="shared" si="0"/>
         <v>P0[0]</v>
       </c>
     </row>
@@ -11779,10 +11835,10 @@
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
-      <c r="M21" s="83" t="s">
+      <c r="M21" s="80" t="s">
         <v>466</v>
       </c>
-      <c r="N21" s="80" t="s">
+      <c r="N21" s="77" t="s">
         <v>457</v>
       </c>
       <c r="O21" t="s">
@@ -11792,7 +11848,7 @@
         <v>427</v>
       </c>
       <c r="Q21" t="str">
-        <f>I21</f>
+        <f t="shared" si="0"/>
         <v>P0[1]</v>
       </c>
     </row>
@@ -11825,10 +11881,10 @@
         <v>297</v>
       </c>
       <c r="L22" s="27"/>
-      <c r="M22" s="83" t="s">
+      <c r="M22" s="80" t="s">
         <v>466</v>
       </c>
-      <c r="N22" s="80" t="s">
+      <c r="N22" s="77" t="s">
         <v>457</v>
       </c>
       <c r="O22" s="56" t="s">
@@ -11838,7 +11894,7 @@
         <v>428</v>
       </c>
       <c r="Q22" t="str">
-        <f>I22</f>
+        <f t="shared" si="0"/>
         <v>P0[11]</v>
       </c>
     </row>
@@ -11871,10 +11927,10 @@
         <v>300</v>
       </c>
       <c r="L23" s="27"/>
-      <c r="M23" s="83" t="s">
+      <c r="M23" s="80" t="s">
         <v>466</v>
       </c>
-      <c r="N23" s="80" t="s">
+      <c r="N23" s="77" t="s">
         <v>457</v>
       </c>
       <c r="O23" s="56" t="s">
@@ -11884,7 +11940,7 @@
         <v>429</v>
       </c>
       <c r="Q23" t="str">
-        <f>I23</f>
+        <f t="shared" si="0"/>
         <v>P0[10]</v>
       </c>
     </row>
@@ -11911,10 +11967,10 @@
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
       <c r="L24" s="29"/>
-      <c r="M24" s="96" t="s">
+      <c r="M24" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N24" s="80" t="s">
+      <c r="N24" s="77" t="s">
         <v>454</v>
       </c>
       <c r="O24" t="s">
@@ -11924,7 +11980,7 @@
         <v>426</v>
       </c>
       <c r="Q24" t="str">
-        <f>I24</f>
+        <f t="shared" si="0"/>
         <v>P2[13]</v>
       </c>
     </row>
@@ -11951,10 +12007,10 @@
       <c r="J25" s="29"/>
       <c r="K25" s="29"/>
       <c r="L25" s="29"/>
-      <c r="M25" s="96" t="s">
+      <c r="M25" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N25" s="80" t="s">
+      <c r="N25" s="77" t="s">
         <v>454</v>
       </c>
       <c r="O25" t="s">
@@ -11964,7 +12020,7 @@
         <v>427</v>
       </c>
       <c r="Q25" t="str">
-        <f>I25</f>
+        <f t="shared" si="0"/>
         <v>P2[12]</v>
       </c>
     </row>
@@ -11991,10 +12047,10 @@
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
       <c r="L26" s="29"/>
-      <c r="M26" s="96" t="s">
+      <c r="M26" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N26" s="80" t="s">
+      <c r="N26" s="77" t="s">
         <v>454</v>
       </c>
       <c r="O26" t="s">
@@ -12004,7 +12060,7 @@
         <v>428</v>
       </c>
       <c r="Q26" t="str">
-        <f>I26</f>
+        <f t="shared" si="0"/>
         <v>P2[11]</v>
       </c>
     </row>
@@ -12031,10 +12087,10 @@
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
-      <c r="M27" s="96" t="s">
+      <c r="M27" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N27" s="80" t="s">
+      <c r="N27" s="77" t="s">
         <v>454</v>
       </c>
       <c r="O27" t="s">
@@ -12044,7 +12100,7 @@
         <v>429</v>
       </c>
       <c r="Q27" t="str">
-        <f>I27</f>
+        <f t="shared" si="0"/>
         <v>P3[25]</v>
       </c>
     </row>
@@ -12071,10 +12127,10 @@
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
-      <c r="M28" s="90" t="s">
+      <c r="M28" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="N28" s="80" t="s">
+      <c r="N28" s="77" t="s">
         <v>458</v>
       </c>
       <c r="O28" t="s">
@@ -12084,7 +12140,7 @@
         <v>426</v>
       </c>
       <c r="Q28" t="str">
-        <f>I28</f>
+        <f t="shared" si="0"/>
         <v>P0[22]</v>
       </c>
     </row>
@@ -12111,10 +12167,10 @@
       <c r="J29" s="24"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
-      <c r="M29" s="90" t="s">
+      <c r="M29" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="N29" s="80" t="s">
+      <c r="N29" s="77" t="s">
         <v>458</v>
       </c>
       <c r="O29" t="s">
@@ -12124,7 +12180,7 @@
         <v>427</v>
       </c>
       <c r="Q29" t="str">
-        <f>I29</f>
+        <f t="shared" si="0"/>
         <v>P0[21]</v>
       </c>
     </row>
@@ -12155,10 +12211,10 @@
         <v>287</v>
       </c>
       <c r="L30" s="24"/>
-      <c r="M30" s="90" t="s">
+      <c r="M30" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="N30" s="80" t="s">
+      <c r="N30" s="77" t="s">
         <v>458</v>
       </c>
       <c r="O30" t="s">
@@ -12168,7 +12224,7 @@
         <v>428</v>
       </c>
       <c r="Q30" t="str">
-        <f>I30</f>
+        <f t="shared" si="0"/>
         <v>P0[20]</v>
       </c>
     </row>
@@ -12199,10 +12255,10 @@
         <v>290</v>
       </c>
       <c r="L31" s="24"/>
-      <c r="M31" s="90" t="s">
+      <c r="M31" s="87" t="s">
         <v>467</v>
       </c>
-      <c r="N31" s="80" t="s">
+      <c r="N31" s="77" t="s">
         <v>458</v>
       </c>
       <c r="O31" t="s">
@@ -12212,7 +12268,7 @@
         <v>429</v>
       </c>
       <c r="Q31" t="str">
-        <f>I31</f>
+        <f t="shared" si="0"/>
         <v>P0[19]</v>
       </c>
     </row>
@@ -12245,10 +12301,10 @@
       <c r="L32" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="M32" s="96" t="s">
+      <c r="M32" s="93" t="s">
         <v>468</v>
       </c>
-      <c r="N32" s="81" t="s">
+      <c r="N32" s="78" t="s">
         <v>453</v>
       </c>
       <c r="O32" t="s">
@@ -12258,7 +12314,7 @@
         <v>426</v>
       </c>
       <c r="Q32" t="str">
-        <f>I32</f>
+        <f t="shared" si="0"/>
         <v>P0[25]</v>
       </c>
     </row>
@@ -12293,10 +12349,10 @@
       <c r="L33" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="M33" s="96" t="s">
+      <c r="M33" s="93" t="s">
         <v>468</v>
       </c>
-      <c r="N33" s="81" t="s">
+      <c r="N33" s="78" t="s">
         <v>453</v>
       </c>
       <c r="O33" s="57" t="s">
@@ -12306,7 +12362,7 @@
         <v>427</v>
       </c>
       <c r="Q33" t="str">
-        <f>I33</f>
+        <f t="shared" si="0"/>
         <v>P0[26]</v>
       </c>
     </row>
@@ -12339,10 +12395,10 @@
         <v>215</v>
       </c>
       <c r="L34" s="13"/>
-      <c r="M34" s="96" t="s">
+      <c r="M34" s="93" t="s">
         <v>468</v>
       </c>
-      <c r="N34" s="80" t="s">
+      <c r="N34" s="77" t="s">
         <v>453</v>
       </c>
       <c r="O34" t="s">
@@ -12352,7 +12408,7 @@
         <v>428</v>
       </c>
       <c r="Q34" t="str">
-        <f>I34</f>
+        <f t="shared" si="0"/>
         <v>P0[3]</v>
       </c>
     </row>
@@ -12385,10 +12441,10 @@
         <v>219</v>
       </c>
       <c r="L35" s="13"/>
-      <c r="M35" s="96" t="s">
+      <c r="M35" s="93" t="s">
         <v>468</v>
       </c>
-      <c r="N35" s="80" t="s">
+      <c r="N35" s="77" t="s">
         <v>453</v>
       </c>
       <c r="O35" t="s">
@@ -12398,7 +12454,7 @@
         <v>429</v>
       </c>
       <c r="Q35" t="str">
-        <f>I35</f>
+        <f t="shared" si="0"/>
         <v>P0[2]</v>
       </c>
     </row>
@@ -12429,10 +12485,10 @@
         <v>257</v>
       </c>
       <c r="L36" s="25"/>
-      <c r="M36" s="96" t="s">
+      <c r="M36" s="93" t="s">
         <v>258</v>
       </c>
-      <c r="N36" s="80" t="s">
+      <c r="N36" s="77" t="s">
         <v>459</v>
       </c>
       <c r="O36" t="s">
@@ -12442,7 +12498,7 @@
         <v>426</v>
       </c>
       <c r="Q36" t="str">
-        <f>I36</f>
+        <f t="shared" ref="Q36:Q63" si="1">I36</f>
         <v>P0[18]</v>
       </c>
     </row>
@@ -12473,10 +12529,10 @@
         <v>261</v>
       </c>
       <c r="L37" s="25"/>
-      <c r="M37" s="96" t="s">
+      <c r="M37" s="93" t="s">
         <v>258</v>
       </c>
-      <c r="N37" s="80" t="s">
+      <c r="N37" s="77" t="s">
         <v>459</v>
       </c>
       <c r="O37" t="s">
@@ -12486,7 +12542,7 @@
         <v>427</v>
       </c>
       <c r="Q37" t="str">
-        <f>I37</f>
+        <f t="shared" si="1"/>
         <v>P0[17]</v>
       </c>
     </row>
@@ -12519,10 +12575,10 @@
       <c r="L38" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="M38" s="96" t="s">
+      <c r="M38" s="93" t="s">
         <v>258</v>
       </c>
-      <c r="N38" s="80" t="s">
+      <c r="N38" s="77" t="s">
         <v>459</v>
       </c>
       <c r="O38" s="56" t="s">
@@ -12532,7 +12588,7 @@
         <v>428</v>
       </c>
       <c r="Q38" t="str">
-        <f>I38</f>
+        <f t="shared" si="1"/>
         <v>P0[16]</v>
       </c>
     </row>
@@ -12563,10 +12619,10 @@
         <v>264</v>
       </c>
       <c r="L39" s="25"/>
-      <c r="M39" s="96" t="s">
+      <c r="M39" s="93" t="s">
         <v>258</v>
       </c>
-      <c r="N39" s="80" t="s">
+      <c r="N39" s="77" t="s">
         <v>459</v>
       </c>
       <c r="O39" s="56" t="s">
@@ -12576,7 +12632,7 @@
         <v>429</v>
       </c>
       <c r="Q39" t="str">
-        <f>I39</f>
+        <f t="shared" si="1"/>
         <v>P0[15]</v>
       </c>
     </row>
@@ -12603,10 +12659,10 @@
       <c r="J40" s="23"/>
       <c r="K40" s="23"/>
       <c r="L40" s="23"/>
-      <c r="M40" s="96" t="s">
+      <c r="M40" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N40" s="80" t="s">
+      <c r="N40" s="77" t="s">
         <v>440</v>
       </c>
       <c r="O40" t="s">
@@ -12616,7 +12672,7 @@
         <v>426</v>
       </c>
       <c r="Q40" t="str">
-        <f>I40</f>
+        <f t="shared" si="1"/>
         <v>P2[7]</v>
       </c>
     </row>
@@ -12643,10 +12699,10 @@
       <c r="J41" s="23"/>
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
-      <c r="M41" s="96" t="s">
+      <c r="M41" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N41" s="80" t="s">
+      <c r="N41" s="77" t="s">
         <v>440</v>
       </c>
       <c r="O41" t="s">
@@ -12656,7 +12712,7 @@
         <v>427</v>
       </c>
       <c r="Q41" t="str">
-        <f>I41</f>
+        <f t="shared" si="1"/>
         <v>P2[6]</v>
       </c>
     </row>
@@ -12685,10 +12741,10 @@
       </c>
       <c r="K42" s="68"/>
       <c r="L42" s="73"/>
-      <c r="M42" s="96" t="s">
+      <c r="M42" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N42" s="80" t="s">
+      <c r="N42" s="77" t="s">
         <v>440</v>
       </c>
       <c r="O42" t="s">
@@ -12698,7 +12754,7 @@
         <v>428</v>
       </c>
       <c r="Q42" t="str">
-        <f>I42</f>
+        <f t="shared" si="1"/>
         <v>P2[5]</v>
       </c>
     </row>
@@ -12727,10 +12783,10 @@
       </c>
       <c r="K43" s="26"/>
       <c r="L43" s="26"/>
-      <c r="M43" s="96" t="s">
+      <c r="M43" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="N43" s="80" t="s">
+      <c r="N43" s="77" t="s">
         <v>440</v>
       </c>
       <c r="O43" t="s">
@@ -12740,7 +12796,7 @@
         <v>429</v>
       </c>
       <c r="Q43" t="str">
-        <f>I43</f>
+        <f t="shared" si="1"/>
         <v>P2[4]</v>
       </c>
     </row>
@@ -12767,10 +12823,10 @@
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
       <c r="L44" s="30"/>
-      <c r="M44" s="96" t="s">
+      <c r="M44" s="93" t="s">
         <v>469</v>
       </c>
-      <c r="N44" s="80" t="s">
+      <c r="N44" s="77" t="s">
         <v>441</v>
       </c>
       <c r="O44" t="s">
@@ -12780,7 +12836,7 @@
         <v>426</v>
       </c>
       <c r="Q44" t="str">
-        <f>I44</f>
+        <f t="shared" si="1"/>
         <v>P1[21]</v>
       </c>
     </row>
@@ -12807,10 +12863,10 @@
       <c r="J45" s="26"/>
       <c r="K45" s="26"/>
       <c r="L45" s="26"/>
-      <c r="M45" s="96" t="s">
+      <c r="M45" s="93" t="s">
         <v>469</v>
       </c>
-      <c r="N45" s="80" t="s">
+      <c r="N45" s="77" t="s">
         <v>441</v>
       </c>
       <c r="O45" t="s">
@@ -12820,7 +12876,7 @@
         <v>427</v>
       </c>
       <c r="Q45" t="str">
-        <f>I45</f>
+        <f t="shared" si="1"/>
         <v>P1[20]</v>
       </c>
     </row>
@@ -12847,10 +12903,10 @@
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
       <c r="L46" s="30"/>
-      <c r="M46" s="96" t="s">
+      <c r="M46" s="93" t="s">
         <v>469</v>
       </c>
-      <c r="N46" s="80" t="s">
+      <c r="N46" s="77" t="s">
         <v>441</v>
       </c>
       <c r="O46" t="s">
@@ -12860,7 +12916,7 @@
         <v>428</v>
       </c>
       <c r="Q46" t="str">
-        <f>I46</f>
+        <f t="shared" si="1"/>
         <v>P1[19]</v>
       </c>
     </row>
@@ -12887,10 +12943,10 @@
       <c r="J47" s="26"/>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
-      <c r="M47" s="96" t="s">
+      <c r="M47" s="93" t="s">
         <v>469</v>
       </c>
-      <c r="N47" s="80" t="s">
+      <c r="N47" s="77" t="s">
         <v>441</v>
       </c>
       <c r="O47" t="s">
@@ -12900,7 +12956,7 @@
         <v>429</v>
       </c>
       <c r="Q47" t="str">
-        <f>I47</f>
+        <f t="shared" si="1"/>
         <v>P1[18]</v>
       </c>
     </row>
@@ -12927,10 +12983,10 @@
       <c r="J48" s="24"/>
       <c r="K48" s="24"/>
       <c r="L48" s="24"/>
-      <c r="M48" s="96" t="s">
+      <c r="M48" s="93" t="s">
         <v>470</v>
       </c>
-      <c r="N48" s="80" t="s">
+      <c r="N48" s="77" t="s">
         <v>442</v>
       </c>
       <c r="O48" t="s">
@@ -12940,7 +12996,7 @@
         <v>426</v>
       </c>
       <c r="Q48" t="str">
-        <f>I48</f>
+        <f t="shared" si="1"/>
         <v>P0[5]</v>
       </c>
     </row>
@@ -12967,10 +13023,10 @@
       <c r="J49" s="24"/>
       <c r="K49" s="24"/>
       <c r="L49" s="24"/>
-      <c r="M49" s="96" t="s">
+      <c r="M49" s="93" t="s">
         <v>470</v>
       </c>
-      <c r="N49" s="80" t="s">
+      <c r="N49" s="77" t="s">
         <v>442</v>
       </c>
       <c r="O49" t="s">
@@ -12980,7 +13036,7 @@
         <v>427</v>
       </c>
       <c r="Q49" t="str">
-        <f>I49</f>
+        <f t="shared" si="1"/>
         <v>P0[4]</v>
       </c>
     </row>
@@ -13009,10 +13065,10 @@
       <c r="L50" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="M50" s="96" t="s">
+      <c r="M50" s="93" t="s">
         <v>470</v>
       </c>
-      <c r="N50" s="80" t="s">
+      <c r="N50" s="77" t="s">
         <v>442</v>
       </c>
       <c r="O50" s="56" t="s">
@@ -13022,7 +13078,7 @@
         <v>428</v>
       </c>
       <c r="Q50" t="str">
-        <f>I50</f>
+        <f t="shared" si="1"/>
         <v>P4[29]</v>
       </c>
     </row>
@@ -13051,10 +13107,10 @@
       <c r="L51" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="M51" s="96" t="s">
+      <c r="M51" s="93" t="s">
         <v>470</v>
       </c>
-      <c r="N51" s="80" t="s">
+      <c r="N51" s="77" t="s">
         <v>442</v>
       </c>
       <c r="O51" s="56" t="s">
@@ -13064,7 +13120,7 @@
         <v>429</v>
       </c>
       <c r="Q51" t="str">
-        <f>I51</f>
+        <f t="shared" si="1"/>
         <v>P4[28]</v>
       </c>
     </row>
@@ -13088,10 +13144,10 @@
       <c r="I52" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="J52" s="84"/>
-      <c r="K52" s="86"/>
-      <c r="L52" s="88"/>
-      <c r="M52" s="96" t="s">
+      <c r="J52" s="81"/>
+      <c r="K52" s="83"/>
+      <c r="L52" s="85"/>
+      <c r="M52" s="93" t="s">
         <v>471</v>
       </c>
       <c r="N52" t="s">
@@ -13104,7 +13160,7 @@
         <v>426</v>
       </c>
       <c r="Q52" t="str">
-        <f>I52</f>
+        <f t="shared" si="1"/>
         <v>P2[8]</v>
       </c>
     </row>
@@ -13131,7 +13187,7 @@
       <c r="J53" s="65"/>
       <c r="K53" s="70"/>
       <c r="L53" s="75"/>
-      <c r="M53" s="96" t="s">
+      <c r="M53" s="93" t="s">
         <v>471</v>
       </c>
       <c r="N53" t="s">
@@ -13144,7 +13200,7 @@
         <v>427</v>
       </c>
       <c r="Q53" t="str">
-        <f>I53</f>
+        <f t="shared" si="1"/>
         <v>P3[26]</v>
       </c>
     </row>
@@ -13168,12 +13224,12 @@
       <c r="I54" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="J54" s="85" t="s">
+      <c r="J54" s="82" t="s">
         <v>383</v>
       </c>
-      <c r="K54" s="87"/>
-      <c r="L54" s="89"/>
-      <c r="M54" s="96" t="s">
+      <c r="K54" s="84"/>
+      <c r="L54" s="86"/>
+      <c r="M54" s="93" t="s">
         <v>471</v>
       </c>
       <c r="N54" t="s">
@@ -13186,7 +13242,7 @@
         <v>428</v>
       </c>
       <c r="Q54" t="str">
-        <f>I54</f>
+        <f t="shared" si="1"/>
         <v>P1[0]</v>
       </c>
     </row>
@@ -13210,12 +13266,12 @@
       <c r="I55" s="13" t="s">
         <v>380</v>
       </c>
-      <c r="J55" s="85" t="s">
+      <c r="J55" s="82" t="s">
         <v>381</v>
       </c>
-      <c r="K55" s="87"/>
-      <c r="L55" s="89"/>
-      <c r="M55" s="96" t="s">
+      <c r="K55" s="84"/>
+      <c r="L55" s="86"/>
+      <c r="M55" s="93" t="s">
         <v>471</v>
       </c>
       <c r="N55" t="s">
@@ -13228,7 +13284,7 @@
         <v>429</v>
       </c>
       <c r="Q55" t="str">
-        <f>I55</f>
+        <f t="shared" si="1"/>
         <v>P1[1]</v>
       </c>
     </row>
@@ -13257,10 +13313,10 @@
       </c>
       <c r="K56" s="29"/>
       <c r="L56" s="29"/>
-      <c r="M56" s="96" t="s">
+      <c r="M56" s="93" t="s">
         <v>472</v>
       </c>
-      <c r="N56" s="80" t="s">
+      <c r="N56" s="77" t="s">
         <v>444</v>
       </c>
       <c r="O56" t="s">
@@ -13270,7 +13326,7 @@
         <v>426</v>
       </c>
       <c r="Q56" t="str">
-        <f>I56</f>
+        <f t="shared" si="1"/>
         <v>P1[17]</v>
       </c>
     </row>
@@ -13299,10 +13355,10 @@
       </c>
       <c r="K57" s="29"/>
       <c r="L57" s="29"/>
-      <c r="M57" s="96" t="s">
+      <c r="M57" s="93" t="s">
         <v>472</v>
       </c>
-      <c r="N57" s="80" t="s">
+      <c r="N57" s="77" t="s">
         <v>444</v>
       </c>
       <c r="O57" t="s">
@@ -13312,7 +13368,7 @@
         <v>427</v>
       </c>
       <c r="Q57" t="str">
-        <f>I57</f>
+        <f t="shared" si="1"/>
         <v>P1[16]</v>
       </c>
     </row>
@@ -13341,10 +13397,10 @@
       </c>
       <c r="K58" s="29"/>
       <c r="L58" s="29"/>
-      <c r="M58" s="96" t="s">
+      <c r="M58" s="93" t="s">
         <v>472</v>
       </c>
-      <c r="N58" s="80" t="s">
+      <c r="N58" s="77" t="s">
         <v>444</v>
       </c>
       <c r="O58" t="s">
@@ -13354,7 +13410,7 @@
         <v>428</v>
       </c>
       <c r="Q58" t="str">
-        <f>I58</f>
+        <f t="shared" si="1"/>
         <v>P1[15]</v>
       </c>
     </row>
@@ -13383,10 +13439,10 @@
       </c>
       <c r="K59" s="29"/>
       <c r="L59" s="29"/>
-      <c r="M59" s="96" t="s">
+      <c r="M59" s="93" t="s">
         <v>472</v>
       </c>
-      <c r="N59" s="80" t="s">
+      <c r="N59" s="77" t="s">
         <v>444</v>
       </c>
       <c r="O59" t="s">
@@ -13396,7 +13452,7 @@
         <v>429</v>
       </c>
       <c r="Q59" t="str">
-        <f>I59</f>
+        <f t="shared" si="1"/>
         <v>P1[14]</v>
       </c>
     </row>
@@ -13425,10 +13481,10 @@
       </c>
       <c r="K60" s="30"/>
       <c r="L60" s="30"/>
-      <c r="M60" s="96" t="s">
+      <c r="M60" s="93" t="s">
         <v>473</v>
       </c>
-      <c r="N60" s="80" t="s">
+      <c r="N60" s="77" t="s">
         <v>445</v>
       </c>
       <c r="O60" t="s">
@@ -13438,7 +13494,7 @@
         <v>426</v>
       </c>
       <c r="Q60" t="str">
-        <f>I60</f>
+        <f t="shared" si="1"/>
         <v>P1[10]</v>
       </c>
     </row>
@@ -13467,10 +13523,10 @@
       </c>
       <c r="K61" s="30"/>
       <c r="L61" s="30"/>
-      <c r="M61" s="96" t="s">
+      <c r="M61" s="93" t="s">
         <v>473</v>
       </c>
-      <c r="N61" s="80" t="s">
+      <c r="N61" s="77" t="s">
         <v>445</v>
       </c>
       <c r="O61" t="s">
@@ -13480,7 +13536,7 @@
         <v>427</v>
       </c>
       <c r="Q61" t="str">
-        <f>I61</f>
+        <f t="shared" si="1"/>
         <v>P1[9]</v>
       </c>
     </row>
@@ -13509,10 +13565,10 @@
       </c>
       <c r="K62" s="30"/>
       <c r="L62" s="30"/>
-      <c r="M62" s="96" t="s">
+      <c r="M62" s="93" t="s">
         <v>473</v>
       </c>
-      <c r="N62" s="80" t="s">
+      <c r="N62" s="77" t="s">
         <v>445</v>
       </c>
       <c r="O62" t="s">
@@ -13522,7 +13578,7 @@
         <v>428</v>
       </c>
       <c r="Q62" t="str">
-        <f>I62</f>
+        <f t="shared" si="1"/>
         <v>P1[8]</v>
       </c>
     </row>
@@ -13551,10 +13607,10 @@
       </c>
       <c r="K63" s="30"/>
       <c r="L63" s="30"/>
-      <c r="M63" s="96" t="s">
+      <c r="M63" s="93" t="s">
         <v>473</v>
       </c>
-      <c r="N63" s="80" t="s">
+      <c r="N63" s="77" t="s">
         <v>445</v>
       </c>
       <c r="O63" t="s">
@@ -13564,7 +13620,7 @@
         <v>429</v>
       </c>
       <c r="Q63" t="str">
-        <f>I63</f>
+        <f t="shared" si="1"/>
         <v>P1[4]</v>
       </c>
     </row>
@@ -13593,10 +13649,10 @@
       </c>
       <c r="K64" s="55"/>
       <c r="L64" s="55"/>
-      <c r="M64" s="96" t="s">
+      <c r="M64" s="93" t="s">
         <v>474</v>
       </c>
-      <c r="N64" s="80" t="s">
+      <c r="N64" s="77" t="s">
         <v>437</v>
       </c>
     </row>
@@ -13625,7 +13681,7 @@
       </c>
       <c r="K65" s="63"/>
       <c r="L65" s="63"/>
-      <c r="N65" s="80" t="s">
+      <c r="N65" s="77" t="s">
         <v>450</v>
       </c>
     </row>
@@ -13654,7 +13710,7 @@
       </c>
       <c r="K66" s="63"/>
       <c r="L66" s="63"/>
-      <c r="N66" s="80" t="s">
+      <c r="N66" s="77" t="s">
         <v>450</v>
       </c>
     </row>
@@ -13683,7 +13739,7 @@
       </c>
       <c r="K67" s="63"/>
       <c r="L67" s="63"/>
-      <c r="N67" s="80" t="s">
+      <c r="N67" s="77" t="s">
         <v>450</v>
       </c>
     </row>
@@ -13712,7 +13768,7 @@
       </c>
       <c r="K68" s="63"/>
       <c r="L68" s="63"/>
-      <c r="N68" s="80" t="s">
+      <c r="N68" s="77" t="s">
         <v>450</v>
       </c>
     </row>
@@ -13741,8 +13797,8 @@
       </c>
       <c r="K69" s="61"/>
       <c r="L69" s="61"/>
-      <c r="M69" s="91"/>
-      <c r="N69" s="80" t="s">
+      <c r="M69" s="88"/>
+      <c r="N69" s="77" t="s">
         <v>54</v>
       </c>
     </row>
@@ -13771,8 +13827,8 @@
       </c>
       <c r="K70" s="61"/>
       <c r="L70" s="61"/>
-      <c r="M70" s="90"/>
-      <c r="N70" s="80" t="s">
+      <c r="M70" s="87"/>
+      <c r="N70" s="77" t="s">
         <v>54</v>
       </c>
     </row>
@@ -13801,8 +13857,8 @@
       </c>
       <c r="K71" s="59"/>
       <c r="L71" s="59"/>
-      <c r="M71" s="92"/>
-      <c r="N71" s="80" t="s">
+      <c r="M71" s="89"/>
+      <c r="N71" s="77" t="s">
         <v>464</v>
       </c>
     </row>
@@ -13818,6 +13874,1898 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="36"/>
+    <col min="6" max="6" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>475</v>
+      </c>
+      <c r="H1" s="58" t="s">
+        <v>477</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>478</v>
+      </c>
+      <c r="J1" s="58" t="s">
+        <v>463</v>
+      </c>
+      <c r="P1" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="33">
+        <v>24</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="97" t="s">
+        <v>451</v>
+      </c>
+      <c r="H2" s="97"/>
+      <c r="I2" s="94"/>
+      <c r="O2" t="s">
+        <v>413</v>
+      </c>
+      <c r="R2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="33">
+        <v>25</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>404</v>
+      </c>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="94"/>
+      <c r="O3" t="s">
+        <v>414</v>
+      </c>
+      <c r="R3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="17">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="80" t="s">
+        <v>465</v>
+      </c>
+      <c r="H4" s="97">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>426</v>
+      </c>
+      <c r="O4" t="s">
+        <v>415</v>
+      </c>
+      <c r="P4" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>419</v>
+      </c>
+      <c r="R4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="17">
+        <v>9</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="80" t="s">
+        <v>465</v>
+      </c>
+      <c r="H5" s="97"/>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>427</v>
+      </c>
+      <c r="O5" t="s">
+        <v>416</v>
+      </c>
+      <c r="P5" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>420</v>
+      </c>
+      <c r="R5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="17">
+        <v>20</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="80" t="s">
+        <v>465</v>
+      </c>
+      <c r="H6" s="97"/>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="17">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="80" t="s">
+        <v>465</v>
+      </c>
+      <c r="H7" s="97"/>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="17">
+        <v>70</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="83"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="H8" s="97">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="17">
+        <v>73</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" s="83"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="H9" s="97"/>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="17">
+        <v>74</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="H10" s="97"/>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="17">
+        <v>75</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="H11" s="97"/>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="17">
+        <v>39</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D12" s="90"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H12" s="97">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="17">
+        <v>38</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H13" s="97"/>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="17">
+        <v>37</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H14" s="97"/>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="17">
+        <v>36</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H15" s="97"/>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="17">
+        <v>45</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H16" s="97">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="17">
+        <v>44</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H17" s="97"/>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="B18" s="17">
+        <v>43</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H18" s="97"/>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="17">
+        <v>40</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H19" s="97"/>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="17">
+        <v>46</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="80" t="s">
+        <v>466</v>
+      </c>
+      <c r="H20" s="97">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="17">
+        <v>47</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="80" t="s">
+        <v>466</v>
+      </c>
+      <c r="H21" s="97"/>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="17">
+        <v>49</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="80" t="s">
+        <v>466</v>
+      </c>
+      <c r="H22" s="97"/>
+      <c r="I22" s="56">
+        <v>3</v>
+      </c>
+      <c r="J22" s="56" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="17">
+        <v>48</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="80" t="s">
+        <v>466</v>
+      </c>
+      <c r="H23" s="97"/>
+      <c r="I23" s="56">
+        <v>4</v>
+      </c>
+      <c r="J23" s="56" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="17">
+        <v>50</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H24" s="97">
+        <v>6</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="17">
+        <v>51</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H25" s="97"/>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="17">
+        <v>52</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H26" s="97"/>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="17">
+        <v>27</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H27" s="97"/>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="17">
+        <v>56</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="87" t="s">
+        <v>467</v>
+      </c>
+      <c r="H28" s="97">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="17">
+        <v>57</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="87" t="s">
+        <v>467</v>
+      </c>
+      <c r="H29" s="97"/>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="17">
+        <v>58</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="F30" s="24"/>
+      <c r="G30" s="87" t="s">
+        <v>467</v>
+      </c>
+      <c r="H30" s="97"/>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="17">
+        <v>59</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="24"/>
+      <c r="G31" s="87" t="s">
+        <v>467</v>
+      </c>
+      <c r="H31" s="97"/>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="17">
+        <v>7</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G32" s="93" t="s">
+        <v>468</v>
+      </c>
+      <c r="H32" s="98">
+        <v>8</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="17">
+        <v>6</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G33" s="93" t="s">
+        <v>468</v>
+      </c>
+      <c r="H33" s="98"/>
+      <c r="I33" s="57">
+        <v>2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="17">
+        <v>99</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="93" t="s">
+        <v>468</v>
+      </c>
+      <c r="H34" s="98"/>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="17">
+        <v>98</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="93" t="s">
+        <v>468</v>
+      </c>
+      <c r="H35" s="98"/>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="17">
+        <v>60</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F36" s="25"/>
+      <c r="G36" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="H36" s="97">
+        <v>9</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="17">
+        <v>61</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="F37" s="25"/>
+      <c r="G37" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="H37" s="97"/>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="17">
+        <v>63</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="G38" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="H38" s="97"/>
+      <c r="I38" s="56">
+        <v>3</v>
+      </c>
+      <c r="J38" s="56" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="17">
+        <v>62</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="F39" s="25"/>
+      <c r="G39" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="H39" s="97"/>
+      <c r="I39" s="56">
+        <v>4</v>
+      </c>
+      <c r="J39" s="56" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="17">
+        <v>66</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H40" s="97">
+        <v>10</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="17">
+        <v>67</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H41" s="97"/>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="17">
+        <v>68</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>276</v>
+      </c>
+      <c r="E42" s="68"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H42" s="97"/>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="17">
+        <v>69</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="93" t="s">
+        <v>303</v>
+      </c>
+      <c r="H43" s="97"/>
+      <c r="I43">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="17">
+        <v>35</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="93" t="s">
+        <v>469</v>
+      </c>
+      <c r="H44" s="97">
+        <v>11</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="17">
+        <v>34</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="93" t="s">
+        <v>469</v>
+      </c>
+      <c r="H45" s="97"/>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B46" s="17">
+        <v>33</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="93" t="s">
+        <v>469</v>
+      </c>
+      <c r="H46" s="97"/>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="17">
+        <v>32</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="93" t="s">
+        <v>469</v>
+      </c>
+      <c r="H47" s="97"/>
+      <c r="I47">
+        <v>4</v>
+      </c>
+      <c r="J47" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="17">
+        <v>80</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="93" t="s">
+        <v>470</v>
+      </c>
+      <c r="H48" s="97">
+        <v>12</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="17">
+        <v>81</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="93" t="s">
+        <v>470</v>
+      </c>
+      <c r="H49" s="97"/>
+      <c r="I49">
+        <v>2</v>
+      </c>
+      <c r="J49" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="17">
+        <v>85</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="G50" s="93" t="s">
+        <v>470</v>
+      </c>
+      <c r="H50" s="97"/>
+      <c r="I50" s="56">
+        <v>3</v>
+      </c>
+      <c r="J50" s="56" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" s="17">
+        <v>82</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="G51" s="93" t="s">
+        <v>470</v>
+      </c>
+      <c r="H51" s="97"/>
+      <c r="I51" s="56">
+        <v>4</v>
+      </c>
+      <c r="J51" s="56" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="17">
+        <v>65</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D52" s="81"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="93" t="s">
+        <v>471</v>
+      </c>
+      <c r="H52" s="97">
+        <v>13</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="17">
+        <v>26</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D53" s="65"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="93" t="s">
+        <v>471</v>
+      </c>
+      <c r="H53" s="97"/>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="17">
+        <v>95</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="D54" s="82" t="s">
+        <v>383</v>
+      </c>
+      <c r="E54" s="84"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="93" t="s">
+        <v>471</v>
+      </c>
+      <c r="H54" s="97"/>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="17">
+        <v>94</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="D55" s="82" t="s">
+        <v>381</v>
+      </c>
+      <c r="E55" s="84"/>
+      <c r="F55" s="86"/>
+      <c r="G55" s="93" t="s">
+        <v>471</v>
+      </c>
+      <c r="H55" s="97"/>
+      <c r="I55">
+        <v>4</v>
+      </c>
+      <c r="J55" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="17">
+        <v>86</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="93" t="s">
+        <v>472</v>
+      </c>
+      <c r="H56" s="97">
+        <v>14</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" s="17">
+        <v>87</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="93" t="s">
+        <v>472</v>
+      </c>
+      <c r="H57" s="97"/>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" s="17">
+        <v>88</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="93" t="s">
+        <v>472</v>
+      </c>
+      <c r="H58" s="97"/>
+      <c r="I58">
+        <v>3</v>
+      </c>
+      <c r="J58" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="17">
+        <v>89</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="93" t="s">
+        <v>472</v>
+      </c>
+      <c r="H59" s="97"/>
+      <c r="I59">
+        <v>4</v>
+      </c>
+      <c r="J59" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" s="17">
+        <v>90</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="93" t="s">
+        <v>473</v>
+      </c>
+      <c r="H60" s="97">
+        <v>15</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" s="17">
+        <v>91</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="93" t="s">
+        <v>473</v>
+      </c>
+      <c r="H61" s="97"/>
+      <c r="I61">
+        <v>2</v>
+      </c>
+      <c r="J61" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="17">
+        <v>92</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="93" t="s">
+        <v>473</v>
+      </c>
+      <c r="H62" s="97"/>
+      <c r="I62">
+        <v>3</v>
+      </c>
+      <c r="J62" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" s="17">
+        <v>93</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="93" t="s">
+        <v>473</v>
+      </c>
+      <c r="H63" s="97"/>
+      <c r="I63">
+        <v>4</v>
+      </c>
+      <c r="J63" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="52">
+        <v>53</v>
+      </c>
+      <c r="C64" s="51" t="s">
+        <v>309</v>
+      </c>
+      <c r="D64" s="55" t="s">
+        <v>409</v>
+      </c>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="93" t="s">
+        <v>474</v>
+      </c>
+      <c r="H64" s="97"/>
+      <c r="I64" s="94"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="39">
+        <v>76</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" s="63" t="s">
+        <v>405</v>
+      </c>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="97" t="s">
+        <v>476</v>
+      </c>
+      <c r="H65" s="97"/>
+      <c r="I65" s="94"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="39">
+        <v>77</v>
+      </c>
+      <c r="C66" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="D66" s="63" t="s">
+        <v>406</v>
+      </c>
+      <c r="E66" s="63"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="97"/>
+      <c r="H66" s="97"/>
+      <c r="I66" s="94"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="39">
+        <v>78</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="D67" s="63" t="s">
+        <v>407</v>
+      </c>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="97"/>
+      <c r="H67" s="97"/>
+      <c r="I67" s="94"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="39">
+        <v>79</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" s="63" t="s">
+        <v>408</v>
+      </c>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="G68" s="97"/>
+      <c r="H68" s="97"/>
+      <c r="I68" s="94"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="33">
+        <v>29</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="D69" s="61" t="s">
+        <v>401</v>
+      </c>
+      <c r="E69" s="61"/>
+      <c r="F69" s="61"/>
+      <c r="G69" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="H69" s="97"/>
+      <c r="I69" s="94"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="33">
+        <v>30</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="D70" s="61" t="s">
+        <v>402</v>
+      </c>
+      <c r="E70" s="61"/>
+      <c r="F70" s="61"/>
+      <c r="G70" s="97"/>
+      <c r="H70" s="97"/>
+      <c r="I70" s="94"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="39">
+        <v>64</v>
+      </c>
+      <c r="C71" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="D71" s="59" t="s">
+        <v>400</v>
+      </c>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="H71" s="97"/>
+      <c r="I71" s="94"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I64:I71"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H64:H71"/>
+    <mergeCell ref="H52:H55"/>
+    <mergeCell ref="H56:H59"/>
+    <mergeCell ref="H60:H63"/>
+    <mergeCell ref="G65:G68"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="H44:H47"/>
+    <mergeCell ref="H48:H51"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H24:H27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W71"/>
   <sheetViews>
@@ -13839,7 +15787,7 @@
     <col min="12" max="12" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="141" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="142" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -16560,7 +18508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>

</xml_diff>